<commit_message>
Content - Activate Xmas season and unhide bothe Xmas Pets
Former-commit-id: 612c95d8fbc2167a1137e23d47ab50ae8aca6f3d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -1827,8 +1827,8 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2053,7 +2053,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
@@ -2102,7 +2102,7 @@
   </sheetPr>
   <dimension ref="B1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Content - Xmas is over (remove Xmas from content)
Former-commit-id: c243ef14ea0e6435cff6a415bad24722e2390e0b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1827,8 +1827,8 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2053,7 +2053,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
New TIDs for seasons
Former-commit-id: de61b1ddb83a664dbeccf96ed98cc3ac9831bf32
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="96">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -341,13 +341,19 @@
   </si>
   <si>
     <t>LOCALIZATION DEFINITIONS</t>
+  </si>
+  <si>
+    <t>TID_SEASON_XMAS_NAME</t>
+  </si>
+  <si>
+    <t>TID_SEASON_HALLOWEEN_NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +421,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -606,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -663,6 +675,9 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1529,13 +1544,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:E18" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
-  <autoFilter ref="B16:E18"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F18" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="B16:F18"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="16"/>
     <tableColumn id="2" name="[sku]" dataDxfId="15"/>
     <tableColumn id="3" name="[active]" dataDxfId="14"/>
     <tableColumn id="4" name="[icon]"/>
+    <tableColumn id="5" name="[tidName]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1828,7 +1844,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2044,6 +2060,9 @@
       <c r="E16" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="F16" s="32" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="3" t="s">
@@ -2058,6 +2077,9 @@
       <c r="E17" t="s">
         <v>4</v>
       </c>
+      <c r="F17" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="3" t="s">
@@ -2071,6 +2093,9 @@
       </c>
       <c r="E18" t="s">
         <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="2:7">

</xml_diff>

<commit_message>
Content - Exported values from Toni + Balance timer HC relation
Former-commit-id: 6a5a3d380560dd4f0a48ebbf7c40f8bd4f279afb
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -427,6 +427,7 @@
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1843,8 +1844,8 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1944,10 +1945,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="1">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
       <c r="E5" s="9">
-        <v>4.5</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>15</v>

</xml_diff>

<commit_message>
Localization: Development - Enabled Latin languages + Russian.
Former-commit-id: 62409963c8dbfc6ab203b4165375374183c7959f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800"/>
+    <workbookView xWindow="5400" yWindow="440" windowWidth="34440" windowHeight="17120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -353,7 +353,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1843,24 +1843,24 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
     <col min="8" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:16" ht="23.25">
+    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
@@ -1874,7 +1874,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="14"/>
       <c r="C3" s="13"/>
@@ -1889,7 +1889,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:16" ht="306">
+    <row r="4" spans="1:16" ht="303" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1983,8 +1983,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1"/>
-    <row r="8" spans="1:16" ht="23.25">
+    <row r="7" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -1998,7 +1998,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="10" spans="1:16" ht="94.5">
+    <row r="10" spans="1:16" ht="94" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2032,8 +2032,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1"/>
-    <row r="14" spans="1:16" ht="23.25">
+    <row r="13" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
@@ -2047,7 +2047,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="16" spans="1:16" ht="104.25">
+    <row r="16" spans="1:16" ht="103" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G22" t="s">
         <v>0</v>
       </c>
@@ -2127,23 +2127,23 @@
   </sheetPr>
   <dimension ref="B1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="6" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:10" ht="23.25">
+    <row r="1" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>93</v>
       </c>
@@ -2156,7 +2156,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="2:10" ht="30">
+    <row r="3" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B3" s="31"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2166,7 +2166,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="119.25">
+    <row r="4" spans="2:10" ht="116" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>91</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="26" t="s">
         <v>3</v>
       </c>
@@ -2224,8 +2224,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="26"/>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="26" t="s">
+        <v>3</v>
+      </c>
       <c r="C6" s="22" t="s">
         <v>79</v>
       </c>
@@ -2251,8 +2253,10 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="23"/>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="26" t="s">
+        <v>3</v>
+      </c>
       <c r="C7" s="22" t="s">
         <v>74</v>
       </c>
@@ -2278,8 +2282,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="23"/>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="26" t="s">
+        <v>3</v>
+      </c>
       <c r="C8" s="22" t="s">
         <v>69</v>
       </c>
@@ -2305,8 +2311,10 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="23"/>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="26" t="s">
+        <v>3</v>
+      </c>
       <c r="C9" s="22" t="s">
         <v>64</v>
       </c>
@@ -2332,8 +2340,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="23"/>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="26" t="s">
+        <v>3</v>
+      </c>
       <c r="C10" s="22" t="s">
         <v>59</v>
       </c>
@@ -2359,8 +2369,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="23"/>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="26" t="s">
+        <v>3</v>
+      </c>
       <c r="C11" s="22" t="s">
         <v>54</v>
       </c>
@@ -2386,7 +2398,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="23"/>
       <c r="C12" s="22" t="s">
         <v>49</v>
@@ -2413,7 +2425,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="23"/>
       <c r="C13" s="22" t="s">
         <v>44</v>
@@ -2440,7 +2452,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="23"/>
       <c r="C14" s="22" t="s">
         <v>39</v>
@@ -2467,34 +2479,34 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="16"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
     </row>
-    <row r="24" spans="2:2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="2:2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="2:2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
     </row>
-    <row r="27" spans="2:2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" s="15"/>
     </row>
-    <row r="28" spans="2:2">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Localization: Content - Enabled all languages, added Traditional Chinese.
Former-commit-id: c02aae76ff90cbc56e3365283470b3dcab022dff
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38180" windowHeight="19860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -166,9 +166,6 @@
     <t>GAME SETTINGS</t>
   </si>
   <si>
-    <t>TID_SETTINGS_LANG_KO</t>
-  </si>
-  <si>
     <t>flags_korean</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>lang_korean</t>
   </si>
   <si>
-    <t>TID_SETTINGS_LANG_JP</t>
-  </si>
-  <si>
     <t>flags_japanese</t>
   </si>
   <si>
@@ -196,24 +190,15 @@
     <t>lang_japanese</t>
   </si>
   <si>
-    <t>TID_SETTINGS_LANG_CN</t>
-  </si>
-  <si>
     <t>flags_chinese</t>
   </si>
   <si>
     <t>simplified_chinese</t>
   </si>
   <si>
-    <t>zh-CN</t>
-  </si>
-  <si>
     <t>lang_chinese</t>
   </si>
   <si>
-    <t>TID_SETTINGS_LANG_RU</t>
-  </si>
-  <si>
     <t>flags_russian</t>
   </si>
   <si>
@@ -226,9 +211,6 @@
     <t>lang_russian</t>
   </si>
   <si>
-    <t>TID_SETTINGS_LANG_BR</t>
-  </si>
-  <si>
     <t>flags_brazilian</t>
   </si>
   <si>
@@ -241,9 +223,6 @@
     <t>lang_brazilian</t>
   </si>
   <si>
-    <t>TID_SETTINGS_LANG_ES</t>
-  </si>
-  <si>
     <t>flags_spanish</t>
   </si>
   <si>
@@ -256,9 +235,6 @@
     <t>lang_spanish</t>
   </si>
   <si>
-    <t>TID_SETTINGS_LANG_DE</t>
-  </si>
-  <si>
     <t>flags_german</t>
   </si>
   <si>
@@ -271,9 +247,6 @@
     <t>lang_german</t>
   </si>
   <si>
-    <t>TID_SETTINGS_LANG_IT</t>
-  </si>
-  <si>
     <t>flags_italian</t>
   </si>
   <si>
@@ -286,9 +259,6 @@
     <t>lang_italian</t>
   </si>
   <si>
-    <t>TID_SETTINGS_LANG_FR</t>
-  </si>
-  <si>
     <t>flags_french</t>
   </si>
   <si>
@@ -301,9 +271,6 @@
     <t>lang_french</t>
   </si>
   <si>
-    <t>TID_SETTINGS_LANG_EN</t>
-  </si>
-  <si>
     <t>flags_english</t>
   </si>
   <si>
@@ -347,13 +314,28 @@
   </si>
   <si>
     <t>TID_SEASON_HALLOWEEN_NAME</t>
+  </si>
+  <si>
+    <t>lang_chinese_trad</t>
+  </si>
+  <si>
+    <t>traditional_chinese</t>
+  </si>
+  <si>
+    <t>zh-CHS</t>
+  </si>
+  <si>
+    <t>zh-CHT</t>
+  </si>
+  <si>
+    <t>TID_SETTINGS_LANG_NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -619,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -659,7 +641,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1559,8 +1540,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:J14" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="B4:J14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:J15" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="B4:J15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="8"/>
     <tableColumn id="8" name="[sku]" dataDxfId="7"/>
@@ -1844,24 +1825,24 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
     <col min="8" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:16" ht="23.25">
+    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
@@ -1875,7 +1856,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="14"/>
       <c r="C3" s="13"/>
@@ -1890,7 +1871,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:16" ht="306">
+    <row r="4" spans="1:16" ht="303" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -1937,7 +1918,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1984,8 +1965,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1"/>
-    <row r="8" spans="1:16" ht="23.25">
+    <row r="7" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -1999,7 +1980,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="10" spans="1:16" ht="94.5">
+    <row r="10" spans="1:16" ht="94" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -2016,7 +1997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2033,8 +2014,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1"/>
-    <row r="14" spans="1:16" ht="23.25">
+    <row r="13" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
@@ -2048,7 +2029,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="16" spans="1:16" ht="104.25">
+    <row r="16" spans="1:16" ht="103" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2061,11 +2042,11 @@
       <c r="E16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="32" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
+      <c r="F16" s="31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2079,10 +2060,10 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
@@ -2096,10 +2077,10 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G22" t="s">
         <v>0</v>
       </c>
@@ -2126,27 +2107,27 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="B1:J28"/>
+  <dimension ref="B1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="6" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:10" ht="23.25">
+    <row r="1" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2157,57 +2138,57 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="2:10" ht="30">
-      <c r="B3" s="31"/>
+    <row r="3" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="B3" s="30"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="119.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="116" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4" s="28" t="s">
+      <c r="D4" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="26" t="s">
+      <c r="J4" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D5" s="21">
         <v>0</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F5" s="20" t="b">
         <v>1</v>
@@ -2216,25 +2197,27 @@
         <v>1</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="26"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="C6" s="22" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D6" s="21">
         <v>1</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F6" s="20" t="b">
         <v>1</v>
@@ -2243,25 +2226,27 @@
         <v>1</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="23"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="C7" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="24">
+        <v>65</v>
+      </c>
+      <c r="D7" s="23">
         <v>2</v>
       </c>
-      <c r="E7" s="25" t="s">
-        <v>73</v>
+      <c r="E7" s="24" t="s">
+        <v>64</v>
       </c>
       <c r="F7" s="20" t="b">
         <v>1</v>
@@ -2270,25 +2255,27 @@
         <v>1</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="23"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="C8" s="22" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D8" s="21">
         <v>3</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F8" s="20" t="b">
         <v>1</v>
@@ -2297,25 +2284,27 @@
         <v>1</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="23"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="C9" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="24">
+        <v>57</v>
+      </c>
+      <c r="D9" s="23">
         <v>4</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F9" s="20" t="b">
         <v>1</v>
@@ -2324,25 +2313,27 @@
         <v>1</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="23"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="C10" s="22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D10" s="21">
         <v>5</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F10" s="20" t="b">
         <v>1</v>
@@ -2351,25 +2342,27 @@
         <v>1</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="23"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="C11" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="24">
+        <v>49</v>
+      </c>
+      <c r="D11" s="23">
         <v>6</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F11" s="20" t="b">
         <v>1</v>
@@ -2378,25 +2371,27 @@
         <v>1</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="23"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="C12" s="22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D12" s="21">
         <v>7</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="F12" s="20" t="b">
         <v>1</v>
@@ -2405,25 +2400,27 @@
         <v>0</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="23"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="C13" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="24">
+        <v>42</v>
+      </c>
+      <c r="D13" s="23">
         <v>8</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F13" s="20" t="b">
         <v>1</v>
@@ -2432,25 +2429,27 @@
         <v>1</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="23"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="C14" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="21">
         <v>9</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="20" t="b">
         <v>1</v>
@@ -2459,51 +2458,80 @@
         <v>1</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="16"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="15"/>
-    </row>
-    <row r="21" spans="2:2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="21">
+        <v>10</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="16"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
     </row>
-    <row r="24" spans="2:2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="2:2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="2:2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
     </row>
-    <row r="27" spans="2:2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" s="15"/>
     </row>
-    <row r="28" spans="2:2">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
     </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="15"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C14">
+  <conditionalFormatting sqref="C5:C15">
     <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G14">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G15">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Localization: Development - Font generation now now capitalizes all letters. Localization: Assets - Re-generated all font assets including all capital letters.
Former-commit-id: 0b5597a5ef8e56090ea8b765b6f9e6cddd5bf774
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -322,13 +322,13 @@
     <t>traditional_chinese</t>
   </si>
   <si>
-    <t>zh-CHS</t>
-  </si>
-  <si>
-    <t>zh-CHT</t>
-  </si>
-  <si>
     <t>TID_SETTINGS_LANG_NAME</t>
+  </si>
+  <si>
+    <t>zh-TW</t>
+  </si>
+  <si>
+    <t>zh-CN</t>
   </si>
 </sst>
 </file>
@@ -2110,7 +2110,7 @@
   <dimension ref="B1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2203,7 +2203,7 @@
         <v>70</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
@@ -2232,7 +2232,7 @@
         <v>66</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
@@ -2261,7 +2261,7 @@
         <v>62</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
@@ -2290,7 +2290,7 @@
         <v>58</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2319,7 +2319,7 @@
         <v>54</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
@@ -2348,7 +2348,7 @@
         <v>50</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
@@ -2377,7 +2377,7 @@
         <v>46</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
@@ -2391,13 +2391,13 @@
         <v>7</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F12" s="20" t="b">
         <v>1</v>
       </c>
       <c r="G12" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="19" t="s">
         <v>44</v>
@@ -2406,7 +2406,7 @@
         <v>43</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -2435,7 +2435,7 @@
         <v>39</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
@@ -2464,7 +2464,7 @@
         <v>35</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
@@ -2493,7 +2493,7 @@
         <v>43</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Localization: Content - Added fontGroupsDefinitions table. Enabled asian languages.
Former-commit-id: aed3ccffc956932c4df911fc3748fbf66ad64f0e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -329,13 +329,67 @@
   </si>
   <si>
     <t>zh-CN</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>zh_simpl</t>
+  </si>
+  <si>
+    <t>zh_trad</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>[fonts]</t>
+  </si>
+  <si>
+    <t>FNT_Bold;FNT_Default;FNT_RU</t>
+  </si>
+  <si>
+    <t>FNT_ZH_Simpl</t>
+  </si>
+  <si>
+    <t>FNT_ZH_Trad</t>
+  </si>
+  <si>
+    <t>FNT_JA</t>
+  </si>
+  <si>
+    <t>FNT_KO</t>
+  </si>
+  <si>
+    <t>[defaultFont]</t>
+  </si>
+  <si>
+    <t>FNT_Default</t>
+  </si>
+  <si>
+    <t>Optional, if not defined the first font in the list will be used</t>
+  </si>
+  <si>
+    <t>flags_taiwanese</t>
+  </si>
+  <si>
+    <t>[fontGroup]</t>
+  </si>
+  <si>
+    <t>FONT GROUPS DEFINITIONS</t>
+  </si>
+  <si>
+    <t>{fontGroupsDefinitions}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,16 +439,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF8FB5CC"/>
-      <name val="Menlo"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF406780"/>
-      <name val="Menlo"/>
     </font>
     <font>
       <b/>
@@ -493,7 +537,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -597,6 +641,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -633,8 +686,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -656,21 +707,24 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+  <dxfs count="49">
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -691,7 +745,36 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -716,107 +799,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -916,6 +902,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -925,13 +918,6 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -951,14 +937,289 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1464,16 +1725,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1488,13 +1739,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="B4:P5"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="31"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="30"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="44"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="43"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="42"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="41"/>
     <tableColumn id="5" name="[incentivizeFBGem]"/>
     <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
     <tableColumn id="15" name="[maxAdsSkipMissions]"/>
@@ -1512,26 +1763,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <autoFilter ref="B10:F11"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="23"/>
-    <tableColumn id="4" name="[hardCurrency]" dataDxfId="22"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="21"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="36"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="35"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="34"/>
+    <tableColumn id="4" name="[hardCurrency]" dataDxfId="33"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F18" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F18" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="B16:F18"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="16"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="3" name="[active]" dataDxfId="14"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="27"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="26"/>
+    <tableColumn id="3" name="[active]" dataDxfId="25"/>
     <tableColumn id="4" name="[icon]"/>
     <tableColumn id="5" name="[tidName]"/>
   </tableColumns>
@@ -1540,18 +1791,32 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:J15" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="B4:J15"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="8"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="7"/>
-    <tableColumn id="3" name="[order]" dataDxfId="6"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="5"/>
-    <tableColumn id="11" name="[android]" dataDxfId="4"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="3"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="2"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="1"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K15" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+  <autoFilter ref="B4:K15"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="20"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="19"/>
+    <tableColumn id="3" name="[order]" dataDxfId="18"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="17"/>
+    <tableColumn id="11" name="[android]" dataDxfId="16"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="15"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="14"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="13"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="4"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B20:E25" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="B20:E25"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="7"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="6"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="5"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2042,7 +2307,7 @@
       <c r="E16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="29" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2087,7 +2352,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="38" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D18"/>
@@ -2107,10 +2372,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="B1:J29"/>
+  <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2118,14 +2383,16 @@
     <col min="1" max="1" width="3.1640625" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
     <col min="6" max="7" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.83203125" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>82</v>
       </c>
@@ -2138,8 +2405,8 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B3" s="30"/>
+    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="B3" s="28"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
@@ -2148,396 +2415,510 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="116" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="116" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>80</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="K4" s="24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="19">
         <v>0</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="20" t="b">
+      <c r="F5" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G5" s="20" t="b">
+      <c r="G5" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="25" t="s">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="19">
         <v>1</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="20" t="b">
+      <c r="F6" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="20" t="b">
+      <c r="G6" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="K6" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="25" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="21">
         <v>2</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="20" t="b">
+      <c r="F7" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="20" t="b">
+      <c r="G7" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="K7" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="25" t="s">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="19">
         <v>3</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="20" t="b">
+      <c r="F8" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G8" s="20" t="b">
+      <c r="G8" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="25" t="s">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="21">
         <v>4</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="20" t="b">
+      <c r="F9" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G9" s="20" t="b">
+      <c r="G9" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="25" t="s">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="19">
         <v>5</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="20" t="b">
+      <c r="F10" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G10" s="20" t="b">
+      <c r="G10" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="K10" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="25" t="s">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="21">
         <v>6</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="20" t="b">
+      <c r="F11" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G11" s="20" t="b">
+      <c r="G11" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="K11" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="25" t="s">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="19">
         <v>7</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="20" t="b">
+      <c r="F12" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G12" s="20" t="b">
+      <c r="G12" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="25" t="s">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="21">
         <v>8</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="20" t="b">
+      <c r="F13" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G13" s="20" t="b">
+      <c r="G13" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="I13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="K13" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="25" t="s">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="19">
         <v>9</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="20" t="b">
+      <c r="F14" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G14" s="20" t="b">
+      <c r="G14" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="K14" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="25" t="s">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="19">
         <v>10</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="20" t="b">
+      <c r="F15" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G15" s="20" t="b">
+      <c r="G15" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="19" t="s">
-        <v>43</v>
+      <c r="I15" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="J15" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="16"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="15"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="15"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="15"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="15"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="15"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="15"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="15"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="15"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="15"/>
+    <row r="17" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="2:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="B19" s="28"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="2:10" ht="118" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C15">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <conditionalFormatting sqref="C21:C25">
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+  </conditionalFormatting>
+  <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G15">
       <formula1>"true,false"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="J5:J15">
+      <formula1>$C$21:$C$25</formula1>
+    </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D21:E25"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Font Group Definitions: Content - Added numbers font to each group.
Former-commit-id: 254a6bd807056cd51c79daee7cf15028ab3575a7
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B040C215-FB73-384A-BA6B-41A39B75DAE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38180" windowHeight="19860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38180" windowHeight="19860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -25,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -349,21 +350,6 @@
     <t>[fonts]</t>
   </si>
   <si>
-    <t>FNT_Bold;FNT_Default;FNT_RU</t>
-  </si>
-  <si>
-    <t>FNT_ZH_Simpl</t>
-  </si>
-  <si>
-    <t>FNT_ZH_Trad</t>
-  </si>
-  <si>
-    <t>FNT_JA</t>
-  </si>
-  <si>
-    <t>FNT_KO</t>
-  </si>
-  <si>
     <t>[defaultFont]</t>
   </si>
   <si>
@@ -383,12 +369,27 @@
   </si>
   <si>
     <t>{fontGroupsDefinitions}</t>
+  </si>
+  <si>
+    <t>FNT_Bold;FNT_Default;FNT_RU;FNT_Numbers</t>
+  </si>
+  <si>
+    <t>FNT_ZH_Simpl;FNT_Numbers</t>
+  </si>
+  <si>
+    <t>FNT_ZH_Trad;FNT_Numbers</t>
+  </si>
+  <si>
+    <t>FNT_JA;FNT_Numbers</t>
+  </si>
+  <si>
+    <t>FNT_KO;FNT_Numbers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -745,60 +746,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -902,6 +849,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -909,15 +865,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -942,6 +889,30 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -1220,6 +1191,26 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1725,6 +1716,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1739,84 +1740,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
-  <autoFilter ref="B4:P5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="B4:P5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="44"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="43"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="42"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="41"/>
-    <tableColumn id="5" name="[incentivizeFBGem]"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]"/>
-    <tableColumn id="7" name="[miniMapHCCost]"/>
-    <tableColumn id="8" name="[miniMapTimer]"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{gameSettings}" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[timeToPCCoefA]" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[timeToPCCoefB]" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incentivizeFBGem]"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[dailyAdsRemoveMissions]"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[maxAdsSkipMissions]"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[cooldownAdsSkipMissions]"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[miniMapHCCost]"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[miniMapTimer]"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[missingRessourcesPCperSC]"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[flyingPigsProbaCoefA]"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[flyingPigsProbaCoefB]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
-  <autoFilter ref="B10:F11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="B10:F11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="36"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="35"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="34"/>
-    <tableColumn id="4" name="[hardCurrency]" dataDxfId="33"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{initialSettings}" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[softCurrency]" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[hardCurrency]" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[initialDragonSKU]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F18" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
-  <autoFilter ref="B16:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F18" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="B16:F18" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="27"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="26"/>
-    <tableColumn id="3" name="[active]" dataDxfId="25"/>
-    <tableColumn id="4" name="[icon]"/>
-    <tableColumn id="5" name="[tidName]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{seasonsDefinitions}" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[active]" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="[icon]"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K15" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="B4:K15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K15" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="B4:K15" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="20"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="19"/>
-    <tableColumn id="3" name="[order]" dataDxfId="18"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="17"/>
-    <tableColumn id="11" name="[android]" dataDxfId="16"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="15"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="14"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="13"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="4"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{localizationDefinitions}" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="[sku]" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="[order]" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[isoCode]" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="[android]" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="[iOS]" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[txtFilename]" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[icon]" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[fontGroup]" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="[tidName]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B20:E25" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
-  <autoFilter ref="B20:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B20:E25" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B20:E25" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="7"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="6"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="5"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{fontGroupsDefinitions}" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="[fonts]" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[defaultFont]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2084,7 +2085,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
@@ -2352,10 +2353,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D18"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D18" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2368,14 +2369,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="B1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2441,7 +2442,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K4" s="24" t="s">
         <v>74</v>
@@ -2790,7 +2791,7 @@
         <v>86</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J15" s="17" t="s">
         <v>92</v>
@@ -2802,7 +2803,7 @@
     <row r="17" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:10" ht="24" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -2818,14 +2819,14 @@
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="2:10" ht="118" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>8</v>
@@ -2834,7 +2835,7 @@
         <v>95</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
@@ -2845,10 +2846,10 @@
         <v>90</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
@@ -2859,7 +2860,7 @@
         <v>91</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E22" s="18"/>
     </row>
@@ -2871,7 +2872,7 @@
         <v>92</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E23" s="18"/>
     </row>
@@ -2883,7 +2884,7 @@
         <v>93</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E24" s="18"/>
     </row>
@@ -2895,25 +2896,25 @@
         <v>94</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E25" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C15">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C25">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G15">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G15" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J5:J15">
+    <dataValidation type="list" allowBlank="1" sqref="J5:J15" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$C$21:$C$25</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D21:E25"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D21:E25" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>

<commit_message>
Content - add new powers + add new season
Former-commit-id: f02c254af0591b913bdac547aff785d4f727a905
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B040C215-FB73-384A-BA6B-41A39B75DAE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38180" windowHeight="19860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -26,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="I4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="111">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -384,13 +383,22 @@
   </si>
   <si>
     <t>FNT_KO;FNT_Numbers</t>
+  </si>
+  <si>
+    <t>spring</t>
+  </si>
+  <si>
+    <t>icon_season_spring</t>
+  </si>
+  <si>
+    <t>TID_SEASON_SPRING_NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,6 +463,13 @@
       <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -655,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -716,6 +731,7 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1740,84 +1756,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
-  <autoFilter ref="B4:P5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="B4:P5"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{gameSettings}" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[timeToPCCoefA]" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[timeToPCCoefB]" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incentivizeFBGem]"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[dailyAdsRemoveMissions]"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[maxAdsSkipMissions]"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[cooldownAdsSkipMissions]"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[miniMapHCCost]"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[miniMapTimer]"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[missingRessourcesPCperSC]"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[flyingPigsProbaCoefA]"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[flyingPigsProbaCoefB]"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="43"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="42"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="41"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="40"/>
+    <tableColumn id="5" name="[incentivizeFBGem]"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]"/>
+    <tableColumn id="7" name="[miniMapHCCost]"/>
+    <tableColumn id="8" name="[miniMapTimer]"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
-  <autoFilter ref="B10:F11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="B10:F11"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{initialSettings}" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[softCurrency]" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[hardCurrency]" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[initialDragonSKU]" dataDxfId="31"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="35"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="34"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="33"/>
+    <tableColumn id="4" name="[hardCurrency]" dataDxfId="32"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F18" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="B16:F18" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F19" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="B16:F19"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{seasonsDefinitions}" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[active]" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="[icon]"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="26"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="3" name="[active]" dataDxfId="24"/>
+    <tableColumn id="4" name="[icon]"/>
+    <tableColumn id="5" name="[tidName]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K15" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
-  <autoFilter ref="B4:K15" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K15" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="B4:K15"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{localizationDefinitions}" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="[sku]" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="[order]" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[isoCode]" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="[android]" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="[iOS]" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[txtFilename]" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[icon]" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[fontGroup]" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="[tidName]" dataDxfId="8"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="17"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="16"/>
+    <tableColumn id="3" name="[order]" dataDxfId="15"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="14"/>
+    <tableColumn id="11" name="[android]" dataDxfId="13"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="12"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="11"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="10"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="9"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B20:E25" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B20:E25" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B20:E25" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B20:E25"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{fontGroupsDefinitions}" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="[fonts]" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[defaultFont]" dataDxfId="0"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="3"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="1"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2085,30 +2101,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
@@ -2122,7 +2138,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="14"/>
       <c r="C3" s="13"/>
@@ -2137,7 +2153,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:16" ht="303" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="306" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -2184,7 +2200,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2231,8 +2247,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -2246,7 +2262,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="10" spans="1:16" ht="94" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -2263,7 +2279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2280,8 +2296,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
@@ -2295,7 +2311,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="16" spans="1:16" ht="103" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="104.25" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2312,7 +2328,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2329,7 +2345,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
@@ -2346,7 +2362,24 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
         <v>0</v>
       </c>
@@ -2356,7 +2389,7 @@
     <cfRule type="duplicateValues" dxfId="48" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D18" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D19"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2369,31 +2402,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A7" zoomScale="101" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="6" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>82</v>
       </c>
@@ -2406,7 +2439,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="28"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2416,7 +2449,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="116" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="119.25" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>80</v>
       </c>
@@ -2448,7 +2481,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
@@ -2480,7 +2513,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
@@ -2512,7 +2545,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
@@ -2544,7 +2577,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
@@ -2576,7 +2609,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
         <v>3</v>
       </c>
@@ -2608,7 +2641,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>3</v>
       </c>
@@ -2640,7 +2673,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>3</v>
       </c>
@@ -2672,7 +2705,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>3</v>
       </c>
@@ -2704,7 +2737,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>3</v>
       </c>
@@ -2736,7 +2769,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>3</v>
       </c>
@@ -2768,7 +2801,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
         <v>3</v>
       </c>
@@ -2800,8 +2833,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:10" ht="24" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B18" s="7" t="s">
         <v>101</v>
       </c>
@@ -2814,7 +2847,7 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="2:10" ht="75" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B19" s="28"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -2824,7 +2857,7 @@
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:10" ht="118" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" ht="118.5" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>102</v>
       </c>
@@ -2838,7 +2871,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="s">
         <v>3</v>
       </c>
@@ -2852,7 +2885,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
         <v>3</v>
       </c>
@@ -2864,7 +2897,7 @@
       </c>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
         <v>3</v>
       </c>
@@ -2876,7 +2909,7 @@
       </c>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="23" t="s">
         <v>3</v>
       </c>
@@ -2888,7 +2921,7 @@
       </c>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="23" t="s">
         <v>3</v>
       </c>
@@ -2908,13 +2941,13 @@
     <cfRule type="duplicateValues" dxfId="22" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G15" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G15">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J5:J15" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="J5:J15">
       <formula1>$C$21:$C$25</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D21:E25" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D21:E25"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>

<commit_message>
Content - Add spring season
Former-commit-id: a008e1b6860d8e687bc6ae3fd29e090f5733dc4c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B040C215-FB73-384A-BA6B-41A39B75DAE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38180" windowHeight="19860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -26,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="I4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="111">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -384,13 +383,22 @@
   </si>
   <si>
     <t>FNT_KO;FNT_Numbers</t>
+  </si>
+  <si>
+    <t>spring</t>
+  </si>
+  <si>
+    <t>icon_season_spring</t>
+  </si>
+  <si>
+    <t>TID_SEASON_SPRING_NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,6 +463,13 @@
       <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -655,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -716,6 +731,7 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1740,84 +1756,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
-  <autoFilter ref="B4:P5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="B4:P5"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{gameSettings}" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[timeToPCCoefA]" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[timeToPCCoefB]" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incentivizeFBGem]"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[dailyAdsRemoveMissions]"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[maxAdsSkipMissions]"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[cooldownAdsSkipMissions]"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[miniMapHCCost]"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[miniMapTimer]"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[missingRessourcesPCperSC]"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[flyingPigsProbaCoefA]"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[flyingPigsProbaCoefB]"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="43"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="42"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="41"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="40"/>
+    <tableColumn id="5" name="[incentivizeFBGem]"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]"/>
+    <tableColumn id="7" name="[miniMapHCCost]"/>
+    <tableColumn id="8" name="[miniMapTimer]"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
-  <autoFilter ref="B10:F11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="B10:F11"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{initialSettings}" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[softCurrency]" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[hardCurrency]" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[initialDragonSKU]" dataDxfId="31"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="35"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="34"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="33"/>
+    <tableColumn id="4" name="[hardCurrency]" dataDxfId="32"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F18" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="B16:F18" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F19" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="B16:F19"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{seasonsDefinitions}" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[active]" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="[icon]"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="26"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="3" name="[active]" dataDxfId="24"/>
+    <tableColumn id="4" name="[icon]"/>
+    <tableColumn id="5" name="[tidName]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K15" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
-  <autoFilter ref="B4:K15" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K15" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="B4:K15"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{localizationDefinitions}" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="[sku]" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="[order]" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[isoCode]" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="[android]" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="[iOS]" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[txtFilename]" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[icon]" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[fontGroup]" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="[tidName]" dataDxfId="8"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="17"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="16"/>
+    <tableColumn id="3" name="[order]" dataDxfId="15"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="14"/>
+    <tableColumn id="11" name="[android]" dataDxfId="13"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="12"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="11"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="10"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="9"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B20:E25" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B20:E25" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B20:E25" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B20:E25"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{fontGroupsDefinitions}" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="[fonts]" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[defaultFont]" dataDxfId="0"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="3"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="1"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2085,30 +2101,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
@@ -2122,7 +2138,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="14"/>
       <c r="C3" s="13"/>
@@ -2137,7 +2153,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:16" ht="303" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="306" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -2184,7 +2200,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2231,8 +2247,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -2246,7 +2262,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="10" spans="1:16" ht="94" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -2263,7 +2279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2280,8 +2296,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
@@ -2295,7 +2311,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="16" spans="1:16" ht="103" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="104.25" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2312,7 +2328,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2329,7 +2345,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
@@ -2346,7 +2362,24 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
         <v>0</v>
       </c>
@@ -2356,7 +2389,7 @@
     <cfRule type="duplicateValues" dxfId="48" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D18" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D19"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2369,31 +2402,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="B16" zoomScale="101" workbookViewId="0">
+      <selection activeCell="H21" sqref="F21:H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="6" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>82</v>
       </c>
@@ -2406,7 +2439,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="28"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2416,7 +2449,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="116" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="119.25" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>80</v>
       </c>
@@ -2448,7 +2481,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
@@ -2480,7 +2513,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
@@ -2512,7 +2545,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
@@ -2544,7 +2577,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
@@ -2576,7 +2609,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
         <v>3</v>
       </c>
@@ -2608,7 +2641,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>3</v>
       </c>
@@ -2640,7 +2673,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>3</v>
       </c>
@@ -2672,7 +2705,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>3</v>
       </c>
@@ -2704,7 +2737,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>3</v>
       </c>
@@ -2736,7 +2769,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>3</v>
       </c>
@@ -2768,7 +2801,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
         <v>3</v>
       </c>
@@ -2800,8 +2833,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:10" ht="24" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B18" s="7" t="s">
         <v>101</v>
       </c>
@@ -2814,7 +2847,7 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="2:10" ht="75" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B19" s="28"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -2824,7 +2857,7 @@
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:10" ht="118" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" ht="118.5" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>102</v>
       </c>
@@ -2838,7 +2871,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="s">
         <v>3</v>
       </c>
@@ -2852,7 +2885,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
         <v>3</v>
       </c>
@@ -2864,7 +2897,7 @@
       </c>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
         <v>3</v>
       </c>
@@ -2876,7 +2909,7 @@
       </c>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="23" t="s">
         <v>3</v>
       </c>
@@ -2888,7 +2921,7 @@
       </c>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="23" t="s">
         <v>3</v>
       </c>
@@ -2908,13 +2941,13 @@
     <cfRule type="duplicateValues" dxfId="22" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G15" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G15">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J5:J15" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="J5:J15">
       <formula1>$C$21:$C$25</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D21:E25" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D21:E25"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>

<commit_message>
[RULES] languages other than english disabled.
Former-commit-id: 6877797bba987f8f6c3a7a78f901eaf3c3477bd2
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19860"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19470" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +25,7 @@
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="I4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -397,7 +392,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2094,7 +2089,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2107,7 +2102,7 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -2408,8 +2403,8 @@
   </sheetPr>
   <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H21" sqref="F21:H21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2527,10 +2522,10 @@
         <v>68</v>
       </c>
       <c r="F6" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>67</v>
@@ -2559,10 +2554,10 @@
         <v>64</v>
       </c>
       <c r="F7" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>63</v>
@@ -2591,10 +2586,10 @@
         <v>60</v>
       </c>
       <c r="F8" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>59</v>
@@ -2623,10 +2618,10 @@
         <v>56</v>
       </c>
       <c r="F9" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>55</v>
@@ -2655,10 +2650,10 @@
         <v>52</v>
       </c>
       <c r="F10" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="17" t="s">
         <v>51</v>
@@ -2687,10 +2682,10 @@
         <v>48</v>
       </c>
       <c r="F11" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>47</v>
@@ -2719,10 +2714,10 @@
         <v>89</v>
       </c>
       <c r="F12" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>44</v>
@@ -2751,10 +2746,10 @@
         <v>41</v>
       </c>
       <c r="F13" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="17" t="s">
         <v>40</v>
@@ -2783,10 +2778,10 @@
         <v>37</v>
       </c>
       <c r="F14" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>36</v>
@@ -2815,10 +2810,10 @@
         <v>88</v>
       </c>
       <c r="F15" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="17" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
Content - Activate Spring season
Former-commit-id: 50aae2bb857caf187b3513e29fe44f2b02c42ccd
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19470" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19470"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +30,7 @@
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0">
+    <comment ref="I4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -392,7 +397,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2089,7 +2094,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2102,8 +2107,8 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2365,7 +2370,7 @@
         <v>108</v>
       </c>
       <c r="D19" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
         <v>109</v>
@@ -2403,7 +2408,7 @@
   </sheetPr>
   <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="101" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[REVERT] David's merge of April 9th
Former-commit-id: e9ebf10d7278668ea66491c948ea396ea4f0e26d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19470" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +30,7 @@
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0">
+    <comment ref="I4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -392,7 +397,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2089,7 +2094,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2102,7 +2107,7 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -2403,8 +2408,8 @@
   </sheetPr>
   <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="B16" zoomScale="101" workbookViewId="0">
+      <selection activeCell="H21" sqref="F21:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,10 +2527,10 @@
         <v>68</v>
       </c>
       <c r="F6" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>67</v>
@@ -2554,10 +2559,10 @@
         <v>64</v>
       </c>
       <c r="F7" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>63</v>
@@ -2586,10 +2591,10 @@
         <v>60</v>
       </c>
       <c r="F8" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>59</v>
@@ -2618,10 +2623,10 @@
         <v>56</v>
       </c>
       <c r="F9" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>55</v>
@@ -2650,10 +2655,10 @@
         <v>52</v>
       </c>
       <c r="F10" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="17" t="s">
         <v>51</v>
@@ -2682,10 +2687,10 @@
         <v>48</v>
       </c>
       <c r="F11" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>47</v>
@@ -2714,10 +2719,10 @@
         <v>89</v>
       </c>
       <c r="F12" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>44</v>
@@ -2746,10 +2751,10 @@
         <v>41</v>
       </c>
       <c r="F13" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="17" t="s">
         <v>40</v>
@@ -2778,10 +2783,10 @@
         <v>37</v>
       </c>
       <c r="F14" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>36</v>
@@ -2810,10 +2815,10 @@
         <v>88</v>
       </c>
       <c r="F15" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="17" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
[REVERT] Reverting David's Commit Revert x_x
Former-commit-id: 215250c381d09ec04bcbe716506a513c4a156ee3
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19470"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19470" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +25,7 @@
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="I4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -397,7 +392,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2094,7 +2089,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2107,8 +2102,8 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2370,7 +2365,7 @@
         <v>108</v>
       </c>
       <c r="D19" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
         <v>109</v>
@@ -2408,7 +2403,7 @@
   </sheetPr>
   <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="101" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding Turkish font and 'language'
Former-commit-id: 725a51a55d13a51b7499711b2cc109b41537ac29
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19470" activeTab="1"/>
   </bookViews>
@@ -25,7 +30,7 @@
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0">
+    <comment ref="I4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="118">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -387,12 +392,33 @@
   </si>
   <si>
     <t>TID_SEASON_SPRING_NAME</t>
+  </si>
+  <si>
+    <t>lang_turkish</t>
+  </si>
+  <si>
+    <t>tr-TR</t>
+  </si>
+  <si>
+    <t>turkish</t>
+  </si>
+  <si>
+    <t>flags_turkish</t>
+  </si>
+  <si>
+    <t>tr</t>
+  </si>
+  <si>
+    <t>FNT_Bold;FNT_TR;FNT_Numbers</t>
+  </si>
+  <si>
+    <t>FNT_TR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -665,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -727,11 +753,42 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="49">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1202,26 +1259,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1727,16 +1764,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1751,13 +1778,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="B4:P5"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="43"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="42"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="41"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="40"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="44"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="43"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="42"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="41"/>
     <tableColumn id="5" name="[incentivizeFBGem]"/>
     <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
     <tableColumn id="15" name="[maxAdsSkipMissions]"/>
@@ -1775,26 +1802,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <autoFilter ref="B10:F11"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="35"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="34"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="33"/>
-    <tableColumn id="4" name="[hardCurrency]" dataDxfId="32"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="31"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="36"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="35"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="34"/>
+    <tableColumn id="4" name="[hardCurrency]" dataDxfId="33"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F19" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F19" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="B16:F19"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="26"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
-    <tableColumn id="3" name="[active]" dataDxfId="24"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="27"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="26"/>
+    <tableColumn id="3" name="[active]" dataDxfId="25"/>
     <tableColumn id="4" name="[icon]"/>
     <tableColumn id="5" name="[tidName]"/>
   </tableColumns>
@@ -1803,32 +1830,32 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K15" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
-  <autoFilter ref="B4:K15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K16" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+  <autoFilter ref="B4:K16"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="17"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="16"/>
-    <tableColumn id="3" name="[order]" dataDxfId="15"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="14"/>
-    <tableColumn id="11" name="[android]" dataDxfId="13"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="12"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="11"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="10"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="9"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="8"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="20"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="19"/>
+    <tableColumn id="3" name="[order]" dataDxfId="18"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="17"/>
+    <tableColumn id="11" name="[android]" dataDxfId="16"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="15"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="14"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="13"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="12"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B20:E25" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B20:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="3"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="1"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="0"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="6"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="4"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2089,7 +2116,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2381,7 +2408,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D19"/>
@@ -2401,10 +2428,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="B1:K25"/>
+  <dimension ref="B1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="101" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2828,56 +2855,74 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B18" s="7" t="s">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="19">
+        <v>11</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B19" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="2:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B19" s="28"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="B20" s="28"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="2:10" ht="118.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="2:10" ht="118.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D21" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E21" s="31" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -2885,22 +2930,24 @@
         <v>3</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="E22" s="18"/>
+        <v>103</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E23" s="18"/>
     </row>
@@ -2909,10 +2956,10 @@
         <v>3</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E24" s="18"/>
     </row>
@@ -2921,33 +2968,60 @@
         <v>3</v>
       </c>
       <c r="C25" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D26" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="22"/>
+      <c r="E26" s="22"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C15">
-    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
+  <conditionalFormatting sqref="C5:C16">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C25">
-    <cfRule type="duplicateValues" dxfId="22" priority="3"/>
+  <conditionalFormatting sqref="C22:C27">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G15">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G16">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J5:J15">
-      <formula1>$C$21:$C$25</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="J5:J16">
+      <formula1>$C$22:$C$27</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D21:E25"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E22:E27 D22:D26"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Localization: Content - All languages enabled! (Except Android Chinese :( )
Former-commit-id: 5f5e36208d47a09a2a0db11b2955c0c24bcf9a29
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DBF94286-D72D-3148-8D98-D4A3661101D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19470" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38180" windowHeight="19480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -25,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -418,7 +419,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -760,36 +761,6 @@
   </cellStyles>
   <dxfs count="49">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1259,6 +1230,26 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1764,6 +1755,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1778,84 +1779,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
-  <autoFilter ref="B4:P5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="B4:P5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="44"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="43"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="42"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="41"/>
-    <tableColumn id="5" name="[incentivizeFBGem]"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]"/>
-    <tableColumn id="7" name="[miniMapHCCost]"/>
-    <tableColumn id="8" name="[miniMapTimer]"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{gameSettings}" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[timeToPCCoefA]" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[timeToPCCoefB]" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incentivizeFBGem]"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[dailyAdsRemoveMissions]"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[maxAdsSkipMissions]"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[cooldownAdsSkipMissions]"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[miniMapHCCost]"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[miniMapTimer]"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[missingRessourcesPCperSC]"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[flyingPigsProbaCoefA]"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[flyingPigsProbaCoefB]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
-  <autoFilter ref="B10:F11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="B10:F11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="36"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="35"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="34"/>
-    <tableColumn id="4" name="[hardCurrency]" dataDxfId="33"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{initialSettings}" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[softCurrency]" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[hardCurrency]" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[initialDragonSKU]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F19" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
-  <autoFilter ref="B16:F19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F19" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="B16:F19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="27"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="26"/>
-    <tableColumn id="3" name="[active]" dataDxfId="25"/>
-    <tableColumn id="4" name="[icon]"/>
-    <tableColumn id="5" name="[tidName]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{seasonsDefinitions}" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[active]" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="[icon]"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K16" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="B4:K16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K16" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="B4:K16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="20"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="19"/>
-    <tableColumn id="3" name="[order]" dataDxfId="18"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="17"/>
-    <tableColumn id="11" name="[android]" dataDxfId="16"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="15"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="14"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="13"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="12"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{localizationDefinitions}" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="[sku]" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="[order]" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[isoCode]" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="[android]" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="[iOS]" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[txtFilename]" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[icon]" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[fontGroup]" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="[tidName]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="B21:E27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B21:E27" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="6"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="4"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{fontGroupsDefinitions}" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="[fonts]" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[defaultFont]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2123,7 +2124,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
@@ -2133,20 +2134,20 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
     <col min="8" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
@@ -2160,7 +2161,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="14"/>
       <c r="C3" s="13"/>
@@ -2175,7 +2176,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:16" ht="306" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="303" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -2222,7 +2223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2269,8 +2270,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -2284,7 +2285,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="10" spans="1:16" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="94" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -2301,7 +2302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2318,8 +2319,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
@@ -2333,7 +2334,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="16" spans="1:16" ht="104.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="103" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2350,7 +2351,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
@@ -2384,7 +2385,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="32" t="s">
         <v>3</v>
       </c>
@@ -2401,17 +2402,17 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G22" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D19"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D19" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2424,31 +2425,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="B1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" customWidth="1"/>
-    <col min="6" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>82</v>
       </c>
@@ -2461,7 +2462,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.2">
       <c r="B3" s="28"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2471,7 +2472,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="119.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="116" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>80</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
@@ -2535,7 +2536,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
@@ -2549,10 +2550,10 @@
         <v>68</v>
       </c>
       <c r="F6" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>67</v>
@@ -2567,7 +2568,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
@@ -2581,10 +2582,10 @@
         <v>64</v>
       </c>
       <c r="F7" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>63</v>
@@ -2599,7 +2600,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
@@ -2613,10 +2614,10 @@
         <v>60</v>
       </c>
       <c r="F8" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>59</v>
@@ -2631,7 +2632,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="23" t="s">
         <v>3</v>
       </c>
@@ -2645,10 +2646,10 @@
         <v>56</v>
       </c>
       <c r="F9" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>55</v>
@@ -2663,7 +2664,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="23" t="s">
         <v>3</v>
       </c>
@@ -2677,10 +2678,10 @@
         <v>52</v>
       </c>
       <c r="F10" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="17" t="s">
         <v>51</v>
@@ -2695,7 +2696,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="23" t="s">
         <v>3</v>
       </c>
@@ -2709,10 +2710,10 @@
         <v>48</v>
       </c>
       <c r="F11" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>47</v>
@@ -2727,7 +2728,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
         <v>3</v>
       </c>
@@ -2744,7 +2745,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>44</v>
@@ -2759,7 +2760,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="23" t="s">
         <v>3</v>
       </c>
@@ -2773,10 +2774,10 @@
         <v>41</v>
       </c>
       <c r="F13" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="17" t="s">
         <v>40</v>
@@ -2791,7 +2792,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
         <v>3</v>
       </c>
@@ -2805,10 +2806,10 @@
         <v>37</v>
       </c>
       <c r="F14" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>36</v>
@@ -2823,7 +2824,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
         <v>3</v>
       </c>
@@ -2837,10 +2838,10 @@
         <v>88</v>
       </c>
       <c r="F15" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="17" t="s">
         <v>86</v>
@@ -2855,7 +2856,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -2869,10 +2870,10 @@
         <v>112</v>
       </c>
       <c r="F16" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="17" t="s">
         <v>113</v>
@@ -2887,8 +2888,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:10" ht="24" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>101</v>
       </c>
@@ -2901,7 +2902,7 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="75" x14ac:dyDescent="0.2">
       <c r="B20" s="28"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -2911,7 +2912,7 @@
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:10" ht="118.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="118" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
         <v>102</v>
       </c>
@@ -2925,7 +2926,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="23" t="s">
         <v>3</v>
       </c>
@@ -2939,7 +2940,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="23" t="s">
         <v>3</v>
       </c>
@@ -2951,7 +2952,7 @@
       </c>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="23" t="s">
         <v>3</v>
       </c>
@@ -2963,7 +2964,7 @@
       </c>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="23" t="s">
         <v>3</v>
       </c>
@@ -2975,7 +2976,7 @@
       </c>
       <c r="E25" s="18"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="23" t="s">
         <v>3</v>
       </c>
@@ -2987,7 +2988,7 @@
       </c>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="23" t="s">
         <v>3</v>
       </c>
@@ -3003,19 +3004,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G16">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G16" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J5:J16">
+    <dataValidation type="list" allowBlank="1" sqref="J5:J16" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$C$22:$C$27</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E22:E27 D22:D26"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E22:E27 D22:D26" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Pre-Reg Rewards: Development - Added popup, integrated into the flow. Pre-Reg Rewards: Content - Created new content tables for the pre-reg rewards. Tutorial Step: Development - Added new step (pre-reg rewards), adjusted other steps to match the new flow.
Former-commit-id: bd761571db7c95c8c8efab2c2ec3f04f616a6af8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DBF94286-D72D-3148-8D98-D4A3661101D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ECA97C19-DC3A-F64F-818D-57A3237157D6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38180" windowHeight="19480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="440" windowWidth="38180" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="142">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -414,6 +414,78 @@
   </si>
   <si>
     <t>FNT_TR</t>
+  </si>
+  <si>
+    <t>PRE-REGISTRATION REWARDS DEFINITIONS</t>
+  </si>
+  <si>
+    <t>{preRegRewardsDefinitions}</t>
+  </si>
+  <si>
+    <t>prereg_reward_1</t>
+  </si>
+  <si>
+    <t>[threshold]</t>
+  </si>
+  <si>
+    <t>[type]</t>
+  </si>
+  <si>
+    <t>[amount]</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>[rewardSku]</t>
+  </si>
+  <si>
+    <t>prereg_reward_2</t>
+  </si>
+  <si>
+    <t>prereg_reward_3</t>
+  </si>
+  <si>
+    <t>prereg_reward_4</t>
+  </si>
+  <si>
+    <t>prereg_reward_5</t>
+  </si>
+  <si>
+    <t>prereg_reward_6</t>
+  </si>
+  <si>
+    <t>prereg_reward_7</t>
+  </si>
+  <si>
+    <t>prereg_reward_8</t>
+  </si>
+  <si>
+    <t>prereg_reward_9</t>
+  </si>
+  <si>
+    <t>prereg_reward_10</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>gf</t>
+  </si>
+  <si>
+    <t>pet</t>
+  </si>
+  <si>
+    <t>pet_67</t>
+  </si>
+  <si>
+    <t>egg_premium</t>
+  </si>
+  <si>
+    <t>egg_betterRates</t>
   </si>
 </sst>
 </file>
@@ -575,7 +647,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -688,11 +760,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -755,11 +847,27 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="56">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1250,6 +1358,196 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1779,13 +2077,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="54" headerRowBorderDxfId="53" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="B4:P5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{gameSettings}" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[timeToPCCoefA]" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[timeToPCCoefB]" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{gameSettings}" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[timeToPCCoefA]" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[timeToPCCoefB]" dataDxfId="47"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incentivizeFBGem]"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[dailyAdsRemoveMissions]"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[maxAdsSkipMissions]"/>
@@ -1803,26 +2101,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="B10:F11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{initialSettings}" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[softCurrency]" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[hardCurrency]" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[initialDragonSKU]" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{initialSettings}" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[softCurrency]" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[hardCurrency]" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[initialDragonSKU]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F19" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F19" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="B16:F19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{seasonsDefinitions}" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[active]" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{seasonsDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[active]" dataDxfId="31"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="[icon]"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]"/>
   </tableColumns>
@@ -1831,6 +2129,24 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{40DA669D-54CE-2249-93B2-544AD0ACA808}" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B24:G34" totalsRowShown="0" headerRowDxfId="30">
+  <autoFilter ref="B24:G34" xr:uid="{F641F703-C53C-E145-ADB5-39185E5CF808}"/>
+  <sortState ref="B25:G34">
+    <sortCondition descending="1" ref="D24:D34"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{9BC02FCC-385F-FA42-8F04-64A63CF90989}" name="{preRegRewardsDefinitions}" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{C0C44249-EE53-BC46-9AC0-C3D7B89DC9E2}" name="[sku]" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{1DE38860-3E86-1544-99D2-F7E4A83EDDD2}" name="[threshold]" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{80BEDF12-1019-7747-8DE3-FA98D7D51C0C}" name="[type]" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{141497E1-8845-2244-9F9B-96B6BFA644D2}" name="[amount]" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{804FA1A8-A3B2-474D-852F-0C732507C408}" name="[rewardSku]" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K16" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="B4:K16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="10">
@@ -1849,7 +2165,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B21:E27" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
@@ -2128,21 +2444,21 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
     <col min="8" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2402,24 +2718,243 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
       <c r="G22" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="24" spans="2:7" ht="135" x14ac:dyDescent="0.2">
+      <c r="B24" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="39">
+        <v>3000000</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="19">
+        <v>1</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D26" s="39">
+        <v>2500000</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="19">
+        <v>5</v>
+      </c>
+      <c r="G26" s="19"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="39">
+        <v>2000000</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F27" s="19">
+        <v>1</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="39">
+        <v>1500000</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" s="19">
+        <v>5</v>
+      </c>
+      <c r="G28" s="19"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="39">
+        <v>1000000</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F29" s="19">
+        <v>1</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="39">
+        <v>500000</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F30" s="19">
+        <v>5</v>
+      </c>
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="39">
+        <v>250000</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="19">
+        <v>5</v>
+      </c>
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="39">
+        <v>100000</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F32" s="19">
+        <v>1500</v>
+      </c>
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="39">
+        <v>50000</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" s="19">
+        <v>500</v>
+      </c>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="39">
+        <v>10000</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" s="19">
+        <v>100</v>
+      </c>
+      <c r="G34" s="19"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="1"/>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D19" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D19 D25:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" sqref="E25:E34" xr:uid="{B2CC7A79-55F3-8B47-8EF0-FC15C2333D69}">
+      <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2431,7 +2966,7 @@
   </sheetPr>
   <dimension ref="B1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="101" workbookViewId="0">
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Localization: Content - Disabled all languages except english... AGAIN -____-
Former-commit-id: 65884fa508a48866d0522c8b9fa6cc797798454c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DBF94286-D72D-3148-8D98-D4A3661101D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5FBB355B-DA54-8640-8553-9C7A293869BD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="38180" windowHeight="19480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2432,7 +2432,7 @@
   <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2550,10 +2550,10 @@
         <v>68</v>
       </c>
       <c r="F6" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>67</v>
@@ -2582,10 +2582,10 @@
         <v>64</v>
       </c>
       <c r="F7" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>63</v>
@@ -2614,10 +2614,10 @@
         <v>60</v>
       </c>
       <c r="F8" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>59</v>
@@ -2646,10 +2646,10 @@
         <v>56</v>
       </c>
       <c r="F9" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>55</v>
@@ -2678,10 +2678,10 @@
         <v>52</v>
       </c>
       <c r="F10" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="17" t="s">
         <v>51</v>
@@ -2710,10 +2710,10 @@
         <v>48</v>
       </c>
       <c r="F11" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>47</v>
@@ -2745,7 +2745,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>44</v>
@@ -2774,10 +2774,10 @@
         <v>41</v>
       </c>
       <c r="F13" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="17" t="s">
         <v>40</v>
@@ -2806,10 +2806,10 @@
         <v>37</v>
       </c>
       <c r="F14" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>36</v>
@@ -2838,10 +2838,10 @@
         <v>88</v>
       </c>
       <c r="F15" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="17" t="s">
         <v>86</v>
@@ -2870,10 +2870,10 @@
         <v>112</v>
       </c>
       <c r="F16" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="17" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Localization: Content - Added new column "serverCode" to match codes used by server features such as Customizer.
Former-commit-id: b46d81284cf3cf814fc3d975fc2b9933d7054531
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ECA97C19-DC3A-F64F-818D-57A3237157D6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E54D11CE-8BFC-A745-B66E-D20B6964FFE9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="440" windowWidth="38180" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38180" windowHeight="19480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="152">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -486,6 +486,36 @@
   </si>
   <si>
     <t>egg_betterRates</t>
+  </si>
+  <si>
+    <t>[serverCode]</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>pt</t>
+  </si>
+  <si>
+    <t>ru</t>
+  </si>
+  <si>
+    <t>zh_cn</t>
+  </si>
+  <si>
+    <t>zh_tw</t>
   </si>
 </sst>
 </file>
@@ -867,7 +897,61 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="57">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1338,26 +1422,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2053,16 +2117,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2077,13 +2131,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="54" headerRowBorderDxfId="53" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
   <autoFilter ref="B4:P5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{gameSettings}" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[timeToPCCoefA]" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[timeToPCCoefB]" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{gameSettings}" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[timeToPCCoefA]" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[timeToPCCoefB]" dataDxfId="49"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incentivizeFBGem]"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[dailyAdsRemoveMissions]"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[maxAdsSkipMissions]"/>
@@ -2101,26 +2155,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="B10:F11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{initialSettings}" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[softCurrency]" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[hardCurrency]" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[initialDragonSKU]" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{initialSettings}" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[softCurrency]" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[hardCurrency]" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[initialDragonSKU]" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F19" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F19" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <autoFilter ref="B16:F19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{seasonsDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[active]" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{seasonsDefinitions}" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[active]" dataDxfId="33"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="[icon]"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]"/>
   </tableColumns>
@@ -2129,50 +2183,51 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{40DA669D-54CE-2249-93B2-544AD0ACA808}" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B24:G34" totalsRowShown="0" headerRowDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{40DA669D-54CE-2249-93B2-544AD0ACA808}" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B24:G34" totalsRowShown="0" headerRowDxfId="32">
   <autoFilter ref="B24:G34" xr:uid="{F641F703-C53C-E145-ADB5-39185E5CF808}"/>
   <sortState ref="B25:G34">
     <sortCondition descending="1" ref="D24:D34"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9BC02FCC-385F-FA42-8F04-64A63CF90989}" name="{preRegRewardsDefinitions}" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{C0C44249-EE53-BC46-9AC0-C3D7B89DC9E2}" name="[sku]" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{1DE38860-3E86-1544-99D2-F7E4A83EDDD2}" name="[threshold]" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{80BEDF12-1019-7747-8DE3-FA98D7D51C0C}" name="[type]" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{141497E1-8845-2244-9F9B-96B6BFA644D2}" name="[amount]" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{804FA1A8-A3B2-474D-852F-0C732507C408}" name="[rewardSku]" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{9BC02FCC-385F-FA42-8F04-64A63CF90989}" name="{preRegRewardsDefinitions}" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{C0C44249-EE53-BC46-9AC0-C3D7B89DC9E2}" name="[sku]" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{1DE38860-3E86-1544-99D2-F7E4A83EDDD2}" name="[threshold]" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{80BEDF12-1019-7747-8DE3-FA98D7D51C0C}" name="[type]" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{141497E1-8845-2244-9F9B-96B6BFA644D2}" name="[amount]" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{804FA1A8-A3B2-474D-852F-0C732507C408}" name="[rewardSku]" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:K16" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
-  <autoFilter ref="B4:K16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{localizationDefinitions}" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="[sku]" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="[order]" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[isoCode]" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="[android]" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="[iOS]" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[txtFilename]" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[icon]" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[fontGroup]" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="[tidName]" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:L16" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="B4:L16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{localizationDefinitions}" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="[sku]" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="[order]" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[isoCode]" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{D105A335-D7D9-8740-AF31-5544650A460E}" name="[serverCode]" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="[android]" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="[iOS]" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[txtFilename]" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[icon]" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[fontGroup]" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="[tidName]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B21:E27" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{fontGroupsDefinitions}" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="[fonts]" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[defaultFont]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{fontGroupsDefinitions}" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="[sku]" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="[fonts]" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[defaultFont]" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2446,7 +2501,7 @@
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -2939,7 +2994,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="55" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D19 D25:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
@@ -2964,10 +3019,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="B1:K27"/>
+  <dimension ref="B1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="101" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2983,8 +3038,8 @@
     <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>82</v>
       </c>
@@ -2997,7 +3052,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:12" ht="30" x14ac:dyDescent="0.2">
       <c r="B3" s="28"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -3007,7 +3062,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="116" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" ht="116" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>80</v>
       </c>
@@ -3021,25 +3076,28 @@
         <v>78</v>
       </c>
       <c r="F4" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="H4" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="I4" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="J4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="K4" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="L4" s="24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
@@ -3052,26 +3110,29 @@
       <c r="E5" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="18" t="b">
-        <v>1</v>
+      <c r="F5" s="18" t="s">
+        <v>143</v>
       </c>
       <c r="G5" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="J5" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="K5" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="L5" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
@@ -3084,26 +3145,29 @@
       <c r="E6" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="18" t="b">
-        <v>1</v>
+      <c r="F6" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="G6" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="J6" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="K6" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="L6" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
@@ -3116,26 +3180,29 @@
       <c r="E7" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="18" t="b">
-        <v>1</v>
+      <c r="F7" s="22" t="s">
+        <v>145</v>
       </c>
       <c r="G7" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="J7" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="K7" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="L7" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
@@ -3148,26 +3215,29 @@
       <c r="E8" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="18" t="b">
-        <v>1</v>
+      <c r="F8" s="18" t="s">
+        <v>146</v>
       </c>
       <c r="G8" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="J8" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="K8" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="L8" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="23" t="s">
         <v>3</v>
       </c>
@@ -3180,26 +3250,29 @@
       <c r="E9" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="18" t="b">
-        <v>1</v>
+      <c r="F9" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="G9" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="J9" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="K9" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="L9" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="23" t="s">
         <v>3</v>
       </c>
@@ -3212,26 +3285,29 @@
       <c r="E10" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="18" t="b">
-        <v>1</v>
+      <c r="F10" s="18" t="s">
+        <v>148</v>
       </c>
       <c r="G10" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="J10" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="K10" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="L10" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="23" t="s">
         <v>3</v>
       </c>
@@ -3244,26 +3320,29 @@
       <c r="E11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="18" t="b">
-        <v>1</v>
+      <c r="F11" s="18" t="s">
+        <v>149</v>
       </c>
       <c r="G11" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="J11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="L11" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
         <v>3</v>
       </c>
@@ -3276,26 +3355,29 @@
       <c r="E12" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="18" t="b">
+      <c r="F12" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="G12" s="18" t="b">
+      <c r="H12" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="I12" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="J12" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="K12" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="L12" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="23" t="s">
         <v>3</v>
       </c>
@@ -3308,26 +3390,29 @@
       <c r="E13" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="18" t="b">
-        <v>1</v>
+      <c r="F13" s="18" t="s">
+        <v>93</v>
       </c>
       <c r="G13" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="J13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="K13" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="L13" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
         <v>3</v>
       </c>
@@ -3340,26 +3425,29 @@
       <c r="E14" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="18" t="b">
-        <v>1</v>
+      <c r="F14" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="G14" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="J14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="K14" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="L14" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
         <v>3</v>
       </c>
@@ -3372,26 +3460,29 @@
       <c r="E15" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="18" t="b">
-        <v>1</v>
+      <c r="F15" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="G15" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="J15" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="K15" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="L15" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -3404,22 +3495,25 @@
       <c r="E16" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="F16" s="18" t="b">
-        <v>1</v>
+      <c r="F16" s="18" t="s">
+        <v>115</v>
       </c>
       <c r="G16" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="J16" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="K16" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="L16" s="15" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3539,16 +3633,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="22" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F5:G16" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J5:J16" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="K5:K16" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$C$22:$C$27</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E22:E27 D22:D26" xr:uid="{00000000-0002-0000-0100-000002000000}"/>

</xml_diff>

<commit_message>
Content - Season activated by default + New promo IAP
Former-commit-id: 7ffe1d4ea9eb7181abd66bebac37e06806878c7a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -602,6 +602,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2511,8 +2512,8 @@
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2791,7 +2792,7 @@
         <v>152</v>
       </c>
       <c r="D20" s="42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="43" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
Content - Switch off the season Mid Autumn and Activate Halloween!
Former-commit-id: 8170271fef88fa635edc171122a591ebf1d84972
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -2513,7 +2513,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,7 +2758,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>
@@ -2792,7 +2792,7 @@
         <v>152</v>
       </c>
       <c r="D20" s="42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="43" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
Content - Desactivate Season AGAIN ;)
Former-commit-id: 1329d61b205edc52b650e32b3c710cb99f67caa1
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -2513,7 +2513,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,7 +2758,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Content - Activate Season Halloween for detla <O_O/
Former-commit-id: 934c33a6661236848f88b898abc79cc40f7193ee
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -2513,7 +2513,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,7 +2758,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Content - Halloween False!
Former-commit-id: 26eacd0b01e57a133faedf09e52d6f6edb9c3f9a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -2512,8 +2512,8 @@
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,7 +2758,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>
@@ -3025,7 +3025,7 @@
     <cfRule type="duplicateValues" dxfId="56" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D17:D20 D25:D34"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D25:D34 D17:D20"/>
     <dataValidation type="list" sqref="E25:E34">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Content - Fix General Content after merge / Chest 4 now gives GF
Former-commit-id: 20e8a08a37369aa8a43119cea273764e9ab4fd9f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="156">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>TID_SEASON_MIDAUTUMNFESTIVAL_NAME</t>
+  </si>
+  <si>
+    <t>[goldenFragments]</t>
   </si>
 </sst>
 </file>
@@ -823,7 +826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -906,11 +909,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="58">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1783,6 +1787,14 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -2142,13 +2154,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
   <autoFilter ref="B4:P5"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="49"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="48"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="52"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="51"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="50"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="49"/>
     <tableColumn id="5" name="[incentivizeFBGem]"/>
     <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
     <tableColumn id="15" name="[maxAdsSkipMissions]"/>
@@ -2166,13 +2178,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
-  <autoFilter ref="B10:F11"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="43"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="42"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="41"/>
-    <tableColumn id="4" name="[hardCurrency]" dataDxfId="40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+  <autoFilter ref="B10:G11"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="44"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="43"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="42"/>
+    <tableColumn id="4" name="[hardCurrency]" dataDxfId="41"/>
+    <tableColumn id="5" name="[goldenFragments]" dataDxfId="40"/>
     <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2512,8 +2525,8 @@
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,8 +2535,8 @@
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="26" width="12" customWidth="1"/>
   </cols>
@@ -2667,7 +2680,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="10" spans="1:16" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="96.75" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -2680,7 +2693,10 @@
       <c r="E10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2697,7 +2713,10 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="44">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3021,11 +3040,11 @@
       <c r="G34" s="19"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="56" priority="1"/>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="duplicateValues" dxfId="57" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D25:D34 D17:D20"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D25:D34 D17:D20 D11:F11"/>
     <dataValidation type="list" sqref="E25:E34">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Adding the language name, instead of a TID
Former-commit-id: 06f3dc3f007e546741fd5d9614358b0f918c6b32
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19485"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="166">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -322,9 +322,6 @@
     <t>traditional_chinese</t>
   </si>
   <si>
-    <t>TID_SETTINGS_LANG_NAME</t>
-  </si>
-  <si>
     <t>zh-TW</t>
   </si>
   <si>
@@ -524,6 +521,42 @@
   </si>
   <si>
     <t>TID_SEASON_MIDAUTUMNFESTIVAL_NAME</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Français</t>
+  </si>
+  <si>
+    <t>Italiano</t>
+  </si>
+  <si>
+    <t>Deutsch</t>
+  </si>
+  <si>
+    <t>Español</t>
+  </si>
+  <si>
+    <t>Português</t>
+  </si>
+  <si>
+    <t>Русский</t>
+  </si>
+  <si>
+    <t>简体中文</t>
+  </si>
+  <si>
+    <t>日本語</t>
+  </si>
+  <si>
+    <t>한국어</t>
+  </si>
+  <si>
+    <t>繁體中文</t>
+  </si>
+  <si>
+    <t>Türkçe</t>
   </si>
 </sst>
 </file>
@@ -2512,7 +2545,7 @@
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -2772,16 +2805,16 @@
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" t="s">
         <v>109</v>
-      </c>
-      <c r="F19" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -2789,22 +2822,22 @@
         <v>3</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D20" s="42" t="b">
         <v>0</v>
       </c>
       <c r="E20" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="43" t="s">
         <v>153</v>
-      </c>
-      <c r="F20" s="43" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B22" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -2816,22 +2849,22 @@
     </row>
     <row r="24" spans="2:7" ht="138" x14ac:dyDescent="0.25">
       <c r="B24" s="34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="E24" s="37" t="s">
+      <c r="F24" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="F24" s="37" t="s">
-        <v>123</v>
-      </c>
       <c r="G24" s="38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -2839,19 +2872,19 @@
         <v>3</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D25" s="39">
         <v>3000000</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F25" s="19">
         <v>1</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -2859,13 +2892,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D26" s="39">
         <v>2500000</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F26" s="19">
         <v>5</v>
@@ -2877,19 +2910,19 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D27" s="39">
         <v>2000000</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F27" s="19">
         <v>1</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -2897,13 +2930,13 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D28" s="39">
         <v>1500000</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F28" s="19">
         <v>5</v>
@@ -2915,19 +2948,19 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D29" s="39">
         <v>1000000</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F29" s="19">
         <v>1</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
@@ -2935,13 +2968,13 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D30" s="39">
         <v>500000</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F30" s="19">
         <v>5</v>
@@ -2953,13 +2986,13 @@
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D31" s="39">
         <v>250000</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F31" s="19">
         <v>5</v>
@@ -2971,13 +3004,13 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D32" s="39">
         <v>100000</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F32" s="19">
         <v>1500</v>
@@ -2989,13 +3022,13 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D33" s="39">
         <v>50000</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F33" s="19">
         <v>500</v>
@@ -3007,13 +3040,13 @@
         <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D34" s="39">
         <v>10000</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F34" s="19">
         <v>100</v>
@@ -3049,8 +3082,8 @@
   </sheetPr>
   <dimension ref="B1:L27"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3104,7 +3137,7 @@
         <v>78</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G4" s="26" t="s">
         <v>77</v>
@@ -3119,7 +3152,7 @@
         <v>6</v>
       </c>
       <c r="K4" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L4" s="24" t="s">
         <v>74</v>
@@ -3139,7 +3172,7 @@
         <v>72</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G5" s="18" t="b">
         <v>1</v>
@@ -3154,10 +3187,10 @@
         <v>70</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -3174,7 +3207,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G6" s="18" t="b">
         <v>1</v>
@@ -3189,10 +3222,10 @@
         <v>66</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>87</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -3209,7 +3242,7 @@
         <v>64</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G7" s="18" t="b">
         <v>1</v>
@@ -3224,10 +3257,10 @@
         <v>62</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>87</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -3244,7 +3277,7 @@
         <v>60</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G8" s="18" t="b">
         <v>1</v>
@@ -3259,10 +3292,10 @@
         <v>58</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>87</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -3279,7 +3312,7 @@
         <v>56</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G9" s="18" t="b">
         <v>1</v>
@@ -3294,10 +3327,10 @@
         <v>54</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>87</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -3314,7 +3347,7 @@
         <v>52</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G10" s="18" t="b">
         <v>1</v>
@@ -3329,10 +3362,10 @@
         <v>50</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>87</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -3349,7 +3382,7 @@
         <v>48</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G11" s="18" t="b">
         <v>1</v>
@@ -3364,10 +3397,10 @@
         <v>46</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>87</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -3381,10 +3414,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G12" s="18" t="b">
         <v>0</v>
@@ -3399,10 +3432,10 @@
         <v>43</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -3419,7 +3452,7 @@
         <v>41</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G13" s="18" t="b">
         <v>1</v>
@@ -3434,10 +3467,10 @@
         <v>39</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
@@ -3454,7 +3487,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G14" s="18" t="b">
         <v>1</v>
@@ -3469,10 +3502,10 @@
         <v>35</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>87</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -3486,10 +3519,10 @@
         <v>10</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G15" s="18" t="b">
         <v>1</v>
@@ -3501,13 +3534,13 @@
         <v>86</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -3515,16 +3548,16 @@
         <v>3</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D16" s="19">
         <v>11</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G16" s="18" t="b">
         <v>1</v>
@@ -3533,22 +3566,22 @@
         <v>1</v>
       </c>
       <c r="I16" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="J16" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="K16" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="K16" s="17" t="s">
-        <v>115</v>
-      </c>
       <c r="L16" s="15" t="s">
-        <v>87</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B19" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -3564,23 +3597,23 @@
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="2:10" ht="118.5" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="31" t="s">
         <v>95</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -3588,13 +3621,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -3602,10 +3635,10 @@
         <v>3</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E23" s="18"/>
     </row>
@@ -3614,10 +3647,10 @@
         <v>3</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E24" s="18"/>
     </row>
@@ -3626,10 +3659,10 @@
         <v>3</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="18"/>
     </row>
@@ -3638,10 +3671,10 @@
         <v>3</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E26" s="22"/>
     </row>
@@ -3650,13 +3683,13 @@
         <v>3</v>
       </c>
       <c r="C27" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="E27" s="18" t="s">
         <v>116</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix from previous merge. Added column [goldenFragments]
Former-commit-id: 2ba65596f60c12210fa3a77de76d1de62e564525
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="167">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -557,6 +557,9 @@
   </si>
   <si>
     <t>Türkçe</t>
+  </si>
+  <si>
+    <t>[goldenFragments]</t>
   </si>
 </sst>
 </file>
@@ -943,7 +946,61 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="58">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1438,26 +1495,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2151,16 +2188,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2175,13 +2202,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <autoFilter ref="B4:P5"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="49"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="48"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="53"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="52"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="51"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="50"/>
     <tableColumn id="5" name="[incentivizeFBGem]"/>
     <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
     <tableColumn id="15" name="[maxAdsSkipMissions]"/>
@@ -2199,26 +2226,27 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:F11" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
-  <autoFilter ref="B10:F11"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="43"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="42"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="41"/>
-    <tableColumn id="4" name="[hardCurrency]" dataDxfId="40"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48" tableBorderDxfId="47" totalsRowBorderDxfId="46">
+  <autoFilter ref="B10:G11"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="45"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="44"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="43"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="0"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="42"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F20" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F20" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <autoFilter ref="B16:F20"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="34"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="33"/>
-    <tableColumn id="3" name="[active]" dataDxfId="32"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="36"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="35"/>
+    <tableColumn id="3" name="[active]" dataDxfId="34"/>
     <tableColumn id="4" name="[icon]"/>
     <tableColumn id="5" name="[tidName]"/>
   </tableColumns>
@@ -2227,51 +2255,51 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B24:G34" totalsRowShown="0" headerRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B24:G34" totalsRowShown="0" headerRowDxfId="33">
   <autoFilter ref="B24:G34"/>
   <sortState ref="B25:G34">
     <sortCondition descending="1" ref="D24:D34"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="30"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="28"/>
-    <tableColumn id="4" name="[type]" dataDxfId="27"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="26"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="25"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="30"/>
+    <tableColumn id="4" name="[type]" dataDxfId="29"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="28"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:L16" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:L16" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="B4:L16"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="18"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="17"/>
-    <tableColumn id="3" name="[order]" dataDxfId="16"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="15"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="14"/>
-    <tableColumn id="11" name="[android]" dataDxfId="13"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="12"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="11"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="10"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="9"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="8"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="22"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="21"/>
+    <tableColumn id="3" name="[order]" dataDxfId="20"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="19"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="18"/>
+    <tableColumn id="11" name="[android]" dataDxfId="17"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="16"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="15"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="14"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="13"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="3"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="1"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="0"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="7"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="6"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="5"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2545,8 +2573,8 @@
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2713,7 +2741,10 @@
       <c r="E10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2730,7 +2761,10 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3054,11 +3088,11 @@
       <c r="G34" s="19"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="56" priority="1"/>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11 D25:D34 D17:D20"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D25:D34 D17:D20 D11:F11"/>
     <dataValidation type="list" sqref="E25:E34">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
@@ -3083,7 +3117,7 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3694,10 +3728,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="23" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
Content - Add value for golden frag given
Former-commit-id: d57e9377e02a6a20da48febd3cfb8517747a2eb0
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19485"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="168">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -560,6 +560,9 @@
   </si>
   <si>
     <t>[goldenFragments]</t>
+  </si>
+  <si>
+    <t>[goldenFragmentsGivenTutorial]</t>
   </si>
 </sst>
 </file>
@@ -951,60 +954,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1495,6 +1444,26 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1902,6 +1871,30 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -2188,6 +2181,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2202,13 +2205,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
-  <autoFilter ref="B4:P5"/>
-  <tableColumns count="15">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="53"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="52"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="51"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+  <autoFilter ref="B4:Q5"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="52"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="51"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="50"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="49"/>
     <tableColumn id="5" name="[incentivizeFBGem]"/>
     <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
     <tableColumn id="15" name="[maxAdsSkipMissions]"/>
@@ -2220,33 +2223,34 @@
     <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]"/>
     <tableColumn id="12" name="[flyingPigsProbaCoefA]"/>
     <tableColumn id="13" name="[flyingPigsProbaCoefB]"/>
+    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48" tableBorderDxfId="47" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="45"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="44"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="43"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="0"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="42"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="41"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="44"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="43"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="42"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="41"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="40"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F20" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F20" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="B16:F20"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="36"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="35"/>
-    <tableColumn id="3" name="[active]" dataDxfId="34"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="34"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="33"/>
+    <tableColumn id="3" name="[active]" dataDxfId="32"/>
     <tableColumn id="4" name="[icon]"/>
     <tableColumn id="5" name="[tidName]"/>
   </tableColumns>
@@ -2255,51 +2259,51 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B24:G34" totalsRowShown="0" headerRowDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B24:G34" totalsRowShown="0" headerRowDxfId="31">
   <autoFilter ref="B24:G34"/>
   <sortState ref="B25:G34">
     <sortCondition descending="1" ref="D24:D34"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="30"/>
-    <tableColumn id="4" name="[type]" dataDxfId="29"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="28"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="27"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="30"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="28"/>
+    <tableColumn id="4" name="[type]" dataDxfId="27"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="26"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:L16" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:L16" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="B4:L16"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="22"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="21"/>
-    <tableColumn id="3" name="[order]" dataDxfId="20"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="19"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="18"/>
-    <tableColumn id="11" name="[android]" dataDxfId="17"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="16"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="15"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="14"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="13"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="12"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="18"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="17"/>
+    <tableColumn id="3" name="[order]" dataDxfId="16"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="15"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="14"/>
+    <tableColumn id="11" name="[android]" dataDxfId="13"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="12"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="11"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="10"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="9"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="7"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="6"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="5"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="4"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="3"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="1"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2571,10 +2575,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2589,8 +2593,8 @@
     <col min="8" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
@@ -2604,7 +2608,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="14"/>
       <c r="C3" s="13"/>
@@ -2619,7 +2623,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:16" ht="306" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="306" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -2665,8 +2669,11 @@
       <c r="P4" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2712,9 +2719,12 @@
       <c r="P5">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="Q5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -2728,7 +2738,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="10" spans="1:16" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -2748,7 +2758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2768,8 +2778,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
@@ -2783,7 +2793,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="16" spans="1:16" ht="104.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="104.25" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -3089,7 +3099,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D25:D34 D17:D20 D11:F11"/>
@@ -3116,8 +3126,8 @@
   </sheetPr>
   <dimension ref="B1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3728,10 +3738,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
Added 3 new seasons
Former-commit-id: e3e8f5159e5a3aac720de3482559cd95b1252baf
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="171">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -563,6 +563,15 @@
   </si>
   <si>
     <t>[goldenFragmentsGivenTutorial]</t>
+  </si>
+  <si>
+    <t>theKidWhoWouldBeKing</t>
+  </si>
+  <si>
+    <t>chineseNewYear</t>
+  </si>
+  <si>
+    <t>sanValentin</t>
   </si>
 </sst>
 </file>
@@ -862,7 +871,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -945,11 +954,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="58">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1444,26 +1484,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2181,16 +2201,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2205,13 +2215,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <autoFilter ref="B4:Q5"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="52"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="51"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="50"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="49"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="53"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="52"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="51"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="50"/>
     <tableColumn id="5" name="[incentivizeFBGem]"/>
     <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
     <tableColumn id="15" name="[maxAdsSkipMissions]"/>
@@ -2230,27 +2240,27 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48" tableBorderDxfId="47" totalsRowBorderDxfId="46">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="44"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="43"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="42"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="41"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="40"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="39"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="45"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="44"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="43"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="42"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="41"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F20" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
-  <autoFilter ref="B16:F20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F23" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="B16:F23"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="34"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="33"/>
-    <tableColumn id="3" name="[active]" dataDxfId="32"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="35"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="34"/>
+    <tableColumn id="3" name="[active]" dataDxfId="33"/>
     <tableColumn id="4" name="[icon]"/>
     <tableColumn id="5" name="[tidName]"/>
   </tableColumns>
@@ -2259,51 +2269,51 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B24:G34" totalsRowShown="0" headerRowDxfId="31">
-  <autoFilter ref="B24:G34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B27:G37" totalsRowShown="0" headerRowDxfId="32">
+  <autoFilter ref="B27:G37"/>
   <sortState ref="B25:G34">
     <sortCondition descending="1" ref="D24:D34"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="30"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="28"/>
-    <tableColumn id="4" name="[type]" dataDxfId="27"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="26"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="25"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="31"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="30"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="29"/>
+    <tableColumn id="4" name="[type]" dataDxfId="28"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="27"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:L16" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:L16" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="B4:L16"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="18"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="17"/>
-    <tableColumn id="3" name="[order]" dataDxfId="16"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="15"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="14"/>
-    <tableColumn id="11" name="[android]" dataDxfId="13"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="12"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="11"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="10"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="9"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="8"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="21"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="20"/>
+    <tableColumn id="3" name="[order]" dataDxfId="19"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="18"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="17"/>
+    <tableColumn id="11" name="[android]" dataDxfId="16"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="15"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="14"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="13"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="12"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="3"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="1"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="0"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="6"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="4"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2575,17 +2585,17 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
@@ -2878,95 +2888,76 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B22" s="7" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+    </row>
+    <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B25" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" t="s">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="138" x14ac:dyDescent="0.25">
-      <c r="B24" s="34" t="s">
+    <row r="27" spans="2:7" ht="138" x14ac:dyDescent="0.25">
+      <c r="B27" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C27" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D27" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="E24" s="37" t="s">
+      <c r="E27" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="37" t="s">
+      <c r="F27" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="38" t="s">
+      <c r="G27" s="38" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D25" s="39">
-        <v>3000000</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="F25" s="19">
-        <v>1</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D26" s="39">
-        <v>2500000</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="F26" s="19">
-        <v>5</v>
-      </c>
-      <c r="G26" s="19"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D27" s="39">
-        <v>2000000</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F27" s="19">
-        <v>1</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -2974,66 +2965,68 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D28" s="39">
-        <v>1500000</v>
+        <v>3000000</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F28" s="19">
-        <v>5</v>
-      </c>
-      <c r="G28" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D29" s="39">
-        <v>1000000</v>
+        <v>2500000</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F29" s="19">
-        <v>1</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>139</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D30" s="39">
-        <v>500000</v>
+        <v>2000000</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F30" s="19">
-        <v>5</v>
-      </c>
-      <c r="G30" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D31" s="39">
-        <v>250000</v>
+        <v>1500000</v>
       </c>
       <c r="E31" s="19" t="s">
         <v>134</v>
@@ -3048,34 +3041,36 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D32" s="39">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="F32" s="19">
-        <v>1500</v>
-      </c>
-      <c r="G32" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D33" s="39">
-        <v>50000</v>
+        <v>500000</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="F33" s="19">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="G33" s="19"/>
     </row>
@@ -3084,26 +3079,80 @@
         <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="39">
+        <v>250000</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="19">
+        <v>5</v>
+      </c>
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="39">
+        <v>100000</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" s="19">
+        <v>1500</v>
+      </c>
+      <c r="G35" s="19"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="39">
+        <v>50000</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F36" s="19">
+        <v>500</v>
+      </c>
+      <c r="G36" s="19"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="39">
+      <c r="D37" s="39">
         <v>10000</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E37" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F37" s="19">
         <v>100</v>
       </c>
-      <c r="G34" s="19"/>
+      <c r="G37" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="57" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D25:D34 D17:D20 D11:F11"/>
-    <dataValidation type="list" sqref="E25:E34">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D28:D37 D17:D23 D11:F11"/>
+    <dataValidation type="list" sqref="E28:E37">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3738,10 +3787,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="23" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
adding tids and icons
Former-commit-id: 1c3d0487b4da83b65ebd408eda77f0565300c9e2
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="176">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -571,7 +571,22 @@
     <t>chineseNewYear</t>
   </si>
   <si>
-    <t>sanValentin</t>
+    <t>valentine</t>
+  </si>
+  <si>
+    <t>TID_SEASON_TKWWBK_NAME</t>
+  </si>
+  <si>
+    <t>TID_SEASON_CHINESENEWYEAR</t>
+  </si>
+  <si>
+    <t>TID_SEASON_VALENTINE</t>
+  </si>
+  <si>
+    <t>icon_season_chineseNewYear</t>
+  </si>
+  <si>
+    <t>icon_season_valentine</t>
   </si>
 </sst>
 </file>
@@ -961,36 +976,6 @@
   </cellStyles>
   <dxfs count="58">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1484,6 +1469,26 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2201,6 +2206,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2215,13 +2230,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
   <autoFilter ref="B4:Q5"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="53"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="52"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="51"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="50"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="52"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="51"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="50"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="49"/>
     <tableColumn id="5" name="[incentivizeFBGem]"/>
     <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
     <tableColumn id="15" name="[maxAdsSkipMissions]"/>
@@ -2240,27 +2255,27 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48" tableBorderDxfId="47" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="45"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="44"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="43"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="42"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="41"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="40"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="44"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="43"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="42"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="41"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="40"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F23" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F23" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="B16:F23"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="35"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="34"/>
-    <tableColumn id="3" name="[active]" dataDxfId="33"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="34"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="33"/>
+    <tableColumn id="3" name="[active]" dataDxfId="32"/>
     <tableColumn id="4" name="[icon]"/>
     <tableColumn id="5" name="[tidName]"/>
   </tableColumns>
@@ -2269,51 +2284,51 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B27:G37" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B27:G37" totalsRowShown="0" headerRowDxfId="31">
   <autoFilter ref="B27:G37"/>
   <sortState ref="B25:G34">
     <sortCondition descending="1" ref="D24:D34"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="31"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="30"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="29"/>
-    <tableColumn id="4" name="[type]" dataDxfId="28"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="27"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="26"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="30"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="28"/>
+    <tableColumn id="4" name="[type]" dataDxfId="27"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="26"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:L16" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:L16" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="B4:L16"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="21"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="20"/>
-    <tableColumn id="3" name="[order]" dataDxfId="19"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="18"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="17"/>
-    <tableColumn id="11" name="[android]" dataDxfId="16"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="15"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="14"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="13"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="12"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="11"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="18"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="17"/>
+    <tableColumn id="3" name="[order]" dataDxfId="16"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="15"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="14"/>
+    <tableColumn id="11" name="[android]" dataDxfId="13"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="12"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="11"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="10"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="9"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="6"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="4"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="3"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="3"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="1"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2588,7 +2603,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2899,7 +2914,9 @@
         <v>0</v>
       </c>
       <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="F21" s="43" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="32" t="s">
@@ -2911,8 +2928,12 @@
       <c r="D22" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
+      <c r="E22" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="40" t="s">
@@ -2924,8 +2945,12 @@
       <c r="D23" s="42" t="b">
         <v>0</v>
       </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
+      <c r="E23" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -3148,7 +3173,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D28:D37 D17:D23 D11:F11"/>
@@ -3787,10 +3812,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
There was a mistake in TID's nomenclature
Former-commit-id: 0c767eef0bd5a9c0fca0ef84c40797ba3d658455
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -577,16 +577,16 @@
     <t>TID_SEASON_TKWWBK_NAME</t>
   </si>
   <si>
-    <t>TID_SEASON_CHINESENEWYEAR</t>
-  </si>
-  <si>
-    <t>TID_SEASON_VALENTINE</t>
-  </si>
-  <si>
     <t>icon_season_chineseNewYear</t>
   </si>
   <si>
     <t>icon_season_valentine</t>
+  </si>
+  <si>
+    <t>TID_SEASON_CHINESENEWYEAR_NAME</t>
+  </si>
+  <si>
+    <t>TID_SEASON_VALENTINE_NAME</t>
   </si>
 </sst>
 </file>
@@ -2603,7 +2603,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2929,10 +2929,10 @@
         <v>0</v>
       </c>
       <c r="E22" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="F22" s="43" t="s">
         <v>174</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -2946,10 +2946,10 @@
         <v>0</v>
       </c>
       <c r="E23" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="F23" s="43" t="s">
         <v>175</v>
-      </c>
-      <c r="F23" s="43" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fixes because we had conflict with branch 1.19
Former-commit-id: c0ca6e115677f0a1dd12aa411aa226d11b1f5677
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -15,7 +15,7 @@
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="177">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -565,18 +565,12 @@
     <t>[goldenFragmentsGivenTutorial]</t>
   </si>
   <si>
-    <t>theKidWhoWouldBeKing</t>
-  </si>
-  <si>
     <t>chineseNewYear</t>
   </si>
   <si>
     <t>valentine</t>
   </si>
   <si>
-    <t>TID_SEASON_TKWWBK_NAME</t>
-  </si>
-  <si>
     <t>icon_season_chineseNewYear</t>
   </si>
   <si>
@@ -587,6 +581,15 @@
   </si>
   <si>
     <t>TID_SEASON_VALENTINE_NAME</t>
+  </si>
+  <si>
+    <t>movie_kwwbk</t>
+  </si>
+  <si>
+    <t>icon_season_movie_kwwbk</t>
+  </si>
+  <si>
+    <t>TID_SEASON_MOVIE_KWWBK_NAME</t>
   </si>
 </sst>
 </file>
@@ -886,7 +889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -970,6 +973,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2603,7 +2607,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2904,18 +2908,20 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="44" t="s">
-        <v>168</v>
-      </c>
-      <c r="D21" s="1" t="b">
+      <c r="C21" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="D21" s="42" t="b">
         <v>0</v>
       </c>
-      <c r="E21" s="43"/>
+      <c r="E21" s="43" t="s">
+        <v>175</v>
+      </c>
       <c r="F21" s="43" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -2923,16 +2929,16 @@
         <v>3</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D22" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E22" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" s="43" t="s">
         <v>172</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -2940,16 +2946,16 @@
         <v>3</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D23" s="42" t="b">
         <v>0</v>
       </c>
       <c r="E23" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="F23" s="43" t="s">
         <v>173</v>
-      </c>
-      <c r="F23" s="43" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3176,7 +3182,7 @@
     <cfRule type="duplicateValues" dxfId="57" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D28:D37 D17:D23 D11:F11"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D28:D37 D11:F11 D17:D23"/>
     <dataValidation type="list" sqref="E28:E37">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Maximum mission ads to watch increased from 10 to 100
Former-commit-id: 052b7e2f741449cb43b00a87a749b1e21eb6fe65
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="38175" windowHeight="19485"/>
+    <workbookView xWindow="0" yWindow="432" windowWidth="38172" windowHeight="19488"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -2606,24 +2606,24 @@
   </sheetPr>
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
     <col min="8" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:17" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
@@ -2637,7 +2637,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="14"/>
       <c r="C3" s="13"/>
@@ -2652,7 +2652,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:17" ht="306" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="292.2" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>15</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2752,8 +2752,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:17" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -2767,7 +2767,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="10" spans="1:17" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="91.8" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2807,8 +2807,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:17" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
@@ -2822,7 +2822,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="16" spans="1:17" ht="104.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="98.4" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="32" t="s">
         <v>3</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="40" t="s">
         <v>3</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="45" t="s">
         <v>3</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="32" t="s">
         <v>3</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="40" t="s">
         <v>3</v>
       </c>
@@ -2958,8 +2958,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B25" s="7" t="s">
         <v>117</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="138" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="130.80000000000001" x14ac:dyDescent="0.3">
       <c r="B27" s="34" t="s">
         <v>118</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>3</v>
       </c>
@@ -3029,7 +3029,7 @@
       </c>
       <c r="G29" s="19"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>3</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>3</v>
       </c>
@@ -3067,7 +3067,7 @@
       </c>
       <c r="G31" s="19"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>3</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>3</v>
       </c>
@@ -3105,7 +3105,7 @@
       </c>
       <c r="G33" s="19"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>3</v>
       </c>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="G34" s="19"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>3</v>
       </c>
@@ -3141,7 +3141,7 @@
       </c>
       <c r="G35" s="19"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>3</v>
       </c>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="G36" s="19"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>3</v>
       </c>
@@ -3210,21 +3210,21 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" customWidth="1"/>
-    <col min="6" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" customWidth="1"/>
+    <col min="6" max="7" width="10.88671875" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B2" s="7" t="s">
         <v>82</v>
       </c>
@@ -3237,7 +3237,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="28"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -3247,7 +3247,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="119.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="113.4" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>80</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>3</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>3</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>3</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
         <v>3</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
         <v>3</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
         <v>3</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
         <v>3</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
@@ -3702,8 +3702,8 @@
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B19" s="7" t="s">
         <v>100</v>
       </c>
@@ -3716,7 +3716,7 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B20" s="28"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -3726,7 +3726,7 @@
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:10" ht="118.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="112.2" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>101</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
         <v>3</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
         <v>3</v>
       </c>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="23" t="s">
         <v>3</v>
       </c>
@@ -3778,7 +3778,7 @@
       </c>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
         <v>3</v>
       </c>
@@ -3790,7 +3790,7 @@
       </c>
       <c r="E25" s="18"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
         <v>3</v>
       </c>
@@ -3802,7 +3802,7 @@
       </c>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="23" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
New content table: shareLocationDefinitions
Former-commit-id: 87576c9165433b7d7cf61503f35bd85d67ba8a60
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="231">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -620,6 +620,138 @@
   </si>
   <si>
     <t>logo</t>
+  </si>
+  <si>
+    <t>SHARES</t>
+  </si>
+  <si>
+    <t>{shareLocationDefinitions}</t>
+  </si>
+  <si>
+    <t>[prefab]</t>
+  </si>
+  <si>
+    <t>[url]</t>
+  </si>
+  <si>
+    <t>[urlChina]</t>
+  </si>
+  <si>
+    <t>[tidPrewrittenCaption]</t>
+  </si>
+  <si>
+    <t>[tidCallToAction]</t>
+  </si>
+  <si>
+    <t>dragon</t>
+  </si>
+  <si>
+    <t>dragon_acquired</t>
+  </si>
+  <si>
+    <t>skin</t>
+  </si>
+  <si>
+    <t>skin_acquired</t>
+  </si>
+  <si>
+    <t>pet_acquired</t>
+  </si>
+  <si>
+    <t>high_score</t>
+  </si>
+  <si>
+    <t>quest</t>
+  </si>
+  <si>
+    <t>tournament_leaderboard_menu</t>
+  </si>
+  <si>
+    <t>tournament_leaderboard_results</t>
+  </si>
+  <si>
+    <t>tournament_leaderboard_rewards</t>
+  </si>
+  <si>
+    <t>league_leaderboard_menu</t>
+  </si>
+  <si>
+    <t>league_leaderboard_results</t>
+  </si>
+  <si>
+    <t>league_finish_no_change</t>
+  </si>
+  <si>
+    <t>league_finish_promotion</t>
+  </si>
+  <si>
+    <t>PF_DragonShareScreen</t>
+  </si>
+  <si>
+    <t>PF_PetShareScreen</t>
+  </si>
+  <si>
+    <t>PF_ScoreShareScreen</t>
+  </si>
+  <si>
+    <t>PF_QuestShareScreen</t>
+  </si>
+  <si>
+    <t>http://bit.ly/HDsocialsharing</t>
+  </si>
+  <si>
+    <t>https://go.onelink.me/l23a/share</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_PREWRITTEN_SENTENCE_OWNED_DRAGON</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_PREWRITTEN_SENTENCE_NEW_DRAGON</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_PREWRITTEN_SENTENCE_NEW_SKIN</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_PREWRITTEN_SENTENCE_NEW_PET</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_PREWRITTEN_SENTENCE_NEW_HIGH_SCORE</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_PREWRITTEN_SENTENCE_COLLAB_QUEST</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_PREWRITTEN_SENTENCE_TOURNAMENT_LEADERBOARD_</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_PREWRITTEN_SENTENCE_LEAGUE_LEADERBOARD_02</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_PREWRITTEN_SENTENCE_LEAGUE_LEADERBOARD_01</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_CALL_TO_ACTION_OWNED_DRAGON</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_CALL_TO_ACTION_NEW_DRAGON</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_CALL_TO_ACTION_NEW_SKIN</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_CALL_TO_ACTION_NEW_PET</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_CALL_TO_ACTION_NEW_HIGH_SCORE</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_CALL_TO_ACTION_COLLAB_QUEST</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_CALL_TO_ACTION_TOURNAMENT_LEADERBOARD</t>
+  </si>
+  <si>
+    <t>TID_REFERRAL_CALL_TO_ACTION_LEAGUE_LEADERBOARD</t>
   </si>
 </sst>
 </file>
@@ -1008,31 +1140,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="76">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1062,6 +1170,92 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1191,6 +1385,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1200,13 +1401,6 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -1226,11 +1420,20 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -1254,177 +1457,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -1559,114 +1592,246 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
           <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1685,6 +1850,251 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2274,6 +2684,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2288,13 +2708,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="58" headerRowBorderDxfId="57" tableBorderDxfId="56" totalsRowBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="74" headerRowBorderDxfId="73" tableBorderDxfId="72" totalsRowBorderDxfId="71">
   <autoFilter ref="B4:Q5"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="54"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="53"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="52"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="51"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="70"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="69"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="68"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="67"/>
     <tableColumn id="5" name="[incentivizeFBGem]"/>
     <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
     <tableColumn id="15" name="[maxAdsSkipMissions]"/>
@@ -2313,27 +2733,27 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="50" headerRowBorderDxfId="49" tableBorderDxfId="48" totalsRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64" totalsRowBorderDxfId="63">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="46"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="45"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="44"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="43"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="42"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="41"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="62"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="61"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="60"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="59"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="58"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F23" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F23" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
   <autoFilter ref="B16:F23"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="36"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="35"/>
-    <tableColumn id="3" name="[active]" dataDxfId="34"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="52"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="51"/>
+    <tableColumn id="3" name="[active]" dataDxfId="50"/>
     <tableColumn id="4" name="[icon]"/>
     <tableColumn id="5" name="[tidName]"/>
   </tableColumns>
@@ -2342,52 +2762,68 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B29:G39" totalsRowShown="0" headerRowDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B29:G39" totalsRowShown="0" headerRowDxfId="49">
   <autoFilter ref="B29:G39"/>
   <sortState ref="B25:G34">
     <sortCondition descending="1" ref="D24:D34"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="30"/>
-    <tableColumn id="4" name="[type]" dataDxfId="29"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="28"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="27"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="46"/>
+    <tableColumn id="4" name="[type]" dataDxfId="45"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="44"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="22"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="21"/>
-    <tableColumn id="3" name="[order]" dataDxfId="20"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="19"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="18"/>
-    <tableColumn id="11" name="[android]" dataDxfId="17"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="16"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="15"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="14"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="0"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="13"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="12"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="36"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="35"/>
+    <tableColumn id="3" name="[order]" dataDxfId="34"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="33"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="32"/>
+    <tableColumn id="11" name="[android]" dataDxfId="31"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="30"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="29"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="28"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="27"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="26"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="7"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="6"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="5"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="4"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="20"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="19"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="18"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H48" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+  <autoFilter ref="B34:H48"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="11"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="10"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="9"/>
+    <tableColumn id="2" name="[url]" dataDxfId="8"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="7"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="6"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3268,7 +3704,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D30:D39 D11:F11 D17:D25"/>
@@ -3293,19 +3729,21 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="B1:M27"/>
+  <dimension ref="B1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="101" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="101" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="32.140625" customWidth="1"/>
-    <col min="6" max="7" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="67.42578125" customWidth="1"/>
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
@@ -3944,12 +4382,383 @@
         <v>116</v>
       </c>
     </row>
+    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B32" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="34" spans="2:8" ht="129.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="F34" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="G34" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="H34" s="31" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="G35" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="H35" s="30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41:C46">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C40">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">
@@ -3958,13 +4767,14 @@
     <dataValidation type="list" allowBlank="1" sqref="L5:L16">
       <formula1>$C$22:$C$27</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E22:E27 D22:D26"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E22:E27 D22:D26 E35:E48 C35:D39"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed xml, info from presummer disapeared
Former-commit-id: 93645dfbd6d755d17be5477c63d5fce5ac983019
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="200">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -620,6 +620,45 @@
   </si>
   <si>
     <t>logo</t>
+  </si>
+  <si>
+    <t>ufoDay</t>
+  </si>
+  <si>
+    <t>icon_season_UFO_Day</t>
+  </si>
+  <si>
+    <t>TID_SEASON_UFO_DAY_NAME</t>
+  </si>
+  <si>
+    <t>preSummerDay</t>
+  </si>
+  <si>
+    <t>icon_season_PreSummer_Day</t>
+  </si>
+  <si>
+    <t>TID_SEASON_PreSummer_DAY_NAME</t>
+  </si>
+  <si>
+    <t>football</t>
+  </si>
+  <si>
+    <t>summer_1</t>
+  </si>
+  <si>
+    <t>icon_season_summer1</t>
+  </si>
+  <si>
+    <t>TID_SEASON_summer_1_NAME</t>
+  </si>
+  <si>
+    <t>summer_2</t>
+  </si>
+  <si>
+    <t>icon_season_summer2</t>
+  </si>
+  <si>
+    <t>TID_SEASON_summer_2_NAME</t>
   </si>
 </sst>
 </file>
@@ -1010,30 +1049,6 @@
   </cellStyles>
   <dxfs count="59">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1231,6 +1246,30 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -2342,8 +2381,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B29:G39" totalsRowShown="0" headerRowDxfId="33">
-  <autoFilter ref="B29:G39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B34:G44" totalsRowShown="0" headerRowDxfId="33">
+  <autoFilter ref="B34:G44"/>
   <sortState ref="B25:G34">
     <sortCondition descending="1" ref="D24:D34"/>
   </sortState>
@@ -2372,22 +2411,22 @@
     <tableColumn id="12" name="[iOS]" dataDxfId="16"/>
     <tableColumn id="5" name="[txtFilename]" dataDxfId="15"/>
     <tableColumn id="2" name="[icon]" dataDxfId="14"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="0"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="13"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="12"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="13"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="12"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="7"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="6"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="5"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="4"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="6"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="4"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2659,10 +2698,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3047,133 +3086,122 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B27" s="7" t="s">
+    <row r="26" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="D26" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>193</v>
+      </c>
+      <c r="D27" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="F28" s="43" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="D29" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="F29" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="F30" s="43" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" t="s">
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="138" x14ac:dyDescent="0.25">
-      <c r="B29" s="34" t="s">
+    <row r="34" spans="2:7" ht="138" x14ac:dyDescent="0.25">
+      <c r="B34" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C34" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D34" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="E29" s="37" t="s">
+      <c r="E34" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="F29" s="37" t="s">
+      <c r="F34" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="G29" s="38" t="s">
+      <c r="G34" s="38" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D30" s="39">
-        <v>3000000</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="F30" s="19">
-        <v>1</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D31" s="39">
-        <v>2500000</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" s="19">
-        <v>5</v>
-      </c>
-      <c r="G31" s="19"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D32" s="39">
-        <v>2000000</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F32" s="19">
-        <v>1</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D33" s="39">
-        <v>1500000</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="F33" s="19">
-        <v>5</v>
-      </c>
-      <c r="G33" s="19"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D34" s="39">
-        <v>1000000</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F34" s="19">
-        <v>1</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
@@ -3181,31 +3209,33 @@
         <v>3</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D35" s="39">
-        <v>500000</v>
+        <v>3000000</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F35" s="19">
-        <v>5</v>
-      </c>
-      <c r="G35" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D36" s="39">
-        <v>250000</v>
+        <v>2500000</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F36" s="19">
         <v>5</v>
@@ -3217,34 +3247,36 @@
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D37" s="39">
-        <v>100000</v>
+        <v>2000000</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="F37" s="19">
-        <v>1500</v>
-      </c>
-      <c r="G37" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D38" s="39">
-        <v>50000</v>
+        <v>1500000</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="F38" s="19">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="G38" s="19"/>
     </row>
@@ -3253,37 +3285,129 @@
         <v>3</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" s="39">
+        <v>1000000</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" s="19">
+        <v>1</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="39">
+        <v>500000</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" s="19">
+        <v>5</v>
+      </c>
+      <c r="G40" s="19"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" s="39">
+        <v>250000</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" s="19">
+        <v>5</v>
+      </c>
+      <c r="G41" s="19"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" s="39">
+        <v>100000</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F42" s="19">
+        <v>1500</v>
+      </c>
+      <c r="G42" s="19"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" s="39">
+        <v>50000</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" s="19">
+        <v>500</v>
+      </c>
+      <c r="G43" s="19"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="39">
+      <c r="D44" s="39">
         <v>10000</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E44" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F39" s="19">
+      <c r="F44" s="19">
         <v>100</v>
       </c>
-      <c r="G39" s="19"/>
+      <c r="G44" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D30:D39 D11:F11 D17:D25"/>
-    <dataValidation type="list" sqref="E30:E39">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D35:D44 D11:F11 D17:D30"/>
+    <dataValidation type="list" sqref="E35:E44">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="4">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3295,7 +3419,7 @@
   </sheetPr>
   <dimension ref="B1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="101" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="101" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -3946,10 +4070,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
clean summer seasons content and sp
Former-commit-id: a5c874beecff651d6f6d72dc5a59d6d965bb9d0e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="197">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -643,22 +643,13 @@
     <t>football</t>
   </si>
   <si>
-    <t>summer_1</t>
-  </si>
-  <si>
-    <t>icon_season_summer1</t>
-  </si>
-  <si>
-    <t>TID_SEASON_summer_1_NAME</t>
-  </si>
-  <si>
-    <t>summer_2</t>
-  </si>
-  <si>
-    <t>icon_season_summer2</t>
-  </si>
-  <si>
-    <t>TID_SEASON_summer_2_NAME</t>
+    <t>summer</t>
+  </si>
+  <si>
+    <t>icon_season_summer</t>
+  </si>
+  <si>
+    <t>TID_SEASON_summer_NAME</t>
   </si>
 </sst>
 </file>
@@ -2723,7 +2714,7 @@
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,21 +3168,11 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>197</v>
-      </c>
-      <c r="D30" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="43" t="s">
-        <v>198</v>
-      </c>
-      <c r="F30" s="43" t="s">
-        <v>199</v>
-      </c>
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
     </row>
     <row r="31" spans="2:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
change summer pets HIDDEN to FALSE Change fottball icon name
Former-commit-id: e3abd73752438ea92152860c79dd14ab0f1c79d3
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="245">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -788,6 +788,12 @@
   </si>
   <si>
     <t>dragon_ar</t>
+  </si>
+  <si>
+    <t>icon_season_football</t>
+  </si>
+  <si>
+    <t>TID_SEASON_football_NAME</t>
   </si>
 </sst>
 </file>
@@ -1200,16 +1206,6 @@
   </cellStyles>
   <dxfs count="77">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1955,6 +1951,16 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2848,50 +2854,50 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="31"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="30"/>
-    <tableColumn id="3" name="[order]" dataDxfId="29"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="28"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="27"/>
-    <tableColumn id="11" name="[android]" dataDxfId="26"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="25"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="24"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="23"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="22"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="20"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" name="[order]" dataDxfId="28"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
+    <tableColumn id="11" name="[android]" dataDxfId="25"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="15"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="13"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="12"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="7"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="6"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="5"/>
-    <tableColumn id="2" name="[url]" dataDxfId="4"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="3"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="1"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
+    <tableColumn id="2" name="[url]" dataDxfId="3"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3165,8 +3171,8 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3579,10 +3585,10 @@
         <v>0</v>
       </c>
       <c r="E27" s="46" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="F27" s="46" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -3849,13 +3855,13 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="4">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3867,7 +3873,7 @@
   </sheetPr>
   <dimension ref="B1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="101" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="101" workbookViewId="0">
       <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
@@ -4949,7 +4955,7 @@
     <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
Fixing TID's names. Some of them in lowercase. TID's names should be, ALWAYS, in UPPERCASE
Former-commit-id: 336974a0eb939846e324b515fe3788783b00d213
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -772,9 +772,6 @@
     <t>icon_season_PreSummer_Day</t>
   </si>
   <si>
-    <t>TID_SEASON_PreSummer_DAY_NAME</t>
-  </si>
-  <si>
     <t>preSummerDay</t>
   </si>
   <si>
@@ -784,16 +781,19 @@
     <t>icon_season_summer</t>
   </si>
   <si>
-    <t>TID_SEASON_summer_NAME</t>
-  </si>
-  <si>
     <t>dragon_ar</t>
   </si>
   <si>
     <t>icon_season_football</t>
   </si>
   <si>
-    <t>TID_SEASON_football_NAME</t>
+    <t>TID_SEASON_FOOTBALL_NAME</t>
+  </si>
+  <si>
+    <t>TID_SEASON_PRESUMMER_DAY_NAME</t>
+  </si>
+  <si>
+    <t>TID_SEASON_SUMMER_NAME</t>
   </si>
 </sst>
 </file>
@@ -3171,8 +3171,8 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3585,10 +3585,10 @@
         <v>0</v>
       </c>
       <c r="E27" s="46" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F27" s="46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -3596,7 +3596,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D28" s="42" t="b">
         <v>0</v>
@@ -3605,7 +3605,7 @@
         <v>236</v>
       </c>
       <c r="F28" s="43" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -3613,16 +3613,16 @@
         <v>3</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D29" s="42" t="b">
         <v>0</v>
       </c>
       <c r="E29" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F29" s="46" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4911,7 +4911,7 @@
         <v>3</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D50" s="18" t="s">
         <v>208</v>

</xml_diff>

<commit_message>
Fixes some missing prefabs
Former-commit-id: 4aa568a25455a08ad95271481ce3cdd9da544f72
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="248">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -794,6 +794,15 @@
   </si>
   <si>
     <t>TID_SEASON_SUMMER_NAME</t>
+  </si>
+  <si>
+    <t>PF_TournamentShareScreen</t>
+  </si>
+  <si>
+    <t>PF_LeagueLeaderboardShareScreen</t>
+  </si>
+  <si>
+    <t>PF_LeagueFinishShareScreen</t>
   </si>
 </sst>
 </file>
@@ -3171,7 +3180,7 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -3873,8 +3882,8 @@
   </sheetPr>
   <dimension ref="B1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="101" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4730,7 +4739,7 @@
         <v>201</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>201</v>
+        <v>245</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>212</v>
@@ -4753,7 +4762,7 @@
         <v>202</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>202</v>
+        <v>245</v>
       </c>
       <c r="E43" s="18" t="s">
         <v>212</v>
@@ -4776,7 +4785,7 @@
         <v>203</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="E44" s="18" t="s">
         <v>212</v>
@@ -4799,7 +4808,7 @@
         <v>204</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>204</v>
+        <v>246</v>
       </c>
       <c r="E45" s="18" t="s">
         <v>212</v>
@@ -4822,7 +4831,7 @@
         <v>205</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>205</v>
+        <v>246</v>
       </c>
       <c r="E46" s="18" t="s">
         <v>212</v>
@@ -4845,7 +4854,7 @@
         <v>206</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>206</v>
+        <v>247</v>
       </c>
       <c r="E47" s="18" t="s">
         <v>212</v>
@@ -4868,7 +4877,7 @@
         <v>207</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>207</v>
+        <v>247</v>
       </c>
       <c r="E48" s="18" t="s">
         <v>212</v>

</xml_diff>

<commit_message>
deleted tkhwbk movie seasonal and for content
Former-commit-id: f21f71b5218a3d5d48573e012900a8a3010070b5
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="245">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -581,15 +581,6 @@
   </si>
   <si>
     <t>TID_SEASON_VALENTINE_NAME</t>
-  </si>
-  <si>
-    <t>movie_kwwbk</t>
-  </si>
-  <si>
-    <t>icon_season_movie_kwwbk</t>
-  </si>
-  <si>
-    <t>TID_SEASON_MOVIE_KWWBK_NAME</t>
   </si>
   <si>
     <t>patricks</t>
@@ -1215,6 +1206,106 @@
   </cellStyles>
   <dxfs count="77">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1962,96 +2053,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2767,16 +2768,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2791,13 +2782,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="75" headerRowBorderDxfId="74" tableBorderDxfId="73" totalsRowBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="76" headerRowBorderDxfId="75" tableBorderDxfId="74" totalsRowBorderDxfId="73">
   <autoFilter ref="B4:Q5"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="71"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="70"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="69"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="68"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="72"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="71"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="70"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="69"/>
     <tableColumn id="5" name="[incentivizeFBGem]"/>
     <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
     <tableColumn id="15" name="[maxAdsSkipMissions]"/>
@@ -2816,27 +2807,27 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65" totalsRowBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66" totalsRowBorderDxfId="65">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="63"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="62"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="61"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="60"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="59"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="58"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="64"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="62"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="61"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="60"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F23" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
-  <autoFilter ref="B16:F23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F22" totalsRowShown="0" headerRowDxfId="58" headerRowBorderDxfId="57" tableBorderDxfId="56" totalsRowBorderDxfId="55">
+  <autoFilter ref="B16:F22"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="53"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="52"/>
-    <tableColumn id="3" name="[active]" dataDxfId="51"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="54"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="53"/>
+    <tableColumn id="3" name="[active]" dataDxfId="52"/>
     <tableColumn id="4" name="[icon]"/>
     <tableColumn id="5" name="[tidName]"/>
   </tableColumns>
@@ -2845,68 +2836,68 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="50">
-  <autoFilter ref="B33:G43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B32:G42" totalsRowShown="0" headerRowDxfId="51">
+  <autoFilter ref="B32:G42"/>
   <sortState ref="B25:G34">
     <sortCondition descending="1" ref="D24:D34"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
-    <tableColumn id="4" name="[type]" dataDxfId="46"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="48"/>
+    <tableColumn id="4" name="[type]" dataDxfId="47"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="46"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="3" name="[order]" dataDxfId="28"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
-    <tableColumn id="11" name="[android]" dataDxfId="25"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="40"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="3" name="[order]" dataDxfId="38"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="37"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="36"/>
+    <tableColumn id="11" name="[android]" dataDxfId="35"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="34"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="33"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="32"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="31"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="30"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="24"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="22"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
-    <tableColumn id="2" name="[url]" dataDxfId="3"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="16"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="15"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="14"/>
+    <tableColumn id="2" name="[url]" dataDxfId="13"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="12"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="11"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3178,10 +3169,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3482,37 +3473,37 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="D21" s="42" t="b">
+      <c r="B21" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F21" s="43" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="44" t="s">
-        <v>168</v>
-      </c>
-      <c r="D22" s="1" t="b">
+      <c r="B22" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" s="42" t="b">
         <v>0</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F22" s="43" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -3520,151 +3511,154 @@
         <v>3</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D23" s="42" t="b">
         <v>0</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F23" s="43" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="46" t="s">
         <v>177</v>
       </c>
       <c r="D24" s="42" t="b">
         <v>0</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="F24" s="43" t="s">
+      <c r="F24" s="46" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="46" t="s">
-        <v>180</v>
+      <c r="B25" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>229</v>
       </c>
       <c r="D25" s="42" t="b">
         <v>0</v>
       </c>
-      <c r="E25" s="46" t="s">
-        <v>181</v>
-      </c>
-      <c r="F25" s="46" t="s">
-        <v>182</v>
+      <c r="E25" s="43" t="s">
+        <v>230</v>
+      </c>
+      <c r="F25" s="43" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="46" t="s">
         <v>232</v>
       </c>
       <c r="D26" s="42" t="b">
         <v>0</v>
       </c>
-      <c r="E26" s="43" t="s">
-        <v>233</v>
-      </c>
-      <c r="F26" s="43" t="s">
-        <v>234</v>
+      <c r="E26" s="46" t="s">
+        <v>238</v>
+      </c>
+      <c r="F26" s="46" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="46" t="s">
-        <v>235</v>
+      <c r="C27" s="41" t="s">
+        <v>234</v>
       </c>
       <c r="D27" s="42" t="b">
         <v>0</v>
       </c>
-      <c r="E27" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="F27" s="46" t="s">
-        <v>242</v>
+      <c r="E27" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="41" t="s">
-        <v>237</v>
+      <c r="C28" s="46" t="s">
+        <v>235</v>
       </c>
       <c r="D28" s="42" t="b">
         <v>0</v>
       </c>
-      <c r="E28" s="43" t="s">
+      <c r="E28" s="46" t="s">
         <v>236</v>
       </c>
-      <c r="F28" s="43" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>238</v>
-      </c>
-      <c r="D29" s="42" t="b">
+      <c r="F28" s="46" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B30" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" t="s">
         <v>0</v>
       </c>
-      <c r="E29" s="46" t="s">
-        <v>239</v>
-      </c>
-      <c r="F29" s="46" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B31" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="138" x14ac:dyDescent="0.25">
-      <c r="B33" s="34" t="s">
+    </row>
+    <row r="32" spans="2:7" ht="138" x14ac:dyDescent="0.25">
+      <c r="B32" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C32" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D32" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="E33" s="37" t="s">
+      <c r="E32" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="F33" s="37" t="s">
+      <c r="F32" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="G33" s="38" t="s">
+      <c r="G32" s="38" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D33" s="39">
+        <v>3000000</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" s="19">
+        <v>1</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
@@ -3672,106 +3666,104 @@
         <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D34" s="39">
-        <v>3000000</v>
+        <v>2500000</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F34" s="19">
-        <v>1</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>138</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G34" s="19"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D35" s="39">
-        <v>2500000</v>
+        <v>2000000</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F35" s="19">
-        <v>5</v>
-      </c>
-      <c r="G35" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D36" s="39">
-        <v>2000000</v>
+        <v>1500000</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F36" s="19">
-        <v>1</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>140</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G36" s="19"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D37" s="39">
-        <v>1500000</v>
+        <v>1000000</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F37" s="19">
-        <v>5</v>
-      </c>
-      <c r="G37" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D38" s="39">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F38" s="19">
-        <v>1</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>139</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G38" s="19"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D39" s="39">
-        <v>500000</v>
+        <v>250000</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>134</v>
@@ -3786,16 +3778,16 @@
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D40" s="39">
-        <v>250000</v>
+        <v>100000</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F40" s="19">
-        <v>5</v>
+        <v>1500</v>
       </c>
       <c r="G40" s="19"/>
     </row>
@@ -3804,16 +3796,16 @@
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D41" s="39">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>123</v>
       </c>
       <c r="F41" s="19">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="G41" s="19"/>
     </row>
@@ -3822,44 +3814,26 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D42" s="39">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>123</v>
       </c>
       <c r="F42" s="19">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="G42" s="19"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" s="39">
-        <v>10000</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="F43" s="19">
-        <v>100</v>
-      </c>
-      <c r="G43" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="76" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 D17:D29"/>
-    <dataValidation type="list" sqref="E34:E43">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D33:D42 D11:F11 D17:D28"/>
+    <dataValidation type="list" sqref="E33:E42">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3882,7 +3856,7 @@
   </sheetPr>
   <dimension ref="B1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="101" workbookViewId="0">
+    <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
@@ -3954,7 +3928,7 @@
         <v>6</v>
       </c>
       <c r="K4" s="25" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="L4" s="25" t="s">
         <v>99</v>
@@ -3992,7 +3966,7 @@
         <v>70</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L5" s="16" t="s">
         <v>89</v>
@@ -4030,7 +4004,7 @@
         <v>66</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L6" s="16" t="s">
         <v>89</v>
@@ -4068,7 +4042,7 @@
         <v>62</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L7" s="16" t="s">
         <v>89</v>
@@ -4106,7 +4080,7 @@
         <v>58</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L8" s="16" t="s">
         <v>89</v>
@@ -4144,7 +4118,7 @@
         <v>54</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L9" s="16" t="s">
         <v>89</v>
@@ -4182,7 +4156,7 @@
         <v>50</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L10" s="16" t="s">
         <v>89</v>
@@ -4220,7 +4194,7 @@
         <v>46</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L11" s="16" t="s">
         <v>89</v>
@@ -4258,7 +4232,7 @@
         <v>43</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L12" s="16" t="s">
         <v>90</v>
@@ -4296,7 +4270,7 @@
         <v>39</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L13" s="16" t="s">
         <v>92</v>
@@ -4334,7 +4308,7 @@
         <v>35</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L14" s="16" t="s">
         <v>93</v>
@@ -4372,7 +4346,7 @@
         <v>98</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L15" s="17" t="s">
         <v>91</v>
@@ -4410,7 +4384,7 @@
         <v>113</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L16" s="17" t="s">
         <v>114</v>
@@ -4536,7 +4510,7 @@
     <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B32" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -4549,25 +4523,25 @@
     </row>
     <row r="34" spans="2:8" ht="129.75" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D34" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="F34" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="G34" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="H34" s="31" t="s">
         <v>190</v>
-      </c>
-      <c r="F34" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="G34" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="H34" s="31" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -4575,22 +4549,22 @@
         <v>3</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -4598,22 +4572,22 @@
         <v>3</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E36" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G36" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="F36" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>215</v>
-      </c>
       <c r="H36" s="18" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -4621,22 +4595,22 @@
         <v>3</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -4644,22 +4618,22 @@
         <v>3</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F38" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G38" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="G38" s="18" t="s">
-        <v>216</v>
-      </c>
       <c r="H38" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
@@ -4667,22 +4641,22 @@
         <v>3</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D39" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="E39" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="E39" s="22" t="s">
-        <v>212</v>
-      </c>
       <c r="F39" s="22" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H39" s="22" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
@@ -4690,22 +4664,22 @@
         <v>3</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D40" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="F40" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="E40" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>213</v>
-      </c>
       <c r="G40" s="18" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
@@ -4713,22 +4687,22 @@
         <v>3</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -4736,22 +4710,22 @@
         <v>3</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -4759,22 +4733,22 @@
         <v>3</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
@@ -4782,22 +4756,22 @@
         <v>3</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -4805,22 +4779,22 @@
         <v>3</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F45" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
@@ -4828,22 +4802,22 @@
         <v>3</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
@@ -4851,22 +4825,22 @@
         <v>3</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -4874,22 +4848,22 @@
         <v>3</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -4897,22 +4871,22 @@
         <v>3</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
@@ -4920,51 +4894,51 @@
         <v>3</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E50" s="30" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G50" s="30" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
WIP content ready to add new dragon tier
Former-commit-id: 9d6bf8754d7134e795af992ae60e1673dda8dd90
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -1114,7 +1114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1132,7 +1132,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45" wrapText="1"/>
     </xf>
@@ -1196,114 +1195,409 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="77">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
+  <dxfs count="91">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -2053,6 +2347,96 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2385,30 +2769,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -2602,53 +2962,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -2768,6 +3081,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2782,122 +3105,122 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="76" headerRowBorderDxfId="75" tableBorderDxfId="74" totalsRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="89" headerRowBorderDxfId="88" tableBorderDxfId="87" totalsRowBorderDxfId="86">
   <autoFilter ref="B4:Q5"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="72"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="71"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="70"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="69"/>
-    <tableColumn id="5" name="[incentivizeFBGem]"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]"/>
-    <tableColumn id="7" name="[miniMapHCCost]"/>
-    <tableColumn id="8" name="[miniMapTimer]"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]"/>
-    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="85"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="84"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="16"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="15"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="14"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="13"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="12"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="11"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="10"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="9"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="8"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="7"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="6"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="5"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="4"/>
+    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66" totalsRowBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="83" headerRowBorderDxfId="82" tableBorderDxfId="81" totalsRowBorderDxfId="80">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="64"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="62"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="61"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="60"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="59"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="79"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="78"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="77"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="76"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="75"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F22" totalsRowShown="0" headerRowDxfId="58" headerRowBorderDxfId="57" tableBorderDxfId="56" totalsRowBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F22" totalsRowShown="0" headerRowDxfId="74" headerRowBorderDxfId="73" tableBorderDxfId="72" totalsRowBorderDxfId="71">
   <autoFilter ref="B16:F22"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="54"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="53"/>
-    <tableColumn id="3" name="[active]" dataDxfId="52"/>
-    <tableColumn id="4" name="[icon]"/>
-    <tableColumn id="5" name="[tidName]"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="70"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="69"/>
+    <tableColumn id="3" name="[active]" dataDxfId="68"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B32:G42" totalsRowShown="0" headerRowDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B32:G42" totalsRowShown="0" headerRowDxfId="67">
   <autoFilter ref="B32:G42"/>
   <sortState ref="B25:G34">
     <sortCondition descending="1" ref="D24:D34"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="48"/>
-    <tableColumn id="4" name="[type]" dataDxfId="47"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="46"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="45"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="66"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="64"/>
+    <tableColumn id="4" name="[type]" dataDxfId="63"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="62"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49" totalsRowBorderDxfId="48">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="40"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="3" name="[order]" dataDxfId="38"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="37"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="36"/>
-    <tableColumn id="11" name="[android]" dataDxfId="35"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="34"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="33"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="32"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="31"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="30"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="29"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="47"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="46"/>
+    <tableColumn id="3" name="[order]" dataDxfId="45"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="44"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="43"/>
+    <tableColumn id="11" name="[android]" dataDxfId="42"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="41"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="40"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="39"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="38"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="37"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="24"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="22"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="21"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="31"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="30"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="29"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="16"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="14"/>
-    <tableColumn id="2" name="[url]" dataDxfId="13"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="12"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="11"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="10"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="23"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="22"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="21"/>
+    <tableColumn id="2" name="[url]" dataDxfId="20"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="19"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="18"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3171,8 +3494,8 @@
   </sheetPr>
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3203,19 +3526,19 @@
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="12" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:17" ht="306" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -3251,7 +3574,7 @@
       <c r="L4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="9" t="s">
         <v>22</v>
       </c>
       <c r="N4" s="4" t="s">
@@ -3277,43 +3600,43 @@
       <c r="D5" s="1">
         <v>0.08</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="47">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="42">
         <v>15</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="42">
         <v>100</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="42">
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="42">
         <v>4</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="42">
         <v>10</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="42">
         <v>240</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="42">
         <v>7.1428571428571426E-3</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="42">
         <v>0.2</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="42">
         <v>0.01</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="42">
         <v>1.2</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="42">
         <v>2.5</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="42">
         <v>25</v>
       </c>
     </row>
@@ -3368,7 +3691,7 @@
       <c r="F11" s="1">
         <v>0</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="42" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3400,7 +3723,7 @@
       <c r="E16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="28" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3408,16 +3731,16 @@
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="44" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="42" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3425,55 +3748,55 @@
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="40" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="42" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="44" t="s">
         <v>107</v>
       </c>
       <c r="D19" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="42" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="41" t="s">
+      <c r="B20" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="D20" s="42" t="b">
+      <c r="D20" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="43" t="s">
+      <c r="F20" s="42" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="44" t="s">
@@ -3482,55 +3805,55 @@
       <c r="D21" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="F21" s="43" t="s">
+      <c r="F21" s="42" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="41" t="s">
+      <c r="B22" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="D22" s="42" t="b">
+      <c r="D22" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="F22" s="43" t="s">
+      <c r="F22" s="42" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="41" t="s">
+      <c r="B23" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="44" t="s">
         <v>174</v>
       </c>
-      <c r="D23" s="42" t="b">
+      <c r="D23" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="E23" s="43" t="s">
+      <c r="E23" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="F23" s="43" t="s">
+      <c r="F23" s="42" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="46" t="s">
+      <c r="B24" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="D24" s="42" t="b">
+      <c r="D24" s="41" t="b">
         <v>0</v>
       </c>
       <c r="E24" s="46" t="s">
@@ -3541,30 +3864,30 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="41" t="s">
+      <c r="B25" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="44" t="s">
         <v>229</v>
       </c>
-      <c r="D25" s="42" t="b">
+      <c r="D25" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="E25" s="43" t="s">
+      <c r="E25" s="42" t="s">
         <v>230</v>
       </c>
-      <c r="F25" s="43" t="s">
+      <c r="F25" s="42" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="46" t="s">
+      <c r="B26" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="D26" s="42" t="b">
+      <c r="D26" s="41" t="b">
         <v>0</v>
       </c>
       <c r="E26" s="46" t="s">
@@ -3575,30 +3898,30 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="41" t="s">
+      <c r="B27" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="D27" s="42" t="b">
+      <c r="D27" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="F27" s="43" t="s">
+      <c r="F27" s="42" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="46" t="s">
+      <c r="B28" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="D28" s="42" t="b">
+      <c r="D28" s="41" t="b">
         <v>0</v>
       </c>
       <c r="E28" s="46" t="s">
@@ -3622,22 +3945,22 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="138" x14ac:dyDescent="0.25">
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="F32" s="37" t="s">
+      <c r="F32" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="G32" s="38" t="s">
+      <c r="G32" s="37" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3648,16 +3971,16 @@
       <c r="C33" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D33" s="39">
+      <c r="D33" s="38">
         <v>3000000</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="F33" s="19">
+      <c r="F33" s="18">
         <v>1</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="18" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3668,16 +3991,16 @@
       <c r="C34" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D34" s="39">
+      <c r="D34" s="38">
         <v>2500000</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F34" s="18">
         <v>5</v>
       </c>
-      <c r="G34" s="19"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
@@ -3686,16 +4009,16 @@
       <c r="C35" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D35" s="39">
+      <c r="D35" s="38">
         <v>2000000</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="F35" s="19">
+      <c r="F35" s="18">
         <v>1</v>
       </c>
-      <c r="G35" s="19" t="s">
+      <c r="G35" s="18" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3706,16 +4029,16 @@
       <c r="C36" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D36" s="39">
+      <c r="D36" s="38">
         <v>1500000</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="F36" s="19">
+      <c r="F36" s="18">
         <v>5</v>
       </c>
-      <c r="G36" s="19"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
@@ -3724,16 +4047,16 @@
       <c r="C37" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D37" s="39">
+      <c r="D37" s="38">
         <v>1000000</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F37" s="18">
         <v>1</v>
       </c>
-      <c r="G37" s="19" t="s">
+      <c r="G37" s="18" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3744,16 +4067,16 @@
       <c r="C38" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D38" s="39">
+      <c r="D38" s="38">
         <v>500000</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="F38" s="19">
+      <c r="F38" s="18">
         <v>5</v>
       </c>
-      <c r="G38" s="19"/>
+      <c r="G38" s="18"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
@@ -3762,16 +4085,16 @@
       <c r="C39" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D39" s="39">
+      <c r="D39" s="38">
         <v>250000</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="F39" s="19">
+      <c r="F39" s="18">
         <v>5</v>
       </c>
-      <c r="G39" s="19"/>
+      <c r="G39" s="18"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
@@ -3780,16 +4103,16 @@
       <c r="C40" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D40" s="39">
+      <c r="D40" s="38">
         <v>100000</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F40" s="19">
+      <c r="F40" s="18">
         <v>1500</v>
       </c>
-      <c r="G40" s="19"/>
+      <c r="G40" s="18"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
@@ -3798,16 +4121,16 @@
       <c r="C41" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D41" s="39">
+      <c r="D41" s="38">
         <v>50000</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F41" s="19">
+      <c r="F41" s="18">
         <v>500</v>
       </c>
-      <c r="G41" s="19"/>
+      <c r="G41" s="18"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
@@ -3816,20 +4139,20 @@
       <c r="C42" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="39">
+      <c r="D42" s="38">
         <v>10000</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="E42" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F42" s="19">
+      <c r="F42" s="18">
         <v>100</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="18"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D33:D42 D11:F11 D17:D28"/>
@@ -3856,7 +4179,7 @@
   </sheetPr>
   <dimension ref="B1:M50"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
@@ -3890,12 +4213,12 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3906,490 +4229,490 @@
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="23" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="18">
         <v>0</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="G5" s="18" t="b">
+      <c r="G5" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="18" t="b">
+      <c r="H5" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="14" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="20" t="s">
+      <c r="B6" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="18">
         <v>1</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="G6" s="18" t="b">
+      <c r="G6" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="18" t="b">
+      <c r="H6" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="14" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <v>2</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="G7" s="18" t="b">
+      <c r="G7" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="18" t="b">
+      <c r="H7" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="K7" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="L7" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="14" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="19">
-        <v>3</v>
-      </c>
-      <c r="E8" s="18" t="s">
+      <c r="D8" s="18">
+        <v>3</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="G8" s="18" t="b">
+      <c r="G8" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="18" t="b">
+      <c r="H8" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="K8" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="L8" s="16" t="s">
+      <c r="L8" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="M8" s="15" t="s">
+      <c r="M8" s="14" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <v>4</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="G9" s="18" t="b">
+      <c r="G9" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="18" t="b">
+      <c r="H9" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K9" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="L9" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="14" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <v>5</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G10" s="18" t="b">
+      <c r="G10" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="18" t="b">
+      <c r="H10" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="16" t="s">
+      <c r="K10" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="L10" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="14" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <v>6</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="G11" s="18" t="b">
+      <c r="G11" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="18" t="b">
+      <c r="H11" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="14" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="20" t="s">
+      <c r="B12" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>7</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="G12" s="18" t="b">
+      <c r="G12" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="H12" s="18" t="b">
+      <c r="H12" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="L12" s="16" t="s">
+      <c r="L12" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="14" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="20" t="s">
+      <c r="B13" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <v>8</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="18" t="b">
+      <c r="G13" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="18" t="b">
+      <c r="H13" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="L13" s="16" t="s">
+      <c r="L13" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="M13" s="14" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="20" t="s">
+      <c r="B14" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="18">
         <v>9</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="G14" s="18" t="b">
+      <c r="G14" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H14" s="18" t="b">
+      <c r="H14" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="K14" s="16" t="s">
+      <c r="K14" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="L14" s="16" t="s">
+      <c r="L14" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="M14" s="14" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="20" t="s">
+      <c r="B15" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="18">
         <v>10</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="G15" s="18" t="b">
+      <c r="G15" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="18" t="b">
+      <c r="H15" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="L15" s="17" t="s">
+      <c r="L15" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="M15" s="15" t="s">
+      <c r="M15" s="14" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="33" t="s">
+      <c r="B16" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="18">
         <v>11</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="G16" s="18" t="b">
+      <c r="G16" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="18" t="b">
+      <c r="H16" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="J16" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="K16" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="L16" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="M16" s="15" t="s">
+      <c r="M16" s="14" t="s">
         <v>165</v>
       </c>
     </row>
@@ -4408,14 +4731,14 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="2:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B20" s="28"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13" t="s">
+      <c r="B20" s="27"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="2:10" ht="118.5" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
@@ -4424,86 +4747,86 @@
       <c r="C21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="30" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="20" t="s">
+      <c r="B22" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="20" t="s">
+      <c r="B23" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="17"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="20" t="s">
+      <c r="B24" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="18"/>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="20" t="s">
+      <c r="B25" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="18"/>
+      <c r="E25" s="17"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="20" t="s">
+      <c r="B26" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="E26" s="22"/>
+      <c r="E26" s="21"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="33" t="s">
+      <c r="B27" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="17" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4528,417 +4851,417 @@
       <c r="C34" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="F34" s="31" t="s">
+      <c r="F34" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="G34" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="H34" s="31" t="s">
+      <c r="H34" s="30" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="20" t="s">
+      <c r="B35" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="F35" s="30" t="s">
+      <c r="F35" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="G35" s="30" t="s">
+      <c r="G35" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="H35" s="30" t="s">
+      <c r="H35" s="29" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="20" t="s">
+      <c r="B36" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F36" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G36" s="18" t="s">
+      <c r="G36" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H36" s="17" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="20" t="s">
+      <c r="B37" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="E37" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F37" s="18" t="s">
+      <c r="F37" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G37" s="18" t="s">
+      <c r="G37" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="H37" s="18" t="s">
+      <c r="H37" s="17" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F38" s="18" t="s">
+      <c r="F38" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G38" s="18" t="s">
+      <c r="G38" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="H38" s="17" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="20" t="s">
+      <c r="B39" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="E39" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="F39" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="G39" s="22" t="s">
+      <c r="G39" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="H39" s="22" t="s">
+      <c r="H39" s="21" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="33" t="s">
+      <c r="B40" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D40" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E40" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F40" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G40" s="18" t="s">
+      <c r="G40" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="H40" s="18" t="s">
+      <c r="H40" s="17" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="20" t="s">
+      <c r="B41" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F41" s="18" t="s">
+      <c r="F41" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G41" s="18" t="s">
+      <c r="G41" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="H41" s="18" t="s">
+      <c r="H41" s="17" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="20" t="s">
+      <c r="B42" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="F42" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G42" s="18" t="s">
+      <c r="G42" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="H42" s="17" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="20" t="s">
+      <c r="B43" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="E43" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F43" s="18" t="s">
+      <c r="F43" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G43" s="18" t="s">
+      <c r="G43" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="H43" s="18" t="s">
+      <c r="H43" s="17" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="20" t="s">
+      <c r="B44" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D44" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="E44" s="18" t="s">
+      <c r="E44" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F44" s="18" t="s">
+      <c r="F44" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G44" s="18" t="s">
+      <c r="G44" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="17" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="20" t="s">
+      <c r="B45" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D45" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="E45" s="18" t="s">
+      <c r="E45" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F45" s="18" t="s">
+      <c r="F45" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G45" s="18" t="s">
+      <c r="G45" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="H45" s="18" t="s">
+      <c r="H45" s="17" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="33" t="s">
+      <c r="B46" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D46" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F46" s="18" t="s">
+      <c r="F46" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G46" s="18" t="s">
+      <c r="G46" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="H46" s="18" t="s">
+      <c r="H46" s="17" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="20" t="s">
+      <c r="B47" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="D47" s="18" t="s">
+      <c r="D47" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="E47" s="18" t="s">
+      <c r="E47" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F47" s="18" t="s">
+      <c r="F47" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G47" s="18" t="s">
+      <c r="G47" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="H47" s="18" t="s">
+      <c r="H47" s="17" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="20" t="s">
+      <c r="B48" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="D48" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="E48" s="18" t="s">
+      <c r="E48" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F48" s="18" t="s">
+      <c r="F48" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G48" s="18" t="s">
+      <c r="G48" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H48" s="18" t="s">
+      <c r="H48" s="17" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="20" t="s">
+      <c r="B49" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D49" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="E49" s="18" t="s">
+      <c r="E49" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F49" s="18" t="s">
+      <c r="F49" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G49" s="18" t="s">
+      <c r="G49" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="H49" s="18" t="s">
+      <c r="H49" s="17" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="20" t="s">
+      <c r="B50" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D50" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="E50" s="30" t="s">
+      <c r="E50" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="F50" s="30" t="s">
+      <c r="F50" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="G50" s="30" t="s">
+      <c r="G50" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="H50" s="30" t="s">
+      <c r="H50" s="29" t="s">
         <v>220</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
adding notification definitions table
Former-commit-id: 37ebfb753b7148785cc19547c0ad44cb32578f65
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38175" windowHeight="19485"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="278">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -794,6 +794,105 @@
   </si>
   <si>
     <t>PF_LeagueFinishShareScreen</t>
+  </si>
+  <si>
+    <t>NOTIFICATIONS</t>
+  </si>
+  <si>
+    <t>{notificationsDefinitions}</t>
+  </si>
+  <si>
+    <t>sku.not.01</t>
+  </si>
+  <si>
+    <t>sku.not.02</t>
+  </si>
+  <si>
+    <t>sku.not.03</t>
+  </si>
+  <si>
+    <t>sku.not.04</t>
+  </si>
+  <si>
+    <t>[trackingSku]</t>
+  </si>
+  <si>
+    <t>TID_NOTIFICATION_EGG_HATCHED</t>
+  </si>
+  <si>
+    <t>Loyalty_EggHatched</t>
+  </si>
+  <si>
+    <t>TID_NOTIFICATION_NEW_MISSIONS</t>
+  </si>
+  <si>
+    <t>Loyalty_NewMissions</t>
+  </si>
+  <si>
+    <t>TID_NOTIFICATION_CHESTS_AVAILABLE</t>
+  </si>
+  <si>
+    <t>Loyalty_NewChests</t>
+  </si>
+  <si>
+    <t>TID_NOTIFICATION_DAILY_REWARD_AVAILABLE</t>
+  </si>
+  <si>
+    <t>Loyalty_DailyReward</t>
+  </si>
+  <si>
+    <t>Monetization_Discount</t>
+  </si>
+  <si>
+    <t>Monetization_DragonOffer</t>
+  </si>
+  <si>
+    <t>Monetization_PetOffer</t>
+  </si>
+  <si>
+    <t>Monetization_GatchaOffer</t>
+  </si>
+  <si>
+    <t>Loyalty_Tournament</t>
+  </si>
+  <si>
+    <t>Loyalty_PassiveEvent</t>
+  </si>
+  <si>
+    <t>Loyalty_Quest</t>
+  </si>
+  <si>
+    <t>Information_Update</t>
+  </si>
+  <si>
+    <t>Information_Season</t>
+  </si>
+  <si>
+    <t>sku.not.05</t>
+  </si>
+  <si>
+    <t>sku.not.06</t>
+  </si>
+  <si>
+    <t>sku.not.07</t>
+  </si>
+  <si>
+    <t>sku.not.08</t>
+  </si>
+  <si>
+    <t>sku.not.09</t>
+  </si>
+  <si>
+    <t>sku.not.10</t>
+  </si>
+  <si>
+    <t>sku.not.11</t>
+  </si>
+  <si>
+    <t>sku.not.12</t>
+  </si>
+  <si>
+    <t>sku.not.13</t>
   </si>
 </sst>
 </file>
@@ -962,7 +1061,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1110,11 +1209,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1201,403 +1330,120 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="91">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2347,96 +2193,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2625,6 +2381,50 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2769,6 +2569,34 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -2964,6 +2792,327 @@
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
           <color auto="1"/>
         </left>
         <right style="thin">
@@ -3081,16 +3230,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3105,122 +3244,122 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="89" headerRowBorderDxfId="88" tableBorderDxfId="87" totalsRowBorderDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88" totalsRowBorderDxfId="87">
   <autoFilter ref="B4:Q5"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="85"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="84"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="16"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="15"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="14"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="13"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="12"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="11"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="10"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="9"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="8"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="7"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="6"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="5"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="4"/>
-    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="3"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="86"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="85"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="84"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="83"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="82"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="81"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="80"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="79"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="78"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="77"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="76"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="74"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="73"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="72"/>
+    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="83" headerRowBorderDxfId="82" tableBorderDxfId="81" totalsRowBorderDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="70" headerRowBorderDxfId="69" tableBorderDxfId="68" totalsRowBorderDxfId="67">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="79"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="78"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="77"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="76"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="75"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="2"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="66"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="64"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="63"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="62"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F22" totalsRowShown="0" headerRowDxfId="74" headerRowBorderDxfId="73" tableBorderDxfId="72" totalsRowBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:F22" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
   <autoFilter ref="B16:F22"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="70"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="69"/>
-    <tableColumn id="3" name="[active]" dataDxfId="68"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
+    <tableColumn id="3" name="[active]" dataDxfId="54"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="53"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B32:G42" totalsRowShown="0" headerRowDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B32:G42" totalsRowShown="0" headerRowDxfId="51">
   <autoFilter ref="B32:G42"/>
   <sortState ref="B25:G34">
     <sortCondition descending="1" ref="D24:D34"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="66"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="64"/>
-    <tableColumn id="4" name="[type]" dataDxfId="63"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="62"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="61"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="48"/>
+    <tableColumn id="4" name="[type]" dataDxfId="47"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="46"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49" totalsRowBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="47"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="46"/>
-    <tableColumn id="3" name="[order]" dataDxfId="45"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="44"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="43"/>
-    <tableColumn id="11" name="[android]" dataDxfId="42"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="41"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="40"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="39"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="38"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="37"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="36"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="40"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="3" name="[order]" dataDxfId="38"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="37"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="36"/>
+    <tableColumn id="11" name="[android]" dataDxfId="35"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="34"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="33"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="32"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="31"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="30"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="31"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="30"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="29"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="28"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="24"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="22"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="23"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="22"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="21"/>
-    <tableColumn id="2" name="[url]" dataDxfId="20"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="19"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="18"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="17"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="16"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="15"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="14"/>
+    <tableColumn id="2" name="[url]" dataDxfId="13"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="12"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="11"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3492,10 +3631,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3503,8 +3642,8 @@
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="26" width="12" customWidth="1"/>
@@ -4150,12 +4289,203 @@
       </c>
       <c r="G42" s="18"/>
     </row>
+    <row r="44" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B45" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
+      <c r="B47" s="49" t="s">
+        <v>246</v>
+      </c>
+      <c r="C47" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" s="51" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>247</v>
+      </c>
+      <c r="D48" s="48" t="s">
+        <v>252</v>
+      </c>
+      <c r="E48" s="48" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="D49" s="48" t="s">
+        <v>254</v>
+      </c>
+      <c r="E49" s="48" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="48" t="s">
+        <v>249</v>
+      </c>
+      <c r="D50" s="48" t="s">
+        <v>256</v>
+      </c>
+      <c r="E50" s="48" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="48" t="s">
+        <v>250</v>
+      </c>
+      <c r="D51" s="48" t="s">
+        <v>258</v>
+      </c>
+      <c r="E51" s="48" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="48" t="s">
+        <v>269</v>
+      </c>
+      <c r="D52" s="48"/>
+      <c r="E52" s="48" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="48" t="s">
+        <v>270</v>
+      </c>
+      <c r="D53" s="48"/>
+      <c r="E53" s="48" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="48" t="s">
+        <v>271</v>
+      </c>
+      <c r="D54" s="48"/>
+      <c r="E54" s="48" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="48" t="s">
+        <v>272</v>
+      </c>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="48" t="s">
+        <v>273</v>
+      </c>
+      <c r="D56" s="48"/>
+      <c r="E56" s="48" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="48" t="s">
+        <v>274</v>
+      </c>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="D58" s="48"/>
+      <c r="E58" s="48" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="D59" s="48"/>
+      <c r="E59" s="48" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="48" t="s">
+        <v>277</v>
+      </c>
+      <c r="D60" s="48"/>
+      <c r="E60" s="48" t="s">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="90" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D33:D42 D11:F11 D17:D28"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D33:D42 D11:F11 D17:D28 D52:D57 E52:E53"/>
     <dataValidation type="list" sqref="E33:E42">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
@@ -4179,7 +4509,7 @@
   </sheetPr>
   <dimension ref="B1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+    <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
@@ -5237,31 +5567,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="60" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="59" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="58" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="57" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="56" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="55" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="54" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="53" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
fixed blood confetti content
Former-commit-id: 28ad09e6b76d9812248aba6b9120ac487d7c0067
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -904,17 +904,17 @@
     <t>TID_SEASON_ANNIVERSARY1_NAME</t>
   </si>
   <si>
-    <t>[ bloodParticles]</t>
-  </si>
-  <si>
     <t>PS_XMasPresentCollect</t>
+  </si>
+  <si>
+    <t>[bloodParticles]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -994,12 +994,6 @@
       <sz val="14"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1277,7 +1271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1377,12 +1371,9 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1405,22 +1396,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1443,104 +1418,164 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -2290,6 +2325,96 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2481,6 +2606,83 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -2622,12 +2824,248 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2659,19 +3097,23 @@
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2683,43 +3125,23 @@
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2843,445 +3265,14 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3297,123 +3288,123 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88" totalsRowBorderDxfId="87">
   <autoFilter ref="B4:Q5"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="85"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="84"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="83"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="82"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="81"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="80"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="79"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="78"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="77"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="74"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="73"/>
-    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="72"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="86"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="85"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="84"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="83"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="82"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="81"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="80"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="79"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="78"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="77"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="76"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="74"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="73"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="72"/>
+    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="70" headerRowBorderDxfId="69" tableBorderDxfId="68" totalsRowBorderDxfId="67">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="67"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="65"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="64"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="63"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="62"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="66"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="64"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="63"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="62"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
   <autoFilter ref="B16:G29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="57"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="56"/>
-    <tableColumn id="3" name="[active]" dataDxfId="55"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="2"/>
-    <tableColumn id="6" name="[ bloodParticles]" dataDxfId="0"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="5"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="4"/>
+    <tableColumn id="3" name="[active]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="1"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="60">
   <autoFilter ref="B33:G43"/>
   <sortState ref="B25:G35">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="53"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="52"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="51"/>
-    <tableColumn id="4" name="[type]" dataDxfId="50"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="49"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="48"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="59"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="58"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="57"/>
+    <tableColumn id="4" name="[type]" dataDxfId="56"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="55"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="43"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="42"/>
-    <tableColumn id="3" name="[order]" dataDxfId="41"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="40"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="39"/>
-    <tableColumn id="11" name="[android]" dataDxfId="38"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="37"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="36"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="35"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="34"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="33"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="32"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="40"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="3" name="[order]" dataDxfId="38"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="37"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="36"/>
+    <tableColumn id="11" name="[android]" dataDxfId="35"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="34"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="33"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="32"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="31"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="30"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="27"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="26"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="25"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="24"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="24"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="22"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="19"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="18"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="17"/>
-    <tableColumn id="2" name="[url]" dataDxfId="16"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="15"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="14"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="13"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="16"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="15"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="14"/>
+    <tableColumn id="2" name="[url]" dataDxfId="13"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="12"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="11"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3687,7 +3678,7 @@
   </sheetPr>
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -3920,7 +3911,7 @@
         <v>74</v>
       </c>
       <c r="G16" s="51" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -4139,7 +4130,7 @@
       </c>
       <c r="G28" s="42"/>
     </row>
-    <row r="29" spans="2:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="54" t="s">
         <v>3</v>
       </c>
@@ -4155,8 +4146,8 @@
       <c r="F29" s="55" t="s">
         <v>280</v>
       </c>
-      <c r="G29" s="56" t="s">
-        <v>282</v>
+      <c r="G29" s="55" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4571,7 +4562,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 E53:E54 D53:D58 D17:D29"/>
@@ -5656,31 +5647,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
Added summer icon for Gelato Pet
Former-commit-id: 748580504a2c2ee44e82c89ddc18775311b6e928
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="281">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -896,12 +896,6 @@
   </si>
   <si>
     <t>Anniversary1</t>
-  </si>
-  <si>
-    <t>icon_season_Anniversary1</t>
-  </si>
-  <si>
-    <t>TID_SEASON_ANNIVERSARY1_NAME</t>
   </si>
   <si>
     <t>PS_XMasPresentCollect</t>
@@ -1380,204 +1374,6 @@
   </cellStyles>
   <dxfs count="92">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2566,6 +2362,204 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3328,83 +3322,83 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
   <autoFilter ref="B16:G29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="5"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="4"/>
-    <tableColumn id="3" name="[active]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="0"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
+    <tableColumn id="3" name="[active]" dataDxfId="54"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="53"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="52"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="50">
   <autoFilter ref="B33:G43"/>
   <sortState ref="B25:G35">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="59"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="58"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="57"/>
-    <tableColumn id="4" name="[type]" dataDxfId="56"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="55"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="54"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
+    <tableColumn id="4" name="[type]" dataDxfId="46"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="40"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="3" name="[order]" dataDxfId="38"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="37"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="36"/>
-    <tableColumn id="11" name="[android]" dataDxfId="35"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="34"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="33"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="32"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="31"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="30"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="29"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" name="[order]" dataDxfId="28"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
+    <tableColumn id="11" name="[android]" dataDxfId="25"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="24"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="22"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="21"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="16"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="14"/>
-    <tableColumn id="2" name="[url]" dataDxfId="13"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="12"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="11"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="10"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
+    <tableColumn id="2" name="[url]" dataDxfId="3"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3679,7 +3673,7 @@
   <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3689,7 +3683,7 @@
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="46.7109375" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="26" width="12" customWidth="1"/>
   </cols>
@@ -3911,7 +3905,7 @@
         <v>74</v>
       </c>
       <c r="G16" s="51" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -4140,14 +4134,14 @@
       <c r="D29" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="E29" s="55" t="s">
+      <c r="E29" s="44" t="s">
+        <v>236</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>241</v>
+      </c>
+      <c r="G29" s="55" t="s">
         <v>279</v>
-      </c>
-      <c r="F29" s="55" t="s">
-        <v>280</v>
-      </c>
-      <c r="G29" s="55" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5647,31 +5641,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="53" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="52" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="51" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="50" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="49" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="48" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="47" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
Just adding a new sheet to show a graph HC / Time
Former-commit-id: c607587cec23a330e6ad0b0a732e810a57871335
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
+    <sheet name="TimeCost" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="285">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -902,6 +903,18 @@
   </si>
   <si>
     <t>[bloodParticles]</t>
+  </si>
+  <si>
+    <t>CoefA</t>
+  </si>
+  <si>
+    <t>CoefB</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>TIME (min)</t>
   </si>
 </sst>
 </file>
@@ -1374,6 +1387,106 @@
   </cellStyles>
   <dxfs count="92">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2121,96 +2234,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3258,16 +3281,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3281,124 +3294,1189 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>TIME(min)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TimeCost!$I$13:$I$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeCost!$J$13:$J$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.6000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12.200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>14.200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8129-4B27-B024-108D633382A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="249649184"/>
+        <c:axId val="246979392"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="249649184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="246979392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="246979392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="249649184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>338137</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88" totalsRowBorderDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="B4:Q5"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="86"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="85"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="84"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="83"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="82"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="81"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="80"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="79"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="78"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="77"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="76"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="74"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="73"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="72"/>
-    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="71"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="85"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="84"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="83"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="82"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="81"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="80"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="79"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="78"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="77"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="74"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="73"/>
+    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="70" headerRowBorderDxfId="69" tableBorderDxfId="68" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="66"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="64"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="63"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="62"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="61"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="67"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="65"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="64"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="63"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
   <autoFilter ref="B16:G29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="56"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
-    <tableColumn id="3" name="[active]" dataDxfId="54"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="53"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="52"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="51"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="56"/>
+    <tableColumn id="3" name="[active]" dataDxfId="55"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="54"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="53"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="51">
   <autoFilter ref="B33:G43"/>
   <sortState ref="B25:G35">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
-    <tableColumn id="4" name="[type]" dataDxfId="46"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="48"/>
+    <tableColumn id="4" name="[type]" dataDxfId="47"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="46"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="3" name="[order]" dataDxfId="28"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
-    <tableColumn id="11" name="[android]" dataDxfId="25"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="40"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="3" name="[order]" dataDxfId="38"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="37"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="36"/>
+    <tableColumn id="11" name="[android]" dataDxfId="35"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="34"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="33"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="32"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="31"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="30"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="24"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="22"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
-    <tableColumn id="2" name="[url]" dataDxfId="3"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="16"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="15"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="14"/>
+    <tableColumn id="2" name="[url]" dataDxfId="13"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="12"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="11"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3672,8 +4750,8 @@
   </sheetPr>
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4556,7 +5634,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="91" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 E53:E54 D53:D58 D17:D29"/>
@@ -5641,31 +6719,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">
@@ -5684,4 +6762,379 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
+  <dimension ref="F4:J48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AC36" sqref="AC36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F4" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>281</v>
+      </c>
+      <c r="G8">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>282</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>284</v>
+      </c>
+      <c r="J12" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <f>($G$8*I13)+$G$9</f>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="14" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14:J48" si="0">($G$8*I14)+$G$9</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="15" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>20</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>25</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>30</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>35</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>3.8000000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>40</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>45</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>50</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>55</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>60</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="25" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>65</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="26" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>70</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>75</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>80</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="29" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>85</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="30" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>90</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="31" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>95</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>8.6000000000000014</v>
+      </c>
+    </row>
+    <row r="32" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>100</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>105</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="34" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>110</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>115</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>10.200000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>120</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="37" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>125</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>130</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="39" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>135</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="40" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>140</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>12.200000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>145</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="42" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>150</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>155</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="44" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>160</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="45" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>165</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>14.200000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>170</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="0"/>
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="47" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>175</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>180</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="0"/>
+        <v>15.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating time/HC desired curve
Former-commit-id: f7756f1ec8b5b5b0c675de9c9d946aeea9c5259a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -16,7 +16,7 @@
     <sheet name="tech" sheetId="3" r:id="rId2"/>
     <sheet name="TimeCost" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="286">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -915,6 +915,9 @@
   </si>
   <si>
     <t>TIME (min)</t>
+  </si>
+  <si>
+    <t>DESIRED</t>
   </si>
 </sst>
 </file>
@@ -1387,106 +1390,6 @@
   </cellStyles>
   <dxfs count="92">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2234,6 +2137,96 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3280,6 +3273,16 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3768,6 +3771,383 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="108"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="8"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.5632675373925198E-2"/>
+          <c:y val="0.52871472484599469"/>
+          <c:w val="0.97134017408023399"/>
+          <c:h val="0.44441187020380707"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>TIME(min)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TimeCost!$I$56:$I$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeCost!$J$56:$J$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.6000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.6000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.6000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-77AE-40EE-A526-43A4259726F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="249649184"/>
+        <c:axId val="246979392"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="249649184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="246979392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="246979392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="249649184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3808,7 +4188,529 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="19">
+  <a:schemeClr val="accent6"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4356,127 +5258,159 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>347663</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88" totalsRowBorderDxfId="87">
   <autoFilter ref="B4:Q5"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="85"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="84"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="83"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="82"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="81"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="80"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="79"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="78"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="77"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="74"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="73"/>
-    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="72"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="86"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="85"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="84"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="83"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="82"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="81"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="80"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="79"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="78"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="77"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="76"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="74"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="73"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="72"/>
+    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="70" headerRowBorderDxfId="69" tableBorderDxfId="68" totalsRowBorderDxfId="67">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="67"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="65"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="64"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="63"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="62"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="66"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="64"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="63"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="62"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
   <autoFilter ref="B16:G29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="57"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="56"/>
-    <tableColumn id="3" name="[active]" dataDxfId="55"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="54"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="53"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="52"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
+    <tableColumn id="3" name="[active]" dataDxfId="54"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="53"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="52"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="50">
   <autoFilter ref="B33:G43"/>
   <sortState ref="B25:G35">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="48"/>
-    <tableColumn id="4" name="[type]" dataDxfId="47"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="46"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="45"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
+    <tableColumn id="4" name="[type]" dataDxfId="46"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="40"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="3" name="[order]" dataDxfId="38"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="37"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="36"/>
-    <tableColumn id="11" name="[android]" dataDxfId="35"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="34"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="33"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="32"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="31"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="30"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="29"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" name="[order]" dataDxfId="28"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
+    <tableColumn id="11" name="[android]" dataDxfId="25"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="24"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="22"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="21"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="16"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="14"/>
-    <tableColumn id="2" name="[url]" dataDxfId="13"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="12"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="11"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="10"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
+    <tableColumn id="2" name="[url]" dataDxfId="3"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5634,7 +6568,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 E53:E54 D53:D58 D17:D29"/>
@@ -6719,31 +7653,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">
@@ -6769,10 +7703,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="F4:J48"/>
+  <dimension ref="F4:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AC36" sqref="AC36"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7133,6 +8067,364 @@
         <v>15.4</v>
       </c>
     </row>
+    <row r="50" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="51" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F51" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>281</v>
+      </c>
+      <c r="G53">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="54" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>282</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>284</v>
+      </c>
+      <c r="J55" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="56" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>5</v>
+      </c>
+      <c r="J56">
+        <f>(I56*$G$53)+$G$54</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="57" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <v>10</v>
+      </c>
+      <c r="J57">
+        <f t="shared" ref="J57:J91" si="1">(I57*$G$53)+$G$54</f>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="58" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <v>15</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="59" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <v>20</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="60" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <v>25</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>30</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="1"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <v>35</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="1"/>
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <v>40</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="1"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="64" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <v>45</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="1"/>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="65" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <v>50</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <v>55</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="1"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="67" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <v>60</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="1"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="68" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <v>65</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="69" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <v>70</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="1"/>
+        <v>3.8000000000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <v>75</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I71">
+        <v>80</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="1"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="72" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I72">
+        <v>85</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="1"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="73" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I73">
+        <v>90</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="1"/>
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="74" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I74">
+        <v>95</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="1"/>
+        <v>4.8000000000000007</v>
+      </c>
+    </row>
+    <row r="75" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I75">
+        <v>100</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I76">
+        <v>105</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="1"/>
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="77" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I77">
+        <v>110</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="1"/>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="78" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I78">
+        <v>115</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="1"/>
+        <v>5.6000000000000005</v>
+      </c>
+    </row>
+    <row r="79" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <v>120</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="1"/>
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="80" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <v>125</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <v>130</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="1"/>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="82" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I82">
+        <v>135</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="1"/>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="83" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <v>140</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="1"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="84" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <v>145</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="1"/>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="85" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <v>150</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <v>155</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="1"/>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="87" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I87">
+        <v>160</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="1"/>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="88" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I88">
+        <v>165</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="1"/>
+        <v>7.6000000000000005</v>
+      </c>
+    </row>
+    <row r="89" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <v>170</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="1"/>
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="90" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I90">
+        <v>175</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I91">
+        <v>180</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="1"/>
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Time cost modified. Now, time-cost curve is more flat
Former-commit-id: a1e92c38a848081bb66dabc5469be5be76e85d6b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="287">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -918,6 +918,9 @@
   </si>
   <si>
     <t>DESIRED</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -3373,112 +3376,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>60</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>65</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>70</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>75</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>80</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>85</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>90</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>95</c:v>
+                  <c:v>285</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>100</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>105</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>110</c:v>
+                  <c:v>330</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>115</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>120</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>125</c:v>
+                  <c:v>375</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>130</c:v>
+                  <c:v>390</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>135</c:v>
+                  <c:v>405</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>140</c:v>
+                  <c:v>420</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>145</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>150</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>155</c:v>
+                  <c:v>465</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>160</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>165</c:v>
+                  <c:v>495</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>170</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>175</c:v>
+                  <c:v>525</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>180</c:v>
+                  <c:v>540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3490,112 +3493,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>1.4</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.4</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8000000000000003</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.2</c:v>
+                  <c:v>10.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>11.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.4</c:v>
+                  <c:v>14.200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.8</c:v>
+                  <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.2</c:v>
+                  <c:v>16.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.6000000000000005</c:v>
+                  <c:v>17.8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.4</c:v>
+                  <c:v>20.2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.8</c:v>
+                  <c:v>21.400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.1999999999999993</c:v>
+                  <c:v>22.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.6000000000000014</c:v>
+                  <c:v>23.8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.4</c:v>
+                  <c:v>26.2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.8000000000000007</c:v>
+                  <c:v>27.400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10.200000000000001</c:v>
+                  <c:v>28.6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10.6</c:v>
+                  <c:v>29.8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>11.4</c:v>
+                  <c:v>32.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11.8</c:v>
+                  <c:v>33.4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>12.200000000000001</c:v>
+                  <c:v>34.6</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>12.6</c:v>
+                  <c:v>35.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13.4</c:v>
+                  <c:v>38.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>13.8</c:v>
+                  <c:v>39.4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>14.200000000000001</c:v>
+                  <c:v>40.6</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>14.6</c:v>
+                  <c:v>41.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>15</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>15.4</c:v>
+                  <c:v>44.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3826,112 +3829,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>60</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>65</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>70</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>75</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>80</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>85</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>90</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>95</c:v>
+                  <c:v>285</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>100</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>105</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>110</c:v>
+                  <c:v>330</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>115</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>120</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>125</c:v>
+                  <c:v>375</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>130</c:v>
+                  <c:v>390</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>135</c:v>
+                  <c:v>405</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>140</c:v>
+                  <c:v>420</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>145</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>150</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>155</c:v>
+                  <c:v>465</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>160</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>165</c:v>
+                  <c:v>495</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>170</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>175</c:v>
+                  <c:v>525</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>180</c:v>
+                  <c:v>540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3943,112 +3946,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>1.2</c:v>
+                  <c:v>4.125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4</c:v>
+                  <c:v>4.6500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6</c:v>
+                  <c:v>5.1750000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8</c:v>
+                  <c:v>5.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>6.2250000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4000000000000004</c:v>
+                  <c:v>7.2750000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.6</c:v>
+                  <c:v>7.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8</c:v>
+                  <c:v>8.3250000000000011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>8.8500000000000014</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2</c:v>
+                  <c:v>9.375</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.4</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.6</c:v>
+                  <c:v>10.425000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.8000000000000003</c:v>
+                  <c:v>10.950000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4</c:v>
+                  <c:v>11.475000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>12.525</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>13.05</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.8000000000000007</c:v>
+                  <c:v>13.575000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5</c:v>
+                  <c:v>14.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.2</c:v>
+                  <c:v>14.625</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.4</c:v>
+                  <c:v>15.15</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.6000000000000005</c:v>
+                  <c:v>15.675000000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.8</c:v>
+                  <c:v>16.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6</c:v>
+                  <c:v>16.725000000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.2</c:v>
+                  <c:v>17.250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.4</c:v>
+                  <c:v>17.775000000000002</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.6000000000000005</c:v>
+                  <c:v>18.3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.8</c:v>
+                  <c:v>18.825000000000003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7</c:v>
+                  <c:v>19.350000000000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.2</c:v>
+                  <c:v>19.875000000000004</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.4</c:v>
+                  <c:v>20.400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>7.6000000000000005</c:v>
+                  <c:v>20.925000000000004</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.8</c:v>
+                  <c:v>21.450000000000003</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8</c:v>
+                  <c:v>21.975000000000001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.1999999999999993</c:v>
+                  <c:v>22.500000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5684,8 +5687,8 @@
   </sheetPr>
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5788,10 +5791,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="1">
-        <v>0.08</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E5" s="45">
-        <v>1</v>
+        <v>3.6</v>
       </c>
       <c r="F5" s="42">
         <v>15</v>
@@ -7703,10 +7706,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="F4:J91"/>
+  <dimension ref="F4:Q91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="N67" sqref="N67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7745,355 +7748,365 @@
     </row>
     <row r="13" spans="6:10" x14ac:dyDescent="0.25">
       <c r="I13">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J13">
         <f>($G$8*I13)+$G$9</f>
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="14" spans="6:10" x14ac:dyDescent="0.25">
       <c r="I14">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="J14">
         <f t="shared" ref="J14:J48" si="0">($G$8*I14)+$G$9</f>
-        <v>1.8</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="15" spans="6:10" x14ac:dyDescent="0.25">
       <c r="I15">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="16" spans="6:10" x14ac:dyDescent="0.25">
       <c r="I16">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>2.6</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="17" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I17">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I18">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>3.4</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="19" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I19">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>3.8000000000000003</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="20" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I20">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="21" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I21">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>4.5999999999999996</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="22" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I22">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I23">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>5.4</v>
+        <v>14.200000000000001</v>
       </c>
     </row>
     <row r="24" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I24">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>5.8</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="25" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I25">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>6.2</v>
+        <v>16.600000000000001</v>
       </c>
     </row>
     <row r="26" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I26">
-        <v>70</v>
+        <v>210</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>6.6000000000000005</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="27" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I27">
-        <v>75</v>
+        <v>225</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I28">
-        <v>80</v>
+        <v>240</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>7.4</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="29" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I29">
-        <v>85</v>
+        <v>255</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>7.8</v>
+        <v>21.400000000000002</v>
       </c>
     </row>
     <row r="30" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I30">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>8.1999999999999993</v>
+        <v>22.6</v>
       </c>
     </row>
     <row r="31" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I31">
-        <v>95</v>
+        <v>285</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>8.6000000000000014</v>
+        <v>23.8</v>
       </c>
     </row>
     <row r="32" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I32">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I33">
-        <v>105</v>
+        <v>315</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>9.4</v>
+        <v>26.2</v>
       </c>
     </row>
     <row r="34" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I34">
-        <v>110</v>
+        <v>330</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>9.8000000000000007</v>
+        <v>27.400000000000002</v>
       </c>
     </row>
     <row r="35" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I35">
-        <v>115</v>
+        <v>345</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>10.200000000000001</v>
+        <v>28.6</v>
       </c>
     </row>
     <row r="36" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I36">
-        <v>120</v>
+        <v>360</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>10.6</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="37" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I37">
-        <v>125</v>
+        <v>375</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I38">
-        <v>130</v>
+        <v>390</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>11.4</v>
+        <v>32.200000000000003</v>
       </c>
     </row>
     <row r="39" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I39">
-        <v>135</v>
+        <v>405</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>11.8</v>
+        <v>33.4</v>
       </c>
     </row>
     <row r="40" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I40">
-        <v>140</v>
+        <v>420</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>12.200000000000001</v>
+        <v>34.6</v>
       </c>
     </row>
     <row r="41" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I41">
-        <v>145</v>
+        <v>435</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>12.6</v>
+        <v>35.800000000000004</v>
       </c>
     </row>
     <row r="42" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I42">
-        <v>150</v>
+        <v>450</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I43">
-        <v>155</v>
+        <v>465</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>13.4</v>
+        <v>38.200000000000003</v>
       </c>
     </row>
     <row r="44" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I44">
-        <v>160</v>
+        <v>480</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>13.8</v>
+        <v>39.4</v>
       </c>
     </row>
     <row r="45" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I45">
-        <v>165</v>
+        <v>495</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>14.200000000000001</v>
+        <v>40.6</v>
       </c>
     </row>
     <row r="46" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I46">
-        <v>170</v>
+        <v>510</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>14.6</v>
+        <v>41.800000000000004</v>
       </c>
     </row>
     <row r="47" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I47">
-        <v>175</v>
+        <v>525</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I48">
-        <v>180</v>
+        <v>540</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="50" spans="6:10" x14ac:dyDescent="0.25">
+        <v>44.2</v>
+      </c>
+    </row>
+    <row r="50" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="51" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F51" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="53" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="Q51">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="52" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="Q52">
+        <f>4*60</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="53" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
         <v>281</v>
       </c>
       <c r="G53">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="54" spans="6:10" x14ac:dyDescent="0.25">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
         <v>282</v>
       </c>
       <c r="G54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="6:10" x14ac:dyDescent="0.25">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="55" spans="6:17" x14ac:dyDescent="0.25">
       <c r="I55" t="s">
         <v>284</v>
       </c>
@@ -8101,328 +8114,337 @@
         <v>283</v>
       </c>
     </row>
-    <row r="56" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>286</v>
+      </c>
       <c r="I56">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J56">
         <f>(I56*$G$53)+$G$54</f>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="57" spans="6:10" x14ac:dyDescent="0.25">
+        <v>4.125</v>
+      </c>
+    </row>
+    <row r="57" spans="6:17" x14ac:dyDescent="0.25">
       <c r="I57">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="J57">
         <f t="shared" ref="J57:J91" si="1">(I57*$G$53)+$G$54</f>
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="58" spans="6:10" x14ac:dyDescent="0.25">
+        <v>4.6500000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="6:17" x14ac:dyDescent="0.25">
       <c r="I58">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="J58">
         <f t="shared" si="1"/>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="59" spans="6:10" x14ac:dyDescent="0.25">
+        <v>5.1750000000000007</v>
+      </c>
+    </row>
+    <row r="59" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>286</v>
+      </c>
       <c r="I59">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="J59">
         <f t="shared" si="1"/>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="60" spans="6:10" x14ac:dyDescent="0.25">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="60" spans="6:17" x14ac:dyDescent="0.25">
       <c r="I60">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="J60">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="6:10" x14ac:dyDescent="0.25">
+        <v>6.2250000000000005</v>
+      </c>
+    </row>
+    <row r="61" spans="6:17" x14ac:dyDescent="0.25">
       <c r="I61">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="J61">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="62" spans="6:10" x14ac:dyDescent="0.25">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="62" spans="6:17" x14ac:dyDescent="0.25">
       <c r="I62">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="J62">
         <f t="shared" si="1"/>
-        <v>2.4000000000000004</v>
-      </c>
-    </row>
-    <row r="63" spans="6:10" x14ac:dyDescent="0.25">
+        <v>7.2750000000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="6:17" x14ac:dyDescent="0.25">
       <c r="I63">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="J63">
         <f t="shared" si="1"/>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="64" spans="6:10" x14ac:dyDescent="0.25">
+        <v>7.8000000000000007</v>
+      </c>
+    </row>
+    <row r="64" spans="6:17" x14ac:dyDescent="0.25">
       <c r="I64">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="J64">
         <f t="shared" si="1"/>
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="65" spans="9:10" x14ac:dyDescent="0.25">
+        <v>8.3250000000000011</v>
+      </c>
+    </row>
+    <row r="65" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I65">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="J65">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="9:10" x14ac:dyDescent="0.25">
+        <v>8.8500000000000014</v>
+      </c>
+    </row>
+    <row r="66" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I66">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="J66">
         <f t="shared" si="1"/>
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="67" spans="9:10" x14ac:dyDescent="0.25">
+        <v>9.375</v>
+      </c>
+    </row>
+    <row r="67" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I67">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="J67">
         <f t="shared" si="1"/>
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="68" spans="9:10" x14ac:dyDescent="0.25">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="68" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I68">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="J68">
         <f t="shared" si="1"/>
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="69" spans="9:10" x14ac:dyDescent="0.25">
+        <v>10.425000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I69">
-        <v>70</v>
+        <v>210</v>
       </c>
       <c r="J69">
         <f t="shared" si="1"/>
-        <v>3.8000000000000003</v>
-      </c>
-    </row>
-    <row r="70" spans="9:10" x14ac:dyDescent="0.25">
+        <v>10.950000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I70">
-        <v>75</v>
+        <v>225</v>
       </c>
       <c r="J70">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="9:10" x14ac:dyDescent="0.25">
+        <v>11.475000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H71" t="s">
+        <v>286</v>
+      </c>
       <c r="I71">
-        <v>80</v>
+        <v>240</v>
       </c>
       <c r="J71">
         <f t="shared" si="1"/>
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="72" spans="9:10" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I72">
-        <v>85</v>
+        <v>255</v>
       </c>
       <c r="J72">
         <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="73" spans="9:10" x14ac:dyDescent="0.25">
+        <v>12.525</v>
+      </c>
+    </row>
+    <row r="73" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I73">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="J73">
         <f t="shared" si="1"/>
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="74" spans="9:10" x14ac:dyDescent="0.25">
+        <v>13.05</v>
+      </c>
+    </row>
+    <row r="74" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I74">
-        <v>95</v>
+        <v>285</v>
       </c>
       <c r="J74">
         <f t="shared" si="1"/>
-        <v>4.8000000000000007</v>
-      </c>
-    </row>
-    <row r="75" spans="9:10" x14ac:dyDescent="0.25">
+        <v>13.575000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I75">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="J75">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="9:10" x14ac:dyDescent="0.25">
+        <v>14.100000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I76">
-        <v>105</v>
+        <v>315</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="77" spans="9:10" x14ac:dyDescent="0.25">
+        <v>14.625</v>
+      </c>
+    </row>
+    <row r="77" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I77">
-        <v>110</v>
+        <v>330</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="78" spans="9:10" x14ac:dyDescent="0.25">
+        <v>15.15</v>
+      </c>
+    </row>
+    <row r="78" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I78">
-        <v>115</v>
+        <v>345</v>
       </c>
       <c r="J78">
         <f t="shared" si="1"/>
-        <v>5.6000000000000005</v>
-      </c>
-    </row>
-    <row r="79" spans="9:10" x14ac:dyDescent="0.25">
+        <v>15.675000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I79">
-        <v>120</v>
+        <v>360</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="80" spans="9:10" x14ac:dyDescent="0.25">
+        <v>16.200000000000003</v>
+      </c>
+    </row>
+    <row r="80" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I80">
-        <v>125</v>
+        <v>375</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>16.725000000000001</v>
       </c>
     </row>
     <row r="81" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I81">
-        <v>130</v>
+        <v>390</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>6.2</v>
+        <v>17.250000000000004</v>
       </c>
     </row>
     <row r="82" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I82">
-        <v>135</v>
+        <v>405</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>6.4</v>
+        <v>17.775000000000002</v>
       </c>
     </row>
     <row r="83" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I83">
-        <v>140</v>
+        <v>420</v>
       </c>
       <c r="J83">
         <f t="shared" si="1"/>
-        <v>6.6000000000000005</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="84" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I84">
-        <v>145</v>
+        <v>435</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>6.8</v>
+        <v>18.825000000000003</v>
       </c>
     </row>
     <row r="85" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I85">
-        <v>150</v>
+        <v>450</v>
       </c>
       <c r="J85">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>19.350000000000001</v>
       </c>
     </row>
     <row r="86" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I86">
-        <v>155</v>
+        <v>465</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>7.2</v>
+        <v>19.875000000000004</v>
       </c>
     </row>
     <row r="87" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I87">
-        <v>160</v>
+        <v>480</v>
       </c>
       <c r="J87">
         <f t="shared" si="1"/>
-        <v>7.4</v>
+        <v>20.400000000000002</v>
       </c>
     </row>
     <row r="88" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I88">
-        <v>165</v>
+        <v>495</v>
       </c>
       <c r="J88">
         <f t="shared" si="1"/>
-        <v>7.6000000000000005</v>
+        <v>20.925000000000004</v>
       </c>
     </row>
     <row r="89" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I89">
-        <v>170</v>
+        <v>510</v>
       </c>
       <c r="J89">
         <f t="shared" si="1"/>
-        <v>7.8</v>
+        <v>21.450000000000003</v>
       </c>
     </row>
     <row r="90" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I90">
-        <v>175</v>
+        <v>525</v>
       </c>
       <c r="J90">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>21.975000000000001</v>
       </c>
     </row>
     <row r="91" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I91">
-        <v>180</v>
+        <v>540</v>
       </c>
       <c r="J91">
         <f t="shared" si="1"/>
-        <v>8.1999999999999993</v>
+        <v>22.500000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Line for Come Back notification added
Former-commit-id: e7cd6ab63c9be1a1fecb3c7d5243c0f25f4b521a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="289">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -918,6 +918,15 @@
   </si>
   <si>
     <t>DESIRED</t>
+  </si>
+  <si>
+    <t>sku.not.14</t>
+  </si>
+  <si>
+    <t>TID_NOTIFICATION_COME_BACK</t>
+  </si>
+  <si>
+    <t>Loyalty_ComeBack</t>
   </si>
 </sst>
 </file>
@@ -3312,7 +3321,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3338,7 +3346,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3660,7 +3668,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="246979392"/>
@@ -3719,7 +3727,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="249649184"/>
@@ -3760,7 +3768,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4137,7 +4145,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5682,10 +5690,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6465,9 +6473,11 @@
       <c r="C53" s="46" t="s">
         <v>269</v>
       </c>
-      <c r="D53" s="46"/>
+      <c r="D53" s="46" t="s">
+        <v>287</v>
+      </c>
       <c r="E53" s="46" t="s">
-        <v>260</v>
+        <v>288</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
@@ -6479,7 +6489,7 @@
       </c>
       <c r="D54" s="46"/>
       <c r="E54" s="46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -6491,7 +6501,7 @@
       </c>
       <c r="D55" s="46"/>
       <c r="E55" s="46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -6503,7 +6513,7 @@
       </c>
       <c r="D56" s="46"/>
       <c r="E56" s="46" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -6515,7 +6525,7 @@
       </c>
       <c r="D57" s="46"/>
       <c r="E57" s="46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -6527,7 +6537,7 @@
       </c>
       <c r="D58" s="46"/>
       <c r="E58" s="46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -6539,7 +6549,7 @@
       </c>
       <c r="D59" s="46"/>
       <c r="E59" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
@@ -6551,7 +6561,7 @@
       </c>
       <c r="D60" s="46"/>
       <c r="E60" s="46" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
@@ -6563,6 +6573,18 @@
       </c>
       <c r="D61" s="46"/>
       <c r="E61" s="46" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="46" t="s">
+        <v>286</v>
+      </c>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46" t="s">
         <v>268</v>
       </c>
     </row>
@@ -6571,7 +6593,7 @@
     <cfRule type="duplicateValues" dxfId="91" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 E53:E54 D53:D58 D17:D29"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 D17:D29 D53:D59 E54:E55"/>
     <dataValidation type="list" sqref="E34:E43">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
@@ -7705,7 +7727,7 @@
   </sheetPr>
   <dimension ref="F4:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Come Back notification line + Timer in content
Former-commit-id: 45b8a5b66b6e5ea26f4f77232d29f7884c88f216
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="290">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -927,6 +927,9 @@
   </si>
   <si>
     <t>Loyalty_ComeBack</t>
+  </si>
+  <si>
+    <t>[notificationComeBackTimer]</t>
   </si>
 </sst>
 </file>
@@ -1397,7 +1400,125 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="93">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2146,96 +2267,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3282,16 +3313,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5302,123 +5323,124 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88" totalsRowBorderDxfId="87">
-  <autoFilter ref="B4:Q5"/>
-  <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="86"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="85"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="84"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="83"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="82"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="81"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="80"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="79"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="78"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="77"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="76"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="74"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="73"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="72"/>
-    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:R5" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90" totalsRowBorderDxfId="89">
+  <autoFilter ref="B4:R5"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="88"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="86"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="85"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="84"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="83"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="82"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="81"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="80"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="79"/>
+    <tableColumn id="17" name="[notificationComeBackTimer]" dataDxfId="0"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="78"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="77"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="75"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="74"/>
+    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="70" headerRowBorderDxfId="69" tableBorderDxfId="68" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="66"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="64"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="63"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="62"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="61"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="68"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="67"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="66"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="65"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="64"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <autoFilter ref="B16:G29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="56"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
-    <tableColumn id="3" name="[active]" dataDxfId="54"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="53"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="52"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="51"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="58"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="57"/>
+    <tableColumn id="3" name="[active]" dataDxfId="56"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="55"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="54"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="52">
   <autoFilter ref="B33:G43"/>
   <sortState ref="B25:G35">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
-    <tableColumn id="4" name="[type]" dataDxfId="46"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="49"/>
+    <tableColumn id="4" name="[type]" dataDxfId="48"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="47"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="3" name="[order]" dataDxfId="28"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
-    <tableColumn id="11" name="[android]" dataDxfId="25"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="41"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="3" name="[order]" dataDxfId="39"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="38"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="37"/>
+    <tableColumn id="11" name="[android]" dataDxfId="36"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="35"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="34"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="33"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="32"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="31"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="25"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="23"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
-    <tableColumn id="2" name="[url]" dataDxfId="3"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="17"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="16"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="15"/>
+    <tableColumn id="2" name="[url]" dataDxfId="14"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="13"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="12"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5690,10 +5712,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5708,8 +5730,8 @@
     <col min="8" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
@@ -5723,7 +5745,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="12"/>
@@ -5738,7 +5760,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:17" ht="306" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="306" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -5770,25 +5792,28 @@
         <v>24</v>
       </c>
       <c r="L4" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -5820,26 +5845,29 @@
         <v>240</v>
       </c>
       <c r="L5" s="42">
+        <v>2880</v>
+      </c>
+      <c r="M5" s="42">
         <v>7.1428571428571426E-3</v>
       </c>
-      <c r="M5" s="42">
+      <c r="N5" s="42">
         <v>0.2</v>
       </c>
-      <c r="N5" s="42">
+      <c r="O5" s="42">
         <v>0.01</v>
       </c>
-      <c r="O5" s="42">
+      <c r="P5" s="42">
         <v>1.2</v>
       </c>
-      <c r="P5" s="42">
+      <c r="Q5" s="42">
         <v>2.5</v>
       </c>
-      <c r="Q5" s="42">
+      <c r="R5" s="42">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -5853,7 +5881,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="10" spans="1:17" ht="96.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="96.75" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -5873,7 +5901,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
@@ -5893,8 +5921,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
@@ -5908,7 +5936,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="16" spans="1:17" ht="104.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="104.25" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -6473,11 +6501,9 @@
       <c r="C53" s="46" t="s">
         <v>269</v>
       </c>
-      <c r="D53" s="46" t="s">
-        <v>287</v>
-      </c>
+      <c r="D53" s="46"/>
       <c r="E53" s="46" t="s">
-        <v>288</v>
+        <v>260</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
@@ -6489,7 +6515,7 @@
       </c>
       <c r="D54" s="46"/>
       <c r="E54" s="46" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -6501,7 +6527,7 @@
       </c>
       <c r="D55" s="46"/>
       <c r="E55" s="46" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -6513,7 +6539,7 @@
       </c>
       <c r="D56" s="46"/>
       <c r="E56" s="46" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -6525,7 +6551,7 @@
       </c>
       <c r="D57" s="46"/>
       <c r="E57" s="46" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -6537,7 +6563,7 @@
       </c>
       <c r="D58" s="46"/>
       <c r="E58" s="46" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -6549,7 +6575,7 @@
       </c>
       <c r="D59" s="46"/>
       <c r="E59" s="46" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
@@ -6561,7 +6587,7 @@
       </c>
       <c r="D60" s="46"/>
       <c r="E60" s="46" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
@@ -6573,7 +6599,7 @@
       </c>
       <c r="D61" s="46"/>
       <c r="E61" s="46" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
@@ -6583,17 +6609,19 @@
       <c r="C62" s="46" t="s">
         <v>286</v>
       </c>
-      <c r="D62" s="46"/>
+      <c r="D62" s="46" t="s">
+        <v>287</v>
+      </c>
       <c r="E62" s="46" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="91" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 D17:D29 D53:D59 E54:E55"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 D17:D29 D53:D59 D62 E53:E54"/>
     <dataValidation type="list" sqref="E34:E43">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
@@ -7675,31 +7703,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
New "source" column added in notificationsDefinitions content
Former-commit-id: 8272323165bc9ac5691488fcb3723f19791c3808
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="293">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -930,6 +930,15 @@
   </si>
   <si>
     <t>[notificationComeBackTimer]</t>
+  </si>
+  <si>
+    <t>[source]</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>server</t>
   </si>
 </sst>
 </file>
@@ -1402,124 +1411,6 @@
   </cellStyles>
   <dxfs count="93">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2267,6 +2158,96 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3008,6 +2989,24 @@
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
@@ -3313,6 +3312,16 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5323,124 +5332,124 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:R5" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90" totalsRowBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:R5" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="B4:R5"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="88"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="86"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="85"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="84"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="83"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="82"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="81"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="80"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="79"/>
-    <tableColumn id="17" name="[notificationComeBackTimer]" dataDxfId="0"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="78"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="77"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="75"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="74"/>
-    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="73"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="85"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="84"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="83"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="82"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="81"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="80"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="79"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="78"/>
+    <tableColumn id="17" name="[notificationComeBackTimer]" dataDxfId="77"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="76"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="74"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="73"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="72"/>
+    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70" totalsRowBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="70" headerRowBorderDxfId="69" tableBorderDxfId="68" totalsRowBorderDxfId="67">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="68"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="67"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="66"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="65"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="64"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="63"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="66"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="64"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="63"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="62"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
   <autoFilter ref="B16:G29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="58"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="57"/>
-    <tableColumn id="3" name="[active]" dataDxfId="56"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="55"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="54"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="53"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
+    <tableColumn id="3" name="[active]" dataDxfId="54"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="53"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="52"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="50">
   <autoFilter ref="B33:G43"/>
   <sortState ref="B25:G35">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="49"/>
-    <tableColumn id="4" name="[type]" dataDxfId="48"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="47"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="46"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
+    <tableColumn id="4" name="[type]" dataDxfId="46"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="41"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[order]" dataDxfId="39"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="38"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="37"/>
-    <tableColumn id="11" name="[android]" dataDxfId="36"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="35"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="34"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="33"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="32"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="31"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="30"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" name="[order]" dataDxfId="28"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
+    <tableColumn id="11" name="[android]" dataDxfId="25"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="25"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="23"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="22"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="17"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="16"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="15"/>
-    <tableColumn id="2" name="[url]" dataDxfId="14"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="13"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="12"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="11"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
+    <tableColumn id="2" name="[url]" dataDxfId="3"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5715,7 +5724,7 @@
   <dimension ref="A1:R62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6437,8 +6446,11 @@
       <c r="E48" s="49" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="49" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>3</v>
       </c>
@@ -6451,8 +6463,11 @@
       <c r="E49" s="46" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="46" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>3</v>
       </c>
@@ -6465,8 +6480,11 @@
       <c r="E50" s="46" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="46" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>3</v>
       </c>
@@ -6479,8 +6497,11 @@
       <c r="E51" s="46" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="46" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>3</v>
       </c>
@@ -6493,8 +6514,11 @@
       <c r="E52" s="46" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="46" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>3</v>
       </c>
@@ -6505,8 +6529,11 @@
       <c r="E53" s="46" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>3</v>
       </c>
@@ -6517,8 +6544,11 @@
       <c r="E54" s="46" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>3</v>
       </c>
@@ -6529,8 +6559,11 @@
       <c r="E55" s="46" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>3</v>
       </c>
@@ -6541,8 +6574,11 @@
       <c r="E56" s="46" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>3</v>
       </c>
@@ -6553,8 +6589,11 @@
       <c r="E57" s="46" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
         <v>3</v>
       </c>
@@ -6565,8 +6604,11 @@
       <c r="E58" s="46" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F58" s="46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>3</v>
       </c>
@@ -6577,8 +6619,11 @@
       <c r="E59" s="46" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>3</v>
       </c>
@@ -6589,8 +6634,11 @@
       <c r="E60" s="46" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F60" s="46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>3</v>
       </c>
@@ -6601,8 +6649,11 @@
       <c r="E61" s="46" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>3</v>
       </c>
@@ -6615,13 +6666,16 @@
       <c r="E62" s="46" t="s">
         <v>288</v>
       </c>
+      <c r="F62" s="46" t="s">
+        <v>291</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 D17:D29 D53:D59 D62 E53:E54"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 D17:D29 D53:D59 D62 E53:E54 F53:F61"/>
     <dataValidation type="list" sqref="E34:E43">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
@@ -7703,31 +7757,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="8" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G5:H16">

</xml_diff>

<commit_message>
Remove Golden Fragments reward and added rate conversion to Gems
Former-commit-id: 7b2022ba089ecbc7455811e76e21c6610421d93f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -563,9 +563,6 @@
     <t>[goldenFragments]</t>
   </si>
   <si>
-    <t>[goldenFragmentsGivenTutorial]</t>
-  </si>
-  <si>
     <t>chineseNewYear</t>
   </si>
   <si>
@@ -921,6 +918,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>[goldenFragmentsToHCCoef]</t>
   </si>
 </sst>
 </file>
@@ -3315,7 +3315,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5315,7 +5314,7 @@
     <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="74"/>
     <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="73"/>
     <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="72"/>
-    <tableColumn id="14" name="[goldenFragmentsGivenTutorial]" dataDxfId="71"/>
+    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5687,8 +5686,8 @@
   </sheetPr>
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5780,7 +5779,7 @@
         <v>19</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>167</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -5830,7 +5829,7 @@
         <v>2.5</v>
       </c>
       <c r="Q5" s="42">
-        <v>25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5920,7 +5919,7 @@
         <v>74</v>
       </c>
       <c r="G16" s="51" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -6000,16 +5999,16 @@
         <v>3</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D21" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F21" s="42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G21" s="42"/>
     </row>
@@ -6018,16 +6017,16 @@
         <v>3</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D22" s="41" t="b">
         <v>0</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F22" s="42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G22" s="40"/>
     </row>
@@ -6036,16 +6035,16 @@
         <v>3</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D23" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E23" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="42" t="s">
         <v>175</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>176</v>
       </c>
       <c r="G23" s="42"/>
     </row>
@@ -6054,16 +6053,16 @@
         <v>3</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D24" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E24" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" s="44" t="s">
         <v>178</v>
-      </c>
-      <c r="F24" s="44" t="s">
-        <v>179</v>
       </c>
       <c r="G24" s="42"/>
     </row>
@@ -6072,16 +6071,16 @@
         <v>3</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D25" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E25" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="F25" s="42" t="s">
         <v>230</v>
-      </c>
-      <c r="F25" s="42" t="s">
-        <v>231</v>
       </c>
       <c r="G25" s="42"/>
     </row>
@@ -6090,16 +6089,16 @@
         <v>3</v>
       </c>
       <c r="C26" s="52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D26" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E26" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="F26" s="44" t="s">
         <v>238</v>
-      </c>
-      <c r="F26" s="44" t="s">
-        <v>239</v>
       </c>
       <c r="G26" s="42"/>
     </row>
@@ -6108,16 +6107,16 @@
         <v>3</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D27" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G27" s="42"/>
     </row>
@@ -6126,16 +6125,16 @@
         <v>3</v>
       </c>
       <c r="C28" s="52" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D28" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E28" s="44" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F28" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G28" s="42"/>
     </row>
@@ -6144,19 +6143,19 @@
         <v>3</v>
       </c>
       <c r="C29" s="55" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D29" s="41" t="b">
         <v>0</v>
       </c>
       <c r="E29" s="44" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F29" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G29" s="55" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -6381,7 +6380,7 @@
     <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B46" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -6393,7 +6392,7 @@
     </row>
     <row r="48" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
       <c r="B48" s="47" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C48" s="48" t="s">
         <v>8</v>
@@ -6402,7 +6401,7 @@
         <v>74</v>
       </c>
       <c r="E48" s="49" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -6410,13 +6409,13 @@
         <v>3</v>
       </c>
       <c r="C49" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D49" s="46" t="s">
+        <v>251</v>
+      </c>
+      <c r="E49" s="46" t="s">
         <v>252</v>
-      </c>
-      <c r="E49" s="46" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
@@ -6424,13 +6423,13 @@
         <v>3</v>
       </c>
       <c r="C50" s="46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D50" s="46" t="s">
+        <v>253</v>
+      </c>
+      <c r="E50" s="46" t="s">
         <v>254</v>
-      </c>
-      <c r="E50" s="46" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -6438,13 +6437,13 @@
         <v>3</v>
       </c>
       <c r="C51" s="46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D51" s="46" t="s">
+        <v>255</v>
+      </c>
+      <c r="E51" s="46" t="s">
         <v>256</v>
-      </c>
-      <c r="E51" s="46" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
@@ -6452,13 +6451,13 @@
         <v>3</v>
       </c>
       <c r="C52" s="46" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D52" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="E52" s="46" t="s">
         <v>258</v>
-      </c>
-      <c r="E52" s="46" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
@@ -6466,11 +6465,11 @@
         <v>3</v>
       </c>
       <c r="C53" s="46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D53" s="46"/>
       <c r="E53" s="46" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
@@ -6478,11 +6477,11 @@
         <v>3</v>
       </c>
       <c r="C54" s="46" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D54" s="46"/>
       <c r="E54" s="46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -6490,11 +6489,11 @@
         <v>3</v>
       </c>
       <c r="C55" s="46" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D55" s="46"/>
       <c r="E55" s="46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -6502,11 +6501,11 @@
         <v>3</v>
       </c>
       <c r="C56" s="46" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D56" s="46"/>
       <c r="E56" s="46" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -6514,11 +6513,11 @@
         <v>3</v>
       </c>
       <c r="C57" s="46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D57" s="46"/>
       <c r="E57" s="46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -6526,11 +6525,11 @@
         <v>3</v>
       </c>
       <c r="C58" s="46" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D58" s="46"/>
       <c r="E58" s="46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -6538,11 +6537,11 @@
         <v>3</v>
       </c>
       <c r="C59" s="46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D59" s="46"/>
       <c r="E59" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
@@ -6550,11 +6549,11 @@
         <v>3</v>
       </c>
       <c r="C60" s="46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D60" s="46"/>
       <c r="E60" s="46" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
@@ -6562,11 +6561,11 @@
         <v>3</v>
       </c>
       <c r="C61" s="46" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D61" s="46"/>
       <c r="E61" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -6670,7 +6669,7 @@
         <v>6</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L4" s="24" t="s">
         <v>99</v>
@@ -6708,7 +6707,7 @@
         <v>70</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>89</v>
@@ -6746,7 +6745,7 @@
         <v>66</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L6" s="15" t="s">
         <v>89</v>
@@ -6784,7 +6783,7 @@
         <v>62</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L7" s="15" t="s">
         <v>89</v>
@@ -6822,7 +6821,7 @@
         <v>58</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>89</v>
@@ -6860,7 +6859,7 @@
         <v>54</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>89</v>
@@ -6898,7 +6897,7 @@
         <v>50</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L10" s="15" t="s">
         <v>89</v>
@@ -6936,7 +6935,7 @@
         <v>46</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L11" s="15" t="s">
         <v>89</v>
@@ -6974,7 +6973,7 @@
         <v>43</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L12" s="15" t="s">
         <v>90</v>
@@ -7012,7 +7011,7 @@
         <v>39</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L13" s="15" t="s">
         <v>92</v>
@@ -7050,7 +7049,7 @@
         <v>35</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L14" s="15" t="s">
         <v>93</v>
@@ -7088,7 +7087,7 @@
         <v>98</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L15" s="16" t="s">
         <v>91</v>
@@ -7126,7 +7125,7 @@
         <v>113</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L16" s="16" t="s">
         <v>114</v>
@@ -7252,7 +7251,7 @@
     <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B32" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -7265,25 +7264,25 @@
     </row>
     <row r="34" spans="2:8" ht="129.75" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D34" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="E34" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="F34" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="F34" s="30" t="s">
+      <c r="G34" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="G34" s="30" t="s">
+      <c r="H34" s="30" t="s">
         <v>189</v>
-      </c>
-      <c r="H34" s="30" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -7291,22 +7290,22 @@
         <v>3</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E35" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="F35" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="F35" s="29" t="s">
+      <c r="G35" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="G35" s="29" t="s">
-        <v>211</v>
-      </c>
       <c r="H35" s="29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -7314,22 +7313,22 @@
         <v>3</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E36" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F36" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F36" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G36" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -7337,22 +7336,22 @@
         <v>3</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E37" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F37" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="G37" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="G37" s="17" t="s">
-        <v>211</v>
-      </c>
       <c r="H37" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -7360,22 +7359,22 @@
         <v>3</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E38" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F38" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F38" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G38" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
@@ -7383,22 +7382,22 @@
         <v>3</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E39" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="F39" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="F39" s="21" t="s">
-        <v>210</v>
-      </c>
       <c r="G39" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
@@ -7406,22 +7405,22 @@
         <v>3</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E40" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F40" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F40" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G40" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
@@ -7429,22 +7428,22 @@
         <v>3</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D41" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E41" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="F41" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F41" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G41" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -7452,22 +7451,22 @@
         <v>3</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E42" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F42" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F42" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G42" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -7475,22 +7474,22 @@
         <v>3</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E43" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F43" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G43" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
@@ -7498,22 +7497,22 @@
         <v>3</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E44" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F44" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F44" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G44" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -7521,22 +7520,22 @@
         <v>3</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E45" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F45" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F45" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G45" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
@@ -7544,22 +7543,22 @@
         <v>3</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E46" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F46" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F46" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G46" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
@@ -7567,22 +7566,22 @@
         <v>3</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E47" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F47" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F47" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G47" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -7590,22 +7589,22 @@
         <v>3</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E48" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F48" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F48" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G48" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -7613,22 +7612,22 @@
         <v>3</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D49" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E49" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="F49" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="F49" s="17" t="s">
-        <v>210</v>
-      </c>
       <c r="G49" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
@@ -7636,22 +7635,22 @@
         <v>3</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E50" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="F50" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="F50" s="29" t="s">
+      <c r="G50" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="G50" s="29" t="s">
-        <v>211</v>
-      </c>
       <c r="H50" s="29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -7724,7 +7723,7 @@
     </row>
     <row r="8" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G8">
         <v>0.08</v>
@@ -7732,7 +7731,7 @@
     </row>
     <row r="9" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -7740,10 +7739,10 @@
     </row>
     <row r="12" spans="6:10" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="6:10" x14ac:dyDescent="0.25">
@@ -8072,7 +8071,7 @@
     </row>
     <row r="50" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="51" spans="6:17" x14ac:dyDescent="0.25">
@@ -8092,7 +8091,7 @@
     </row>
     <row r="53" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G53">
         <v>3.5000000000000003E-2</v>
@@ -8100,7 +8099,7 @@
     </row>
     <row r="54" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G54">
         <v>3.6</v>
@@ -8108,15 +8107,15 @@
     </row>
     <row r="55" spans="6:17" x14ac:dyDescent="0.25">
       <c r="I55" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J55" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="56" spans="6:17" x14ac:dyDescent="0.25">
       <c r="H56" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I56">
         <v>15</v>
@@ -8146,7 +8145,7 @@
     </row>
     <row r="59" spans="6:17" x14ac:dyDescent="0.25">
       <c r="H59" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I59">
         <v>60</v>
@@ -8257,7 +8256,7 @@
     </row>
     <row r="71" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H71" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I71">
         <v>240</v>

</xml_diff>

<commit_message>
Halloween activated by default
Former-commit-id: a980fa3d6fbb61843e25c04f8d9767f6b0803091
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3358,7 +3358,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3680,7 +3680,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="246979392"/>
@@ -3739,7 +3739,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="249649184"/>
@@ -3780,7 +3780,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4157,7 +4157,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5704,8 +5704,8 @@
   </sheetPr>
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5966,7 +5966,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Activating XMas season, deactivating Halloween season
Former-commit-id: fac575d3f233943f88efc496bfa30c937466ee0a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
     <sheet name="tech" sheetId="3" r:id="rId2"/>
     <sheet name="TimeCost" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3332,7 +3332,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5704,8 +5703,8 @@
   </sheetPr>
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5948,7 +5947,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>4</v>
@@ -5966,7 +5965,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>1</v>
@@ -6674,7 +6673,7 @@
   </sheetPr>
   <dimension ref="B1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="101" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="101" workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added local notification in content for the free reward in the shop
Former-commit-id: c4a3d1105c3b53e84c9ced13548fd0de7a7ab356
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="296">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -939,6 +939,15 @@
   </si>
   <si>
     <t>Loyalty_ComeBack</t>
+  </si>
+  <si>
+    <t>sku.not.15</t>
+  </si>
+  <si>
+    <t>TID_NOTIFICATION_FREE_DAILY_REWARD</t>
+  </si>
+  <si>
+    <t>Loyalty_ShopReward</t>
   </si>
 </sst>
 </file>
@@ -3357,7 +3366,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3679,7 +3688,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="246979392"/>
@@ -3738,7 +3747,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="249649184"/>
@@ -3779,7 +3788,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4156,7 +4165,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5701,10 +5710,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6641,6 +6650,23 @@
         <v>292</v>
       </c>
       <c r="F62" s="46" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="D63" s="46" t="s">
+        <v>294</v>
+      </c>
+      <c r="E63" s="46" t="s">
+        <v>295</v>
+      </c>
+      <c r="F63" s="46" t="s">
         <v>288</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new column for pills FX
Former-commit-id: de4eb073bb56392070f8b85b826273c913ece6d5
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="299">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -948,6 +948,15 @@
   </si>
   <si>
     <t>Loyalty_ShopReward</t>
+  </si>
+  <si>
+    <t>[pillParticles]</t>
+  </si>
+  <si>
+    <t>PS_Xmas</t>
+  </si>
+  <si>
+    <t>PS_Bats</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1426,23 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="93">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3366,7 +3391,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3688,7 +3713,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="246979392"/>
@@ -3747,7 +3772,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="249649184"/>
@@ -3788,7 +3813,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4165,7 +4190,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5322,123 +5347,124 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88" totalsRowBorderDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="B4:Q5"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="86"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="85"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="84"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="83"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="82"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="81"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="80"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="79"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="78"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="77"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="76"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="74"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="73"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="72"/>
-    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="71"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="85"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="84"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="83"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="82"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="81"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="80"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="79"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="78"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="77"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="74"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="73"/>
+    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="70" headerRowBorderDxfId="69" tableBorderDxfId="68" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="66"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="64"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="63"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="62"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="61"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="67"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="65"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="64"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="63"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
-  <autoFilter ref="B16:G29"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="56"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
-    <tableColumn id="3" name="[active]" dataDxfId="54"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="53"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="52"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:H29" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+  <autoFilter ref="B16:H29"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="56"/>
+    <tableColumn id="3" name="[active]" dataDxfId="55"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="54"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="53"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="52"/>
+    <tableColumn id="7" name="[pillParticles]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="51">
   <autoFilter ref="B33:G43"/>
   <sortState ref="B25:G35">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
-    <tableColumn id="4" name="[type]" dataDxfId="46"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="48"/>
+    <tableColumn id="4" name="[type]" dataDxfId="47"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="46"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="3" name="[order]" dataDxfId="28"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
-    <tableColumn id="11" name="[android]" dataDxfId="25"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="31"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="30"/>
+    <tableColumn id="3" name="[order]" dataDxfId="29"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="28"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="27"/>
+    <tableColumn id="11" name="[android]" dataDxfId="26"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="25"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="24"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="23"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="22"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="15"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="13"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
-    <tableColumn id="2" name="[url]" dataDxfId="3"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="7"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="6"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="5"/>
+    <tableColumn id="2" name="[url]" dataDxfId="4"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="3"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5712,8 +5738,8 @@
   </sheetPr>
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5947,8 +5973,11 @@
       <c r="G16" s="51" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="51" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -5956,7 +5985,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>4</v>
@@ -5965,8 +5994,11 @@
         <v>83</v>
       </c>
       <c r="G17" s="50"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="50" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
@@ -5983,8 +6015,11 @@
         <v>84</v>
       </c>
       <c r="G18" s="42"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="42" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="31" t="s">
         <v>3</v>
       </c>
@@ -6001,8 +6036,9 @@
         <v>109</v>
       </c>
       <c r="G19" s="42"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="42"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="39" t="s">
         <v>3</v>
       </c>
@@ -6019,8 +6055,9 @@
         <v>153</v>
       </c>
       <c r="G20" s="42"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="42"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="31" t="s">
         <v>3</v>
       </c>
@@ -6037,8 +6074,9 @@
         <v>171</v>
       </c>
       <c r="G21" s="42"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="42"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="39" t="s">
         <v>3</v>
       </c>
@@ -6055,8 +6093,9 @@
         <v>172</v>
       </c>
       <c r="G22" s="40"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="40"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="52" t="s">
         <v>3</v>
       </c>
@@ -6073,8 +6112,9 @@
         <v>175</v>
       </c>
       <c r="G23" s="50"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="50"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="52" t="s">
         <v>3</v>
       </c>
@@ -6091,8 +6131,9 @@
         <v>178</v>
       </c>
       <c r="G24" s="42"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="42"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="52" t="s">
         <v>3</v>
       </c>
@@ -6109,8 +6150,9 @@
         <v>230</v>
       </c>
       <c r="G25" s="42"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="42"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="52" t="s">
         <v>3</v>
       </c>
@@ -6127,8 +6169,9 @@
         <v>238</v>
       </c>
       <c r="G26" s="42"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="42"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="52" t="s">
         <v>3</v>
       </c>
@@ -6145,8 +6188,9 @@
         <v>239</v>
       </c>
       <c r="G27" s="42"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="42"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="52" t="s">
         <v>3</v>
       </c>
@@ -6163,8 +6207,9 @@
         <v>240</v>
       </c>
       <c r="G28" s="40"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="40"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="53" t="s">
         <v>3</v>
       </c>
@@ -6183,9 +6228,10 @@
       <c r="G29" s="54" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="H29" s="54"/>
+    </row>
+    <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B31" s="7" t="s">
         <v>117</v>
       </c>
@@ -6672,7 +6718,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="91" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 E53:E54 D53:D58 D17:D29"/>
@@ -7757,31 +7803,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="L5:L16">

</xml_diff>

<commit_message>
upgrade map doesn't last the same if upgraded with Gems or with Ads
Former-commit-id: 4d4079b7a78791634b02c2519164f96aae22e2fc
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="297">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -948,6 +948,9 @@
   </si>
   <si>
     <t>Loyalty_ShopReward</t>
+  </si>
+  <si>
+    <t>[miniMapTimerAd]</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1413,11 +1416,130 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="93">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2166,96 +2288,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3302,16 +3334,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5322,123 +5344,124 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88" totalsRowBorderDxfId="87">
-  <autoFilter ref="B4:Q5"/>
-  <tableColumns count="16">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="86"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="85"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="84"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="83"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="82"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="81"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="80"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="79"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="78"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="77"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="76"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="74"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="73"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="72"/>
-    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:R5" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90" totalsRowBorderDxfId="89">
+  <autoFilter ref="B4:R5"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="88"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="86"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="85"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="84"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="83"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="82"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="81"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="80"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="79"/>
+    <tableColumn id="17" name="[miniMapTimerAd]" dataDxfId="0"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="78"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="77"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="75"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="74"/>
+    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="70" headerRowBorderDxfId="69" tableBorderDxfId="68" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="66"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="64"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="63"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="62"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="61"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="68"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="67"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="66"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="65"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="64"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <autoFilter ref="B16:G29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="56"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
-    <tableColumn id="3" name="[active]" dataDxfId="54"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="53"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="52"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="51"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="58"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="57"/>
+    <tableColumn id="3" name="[active]" dataDxfId="56"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="55"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="54"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="52">
   <autoFilter ref="B33:G43"/>
   <sortState ref="B25:G35">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
-    <tableColumn id="4" name="[type]" dataDxfId="46"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="49"/>
+    <tableColumn id="4" name="[type]" dataDxfId="48"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="47"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="3" name="[order]" dataDxfId="28"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
-    <tableColumn id="11" name="[android]" dataDxfId="25"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="41"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="3" name="[order]" dataDxfId="39"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="38"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="37"/>
+    <tableColumn id="11" name="[android]" dataDxfId="36"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="35"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="34"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="33"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="32"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="31"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="25"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="23"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
-    <tableColumn id="2" name="[url]" dataDxfId="3"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="17"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="16"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="15"/>
+    <tableColumn id="2" name="[url]" dataDxfId="14"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="13"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="12"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5710,10 +5733,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:Q63"/>
+  <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5725,11 +5748,11 @@
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="26" width="12" customWidth="1"/>
+    <col min="8" max="27" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
@@ -5742,8 +5765,9 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L2" s="55"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="12"/>
@@ -5757,8 +5781,9 @@
       <c r="I3" s="11"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
-    </row>
-    <row r="4" spans="1:17" ht="306" x14ac:dyDescent="0.25">
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="1:18" ht="306" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -5790,25 +5815,28 @@
         <v>24</v>
       </c>
       <c r="L4" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -5840,26 +5868,29 @@
         <v>240</v>
       </c>
       <c r="L5" s="42">
+        <v>20</v>
+      </c>
+      <c r="M5" s="42">
         <v>7.1428571428571426E-3</v>
       </c>
-      <c r="M5" s="42">
+      <c r="N5" s="42">
         <v>0.2</v>
       </c>
-      <c r="N5" s="42">
+      <c r="O5" s="42">
         <v>0.01</v>
       </c>
-      <c r="O5" s="42">
+      <c r="P5" s="42">
         <v>1.2</v>
       </c>
-      <c r="P5" s="42">
+      <c r="Q5" s="42">
         <v>2.5</v>
       </c>
-      <c r="Q5" s="42">
+      <c r="R5" s="42">
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -5872,8 +5903,9 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-    </row>
-    <row r="10" spans="1:17" ht="96.75" x14ac:dyDescent="0.25">
+      <c r="L8" s="55"/>
+    </row>
+    <row r="10" spans="1:18" ht="96.75" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -5893,7 +5925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
@@ -5913,8 +5945,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
@@ -5927,8 +5959,9 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
-    </row>
-    <row r="16" spans="1:17" ht="104.25" x14ac:dyDescent="0.25">
+      <c r="L14" s="55"/>
+    </row>
+    <row r="16" spans="1:18" ht="104.25" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -6672,7 +6705,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="91" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 E53:E54 D53:D58 D17:D29"/>
@@ -7757,31 +7790,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="L5:L16">

</xml_diff>

<commit_message>
Adding table to set values for No Ads feature
Former-commit-id: d4e4cef12bec61c68b28fd07f0c58fef8f88019f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="311">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -951,6 +951,48 @@
   </si>
   <si>
     <t>[miniMapTimerAd]</t>
+  </si>
+  <si>
+    <t>NO ADS CONFIG</t>
+  </si>
+  <si>
+    <t>{removeAdsOfferDefinitions}</t>
+  </si>
+  <si>
+    <t>remove_ads_offer</t>
+  </si>
+  <si>
+    <t>[easyExtraMissions]</t>
+  </si>
+  <si>
+    <t>[mediumExtraMissions]</t>
+  </si>
+  <si>
+    <t>[hardExtraMissions]</t>
+  </si>
+  <si>
+    <t>[easyMissionCooldownMultiplier]</t>
+  </si>
+  <si>
+    <t>[mediumMissionCooldownMultiplier]</t>
+  </si>
+  <si>
+    <t>[hardMissionCooldownMultiplier]</t>
+  </si>
+  <si>
+    <t>[mapRevealDurationSecs]</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>[mapRevealCooldownSecs]</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>[freeRevives]</t>
   </si>
 </sst>
 </file>
@@ -1314,7 +1356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1417,29 +1459,14 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="93">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3024,6 +3051,24 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -5357,111 +5402,111 @@
     <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="81"/>
     <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="80"/>
     <tableColumn id="8" name="[miniMapTimer]" dataDxfId="79"/>
-    <tableColumn id="17" name="[miniMapTimerAd]" dataDxfId="0"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="78"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="77"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="75"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="74"/>
-    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="73"/>
+    <tableColumn id="17" name="[miniMapTimerAd]" dataDxfId="78"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="77"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="74"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="73"/>
+    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70" totalsRowBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="68"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="67"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="66"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="65"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="64"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="63"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="67"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="65"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="64"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="63"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:G29" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
   <autoFilter ref="B16:G29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="58"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="57"/>
-    <tableColumn id="3" name="[active]" dataDxfId="56"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="55"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="54"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="53"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="56"/>
+    <tableColumn id="3" name="[active]" dataDxfId="55"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="54"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="53"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="51">
   <autoFilter ref="B33:G43"/>
   <sortState ref="B25:G35">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="49"/>
-    <tableColumn id="4" name="[type]" dataDxfId="48"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="47"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="46"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="48"/>
+    <tableColumn id="4" name="[type]" dataDxfId="47"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="46"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="41"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[order]" dataDxfId="39"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="38"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="37"/>
-    <tableColumn id="11" name="[android]" dataDxfId="36"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="35"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="34"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="33"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="32"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="31"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="30"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="40"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="3" name="[order]" dataDxfId="38"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="37"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="36"/>
+    <tableColumn id="11" name="[android]" dataDxfId="35"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="34"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="33"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="32"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="31"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="30"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="25"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="23"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="22"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="24"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="22"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="17"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="16"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="15"/>
-    <tableColumn id="2" name="[url]" dataDxfId="14"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="13"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="12"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="11"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="16"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="15"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="14"/>
+    <tableColumn id="2" name="[url]" dataDxfId="13"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="12"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="11"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5733,10 +5778,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:R63"/>
+  <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="L79" sqref="L79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6703,9 +6748,110 @@
         <v>288</v>
       </c>
     </row>
+    <row r="65" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B66" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" ht="176.25" x14ac:dyDescent="0.25">
+      <c r="B68" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="C68" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="49" t="s">
+        <v>300</v>
+      </c>
+      <c r="E68" s="49" t="s">
+        <v>301</v>
+      </c>
+      <c r="F68" s="49" t="s">
+        <v>302</v>
+      </c>
+      <c r="G68" s="56" t="s">
+        <v>303</v>
+      </c>
+      <c r="H68" s="56" t="s">
+        <v>304</v>
+      </c>
+      <c r="I68" s="56" t="s">
+        <v>305</v>
+      </c>
+      <c r="J68" s="56" t="s">
+        <v>306</v>
+      </c>
+      <c r="K68" s="56" t="s">
+        <v>308</v>
+      </c>
+      <c r="L68" s="56" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="46" t="s">
+        <v>299</v>
+      </c>
+      <c r="D69" s="46">
+        <v>2</v>
+      </c>
+      <c r="E69" s="46">
+        <v>1</v>
+      </c>
+      <c r="F69" s="46">
+        <v>1</v>
+      </c>
+      <c r="G69" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="H69" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="I69" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="J69" s="46">
+        <v>14400</v>
+      </c>
+      <c r="K69" s="46">
+        <v>86400</v>
+      </c>
+      <c r="L69" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>307</v>
+      </c>
+      <c r="K71" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J74">
+        <f>3600*4</f>
+        <v>14400</v>
+      </c>
+      <c r="K74">
+        <f>3600*24</f>
+        <v>86400</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 E53:E54 D53:D58 D17:D29"/>
@@ -7790,31 +7936,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="8" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="L5:L16">

</xml_diff>

<commit_message>
Adding particles for CNY and St. Valentine
Former-commit-id: c2557e77bda03a5a42d9a14af94c7590dc0f770e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="316">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1002,6 +1002,12 @@
   </si>
   <si>
     <t>1d</t>
+  </si>
+  <si>
+    <t>PS_Hearts</t>
+  </si>
+  <si>
+    <t>PS_Sparkles</t>
   </si>
 </sst>
 </file>
@@ -1476,124 +1482,6 @@
   </cellStyles>
   <dxfs count="94">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2341,6 +2229,96 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3098,6 +3076,24 @@
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
@@ -3403,6 +3399,16 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5413,125 +5419,125 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:R5" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:R5" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90" totalsRowBorderDxfId="89">
   <autoFilter ref="B4:R5"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="89"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="87"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="86"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="85"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="84"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="83"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="82"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="81"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="80"/>
-    <tableColumn id="17" name="[miniMapTimerAd]" dataDxfId="0"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="79"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="78"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="77"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="76"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="75"/>
-    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="74"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="88"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="86"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="85"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="84"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="83"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="82"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="81"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="80"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="79"/>
+    <tableColumn id="17" name="[miniMapTimerAd]" dataDxfId="78"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="77"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="74"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="73"/>
+    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="73" headerRowBorderDxfId="72" tableBorderDxfId="71" totalsRowBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="gameSettings21" displayName="gameSettings21" ref="B10:G11" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="69"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="68"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="67"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="66"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="65"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="64"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="67"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="65"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="64"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="63"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:H29" totalsRowShown="0" headerRowDxfId="63" headerRowBorderDxfId="62" tableBorderDxfId="61" totalsRowBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="gameSettings2114" displayName="gameSettings2114" ref="B16:H29" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
   <autoFilter ref="B16:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="59"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="58"/>
-    <tableColumn id="3" name="[active]" dataDxfId="57"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="56"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="55"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="54"/>
-    <tableColumn id="7" name="[pillParticles]" dataDxfId="53"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="56"/>
+    <tableColumn id="3" name="[active]" dataDxfId="55"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="54"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="53"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="52"/>
+    <tableColumn id="7" name="[pillParticles]" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="preRegRewardsDefinitions" displayName="preRegRewardsDefinitions" ref="B33:G43" totalsRowShown="0" headerRowDxfId="50">
   <autoFilter ref="B33:G43"/>
   <sortState ref="B25:G35">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="49"/>
-    <tableColumn id="4" name="[type]" dataDxfId="48"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="47"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="46"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
+    <tableColumn id="4" name="[type]" dataDxfId="46"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="41"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[order]" dataDxfId="39"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="38"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="37"/>
-    <tableColumn id="11" name="[android]" dataDxfId="36"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="35"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="34"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="33"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="32"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="31"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="30"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" name="[order]" dataDxfId="28"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
+    <tableColumn id="11" name="[android]" dataDxfId="25"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="25"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="23"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="22"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="17"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="16"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="15"/>
-    <tableColumn id="2" name="[url]" dataDxfId="14"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="13"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="12"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="11"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
+    <tableColumn id="2" name="[url]" dataDxfId="3"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5805,8 +5811,8 @@
   </sheetPr>
   <dimension ref="A1:R73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6147,7 +6153,9 @@
         <v>171</v>
       </c>
       <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="H21" s="42" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="39" t="s">
@@ -6166,7 +6174,9 @@
         <v>172</v>
       </c>
       <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
+      <c r="H22" s="40" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="52" t="s">
@@ -6892,7 +6902,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D34:D43 D11:F11 E53:E54 D53:D58 D17:D29"/>
@@ -7977,31 +7987,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="8" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="L5:L16">

</xml_diff>

<commit_message>
added pf and Sp for xmaspresent_mod Added bundle
Former-commit-id: b5871f2ccbcd6f84b80080ee81d1d508ccba16e0
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="338">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1065,6 +1065,15 @@
   </si>
   <si>
     <t>jalapeño</t>
+  </si>
+  <si>
+    <t>Anniversary_No_Equip</t>
+  </si>
+  <si>
+    <t>icon_season_anniversary_no_equip</t>
+  </si>
+  <si>
+    <t>TID_SEASON_ANNNIVERSARY_NO_EQUIP_NAME</t>
   </si>
 </sst>
 </file>
@@ -1421,7 +1430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1521,6 +1530,7 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5505,8 +5515,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H36" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
-  <autoFilter ref="B16:H36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H37" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+  <autoFilter ref="B16:H37"/>
   <tableColumns count="7">
     <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="58"/>
     <tableColumn id="2" name="[sku]" dataDxfId="57"/>
@@ -5521,8 +5531,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B40:G50" totalsRowShown="0" headerRowDxfId="51">
-  <autoFilter ref="B40:G50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B41:G51" totalsRowShown="0" headerRowDxfId="51">
+  <autoFilter ref="B41:G51"/>
   <sortState ref="B34:G44">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
@@ -5854,10 +5864,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:R80"/>
+  <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6495,57 +6505,56 @@
       <c r="G36" s="39"/>
       <c r="H36" s="39"/>
     </row>
-    <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B38" s="7" t="s">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="D37" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>336</v>
+      </c>
+      <c r="F37" s="37" t="s">
+        <v>337</v>
+      </c>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+    </row>
+    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B39" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" t="s">
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="138" x14ac:dyDescent="0.25">
-      <c r="B40" s="31" t="s">
+    <row r="41" spans="2:8" ht="138" x14ac:dyDescent="0.25">
+      <c r="B41" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C41" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="33" t="s">
+      <c r="D41" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="E40" s="34" t="s">
+      <c r="E41" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="F40" s="34" t="s">
+      <c r="F41" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="G40" s="35" t="s">
+      <c r="G41" s="35" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D41" s="36">
-        <v>3000000</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="F41" s="18">
-        <v>1</v>
-      </c>
-      <c r="G41" s="18" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -6553,104 +6562,106 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D42" s="36">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F42" s="18">
-        <v>5</v>
-      </c>
-      <c r="G42" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D43" s="36">
-        <v>2000000</v>
+        <v>2500000</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F43" s="18">
-        <v>1</v>
-      </c>
-      <c r="G43" s="18" t="s">
-        <v>140</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G43" s="18"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D44" s="36">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F44" s="18">
-        <v>5</v>
-      </c>
-      <c r="G44" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D45" s="36">
-        <v>1000000</v>
+        <v>1500000</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F45" s="18">
-        <v>1</v>
-      </c>
-      <c r="G45" s="18" t="s">
-        <v>139</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G45" s="18"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D46" s="36">
-        <v>500000</v>
+        <v>1000000</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F46" s="18">
-        <v>5</v>
-      </c>
-      <c r="G46" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D47" s="36">
-        <v>250000</v>
+        <v>500000</v>
       </c>
       <c r="E47" s="18" t="s">
         <v>134</v>
@@ -6665,16 +6676,16 @@
         <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D48" s="36">
-        <v>100000</v>
+        <v>250000</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="F48" s="18">
-        <v>1500</v>
+        <v>5</v>
       </c>
       <c r="G48" s="18"/>
     </row>
@@ -6683,16 +6694,16 @@
         <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D49" s="36">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="E49" s="18" t="s">
         <v>123</v>
       </c>
       <c r="F49" s="18">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="G49" s="18"/>
     </row>
@@ -6701,64 +6712,65 @@
         <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D50" s="36">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>123</v>
       </c>
       <c r="F50" s="18">
+        <v>500</v>
+      </c>
+      <c r="G50" s="18"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" s="36">
+        <v>10000</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F51" s="18">
         <v>100</v>
       </c>
-      <c r="G50" s="18"/>
-    </row>
-    <row r="52" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B53" s="7" t="s">
+      <c r="G51" s="18"/>
+    </row>
+    <row r="53" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B54" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" t="s">
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
-      <c r="B55" s="44" t="s">
+    <row r="56" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
+      <c r="B56" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="C55" s="45" t="s">
+      <c r="C56" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="46" t="s">
+      <c r="D56" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E55" s="46" t="s">
+      <c r="E56" s="46" t="s">
         <v>250</v>
       </c>
-      <c r="F55" s="46" t="s">
+      <c r="F56" s="46" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" s="43" t="s">
-        <v>246</v>
-      </c>
-      <c r="D56" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="E56" s="43" t="s">
-        <v>252</v>
-      </c>
-      <c r="F56" s="43" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
@@ -6766,13 +6778,13 @@
         <v>3</v>
       </c>
       <c r="C57" s="43" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D57" s="43" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F57" s="43" t="s">
         <v>288</v>
@@ -6783,13 +6795,13 @@
         <v>3</v>
       </c>
       <c r="C58" s="43" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E58" s="43" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F58" s="43" t="s">
         <v>288</v>
@@ -6800,13 +6812,13 @@
         <v>3</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D59" s="43" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E59" s="43" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F59" s="43" t="s">
         <v>288</v>
@@ -6817,14 +6829,16 @@
         <v>3</v>
       </c>
       <c r="C60" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="D60" s="43"/>
+        <v>249</v>
+      </c>
+      <c r="D60" s="43" t="s">
+        <v>257</v>
+      </c>
       <c r="E60" s="43" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F60" s="43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
@@ -6832,11 +6846,11 @@
         <v>3</v>
       </c>
       <c r="C61" s="43" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D61" s="43"/>
       <c r="E61" s="43" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F61" s="43" t="s">
         <v>289</v>
@@ -6847,11 +6861,11 @@
         <v>3</v>
       </c>
       <c r="C62" s="43" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D62" s="43"/>
       <c r="E62" s="43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F62" s="43" t="s">
         <v>289</v>
@@ -6862,11 +6876,11 @@
         <v>3</v>
       </c>
       <c r="C63" s="43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D63" s="43"/>
       <c r="E63" s="43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F63" s="43" t="s">
         <v>289</v>
@@ -6877,11 +6891,11 @@
         <v>3</v>
       </c>
       <c r="C64" s="43" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D64" s="43"/>
       <c r="E64" s="43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F64" s="43" t="s">
         <v>289</v>
@@ -6892,11 +6906,11 @@
         <v>3</v>
       </c>
       <c r="C65" s="43" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D65" s="43"/>
       <c r="E65" s="43" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F65" s="43" t="s">
         <v>289</v>
@@ -6907,11 +6921,11 @@
         <v>3</v>
       </c>
       <c r="C66" s="43" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D66" s="43"/>
       <c r="E66" s="43" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F66" s="43" t="s">
         <v>289</v>
@@ -6922,11 +6936,11 @@
         <v>3</v>
       </c>
       <c r="C67" s="43" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D67" s="43"/>
       <c r="E67" s="43" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F67" s="43" t="s">
         <v>289</v>
@@ -6937,11 +6951,11 @@
         <v>3</v>
       </c>
       <c r="C68" s="43" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D68" s="43"/>
       <c r="E68" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F68" s="43" t="s">
         <v>289</v>
@@ -6952,16 +6966,14 @@
         <v>3</v>
       </c>
       <c r="C69" s="43" t="s">
-        <v>290</v>
-      </c>
-      <c r="D69" s="43" t="s">
-        <v>291</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="D69" s="43"/>
       <c r="E69" s="43" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="F69" s="43" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.25">
@@ -6969,115 +6981,132 @@
         <v>3</v>
       </c>
       <c r="C70" s="43" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D70" s="43" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E70" s="43" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F70" s="43" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="71" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B72" s="7" t="s">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B71" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="43" t="s">
+        <v>293</v>
+      </c>
+      <c r="D71" s="43" t="s">
+        <v>294</v>
+      </c>
+      <c r="E71" s="43" t="s">
+        <v>295</v>
+      </c>
+      <c r="F71" s="43" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B73" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" t="s">
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:12" ht="176.25" x14ac:dyDescent="0.25">
-      <c r="B74" s="44" t="s">
+    <row r="75" spans="2:12" ht="176.25" x14ac:dyDescent="0.25">
+      <c r="B75" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="C74" s="45" t="s">
+      <c r="C75" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D74" s="46" t="s">
+      <c r="D75" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="E74" s="46" t="s">
+      <c r="E75" s="46" t="s">
         <v>303</v>
       </c>
-      <c r="F74" s="46" t="s">
+      <c r="F75" s="46" t="s">
         <v>304</v>
       </c>
-      <c r="G74" s="51" t="s">
+      <c r="G75" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="H74" s="51" t="s">
+      <c r="H75" s="51" t="s">
         <v>306</v>
       </c>
-      <c r="I74" s="51" t="s">
+      <c r="I75" s="51" t="s">
         <v>307</v>
       </c>
-      <c r="J74" s="51" t="s">
+      <c r="J75" s="51" t="s">
         <v>308</v>
       </c>
-      <c r="K74" s="51" t="s">
+      <c r="K75" s="51" t="s">
         <v>309</v>
       </c>
-      <c r="L74" s="51" t="s">
+      <c r="L75" s="51" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B75" s="3" t="s">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C75" s="43" t="s">
+      <c r="C76" s="43" t="s">
         <v>311</v>
       </c>
-      <c r="D75" s="43">
+      <c r="D76" s="43">
         <v>2</v>
       </c>
-      <c r="E75" s="43">
+      <c r="E76" s="43">
         <v>1</v>
       </c>
-      <c r="F75" s="43">
+      <c r="F76" s="43">
         <v>1</v>
       </c>
-      <c r="G75" s="43">
+      <c r="G76" s="43">
         <v>0.5</v>
       </c>
-      <c r="H75" s="43">
+      <c r="H76" s="43">
         <v>0.5</v>
       </c>
-      <c r="I75" s="43">
+      <c r="I76" s="43">
         <v>0.5</v>
       </c>
-      <c r="J75" s="43">
+      <c r="J76" s="43">
         <v>14400</v>
       </c>
-      <c r="K75" s="43">
+      <c r="K76" s="43">
         <v>86400</v>
       </c>
-      <c r="L75" s="43">
+      <c r="L76" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J77" t="s">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
         <v>312</v>
       </c>
-      <c r="K77" t="s">
+      <c r="K78" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J80">
+    <row r="81" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J81">
         <f>3600*4</f>
         <v>14400</v>
       </c>
-      <c r="K80">
+      <c r="K81">
         <f>3600*24</f>
         <v>86400</v>
       </c>
@@ -7087,8 +7116,8 @@
     <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D41:D50 D11:F11 E60:E61 D60:D65 D17:D36"/>
-    <dataValidation type="list" sqref="E41:E50">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D42:D51 D11:F11 E61:E62 D61:D66 D17:D37"/>
+    <dataValidation type="list" sqref="E42:E51">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added alien season same as UFO but only alien mask
Former-commit-id: d0cc667e9e4eff2bf26728e81ca2c901a3db0fe3
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="341">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1074,6 +1074,15 @@
   </si>
   <si>
     <t>TID_SEASON_ANNNIVERSARY_NO_EQUIP_NAME</t>
+  </si>
+  <si>
+    <t>Alien</t>
+  </si>
+  <si>
+    <t>icon_season_Alien</t>
+  </si>
+  <si>
+    <t>TID_ENTITY_DISGUISE_ALIEN_NAME</t>
   </si>
 </sst>
 </file>
@@ -5515,8 +5524,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H37" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
-  <autoFilter ref="B16:H37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H38" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+  <autoFilter ref="B16:H38"/>
   <tableColumns count="7">
     <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="58"/>
     <tableColumn id="2" name="[sku]" dataDxfId="57"/>
@@ -5531,8 +5540,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B41:G51" totalsRowShown="0" headerRowDxfId="51">
-  <autoFilter ref="B41:G51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B42:G52" totalsRowShown="0" headerRowDxfId="51">
+  <autoFilter ref="B42:G52"/>
   <sortState ref="B34:G44">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
@@ -5864,10 +5873,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:R81"/>
+  <dimension ref="A1:R82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6524,57 +6533,56 @@
       <c r="G37" s="37"/>
       <c r="H37" s="37"/>
     </row>
-    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B39" s="7" t="s">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="50" t="s">
+        <v>338</v>
+      </c>
+      <c r="D38" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>339</v>
+      </c>
+      <c r="F38" s="37" t="s">
+        <v>340</v>
+      </c>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+    </row>
+    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B40" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" t="s">
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="138" x14ac:dyDescent="0.25">
-      <c r="B41" s="31" t="s">
+    <row r="42" spans="2:8" ht="138" x14ac:dyDescent="0.25">
+      <c r="B42" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="C42" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="33" t="s">
+      <c r="D42" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E42" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="F41" s="34" t="s">
+      <c r="F42" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="G41" s="35" t="s">
+      <c r="G42" s="35" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D42" s="36">
-        <v>3000000</v>
-      </c>
-      <c r="E42" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="F42" s="18">
-        <v>1</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -6582,104 +6590,106 @@
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D43" s="36">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F43" s="18">
-        <v>5</v>
-      </c>
-      <c r="G43" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D44" s="36">
-        <v>2000000</v>
+        <v>2500000</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F44" s="18">
-        <v>1</v>
-      </c>
-      <c r="G44" s="18" t="s">
-        <v>140</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G44" s="18"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D45" s="36">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F45" s="18">
-        <v>5</v>
-      </c>
-      <c r="G45" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D46" s="36">
-        <v>1000000</v>
+        <v>1500000</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F46" s="18">
-        <v>1</v>
-      </c>
-      <c r="G46" s="18" t="s">
-        <v>139</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G46" s="18"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D47" s="36">
-        <v>500000</v>
+        <v>1000000</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F47" s="18">
-        <v>5</v>
-      </c>
-      <c r="G47" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D48" s="36">
-        <v>250000</v>
+        <v>500000</v>
       </c>
       <c r="E48" s="18" t="s">
         <v>134</v>
@@ -6694,16 +6704,16 @@
         <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D49" s="36">
-        <v>100000</v>
+        <v>250000</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="F49" s="18">
-        <v>1500</v>
+        <v>5</v>
       </c>
       <c r="G49" s="18"/>
     </row>
@@ -6712,16 +6722,16 @@
         <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D50" s="36">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>123</v>
       </c>
       <c r="F50" s="18">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="G50" s="18"/>
     </row>
@@ -6730,64 +6740,65 @@
         <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D51" s="36">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="E51" s="18" t="s">
         <v>123</v>
       </c>
       <c r="F51" s="18">
+        <v>500</v>
+      </c>
+      <c r="G51" s="18"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D52" s="36">
+        <v>10000</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F52" s="18">
         <v>100</v>
       </c>
-      <c r="G51" s="18"/>
-    </row>
-    <row r="53" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B54" s="7" t="s">
+      <c r="G52" s="18"/>
+    </row>
+    <row r="54" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B55" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" t="s">
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
-      <c r="B56" s="44" t="s">
+    <row r="57" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
+      <c r="B57" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="C56" s="45" t="s">
+      <c r="C57" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D56" s="46" t="s">
+      <c r="D57" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E56" s="46" t="s">
+      <c r="E57" s="46" t="s">
         <v>250</v>
       </c>
-      <c r="F56" s="46" t="s">
+      <c r="F57" s="46" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" s="43" t="s">
-        <v>246</v>
-      </c>
-      <c r="D57" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="E57" s="43" t="s">
-        <v>252</v>
-      </c>
-      <c r="F57" s="43" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
@@ -6795,13 +6806,13 @@
         <v>3</v>
       </c>
       <c r="C58" s="43" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E58" s="43" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F58" s="43" t="s">
         <v>288</v>
@@ -6812,13 +6823,13 @@
         <v>3</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D59" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E59" s="43" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F59" s="43" t="s">
         <v>288</v>
@@ -6829,13 +6840,13 @@
         <v>3</v>
       </c>
       <c r="C60" s="43" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D60" s="43" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E60" s="43" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F60" s="43" t="s">
         <v>288</v>
@@ -6846,14 +6857,16 @@
         <v>3</v>
       </c>
       <c r="C61" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="D61" s="43"/>
+        <v>249</v>
+      </c>
+      <c r="D61" s="43" t="s">
+        <v>257</v>
+      </c>
       <c r="E61" s="43" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F61" s="43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
@@ -6861,11 +6874,11 @@
         <v>3</v>
       </c>
       <c r="C62" s="43" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D62" s="43"/>
       <c r="E62" s="43" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F62" s="43" t="s">
         <v>289</v>
@@ -6876,11 +6889,11 @@
         <v>3</v>
       </c>
       <c r="C63" s="43" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D63" s="43"/>
       <c r="E63" s="43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F63" s="43" t="s">
         <v>289</v>
@@ -6891,11 +6904,11 @@
         <v>3</v>
       </c>
       <c r="C64" s="43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D64" s="43"/>
       <c r="E64" s="43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F64" s="43" t="s">
         <v>289</v>
@@ -6906,11 +6919,11 @@
         <v>3</v>
       </c>
       <c r="C65" s="43" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D65" s="43"/>
       <c r="E65" s="43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F65" s="43" t="s">
         <v>289</v>
@@ -6921,11 +6934,11 @@
         <v>3</v>
       </c>
       <c r="C66" s="43" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D66" s="43"/>
       <c r="E66" s="43" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F66" s="43" t="s">
         <v>289</v>
@@ -6936,11 +6949,11 @@
         <v>3</v>
       </c>
       <c r="C67" s="43" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D67" s="43"/>
       <c r="E67" s="43" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F67" s="43" t="s">
         <v>289</v>
@@ -6951,11 +6964,11 @@
         <v>3</v>
       </c>
       <c r="C68" s="43" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D68" s="43"/>
       <c r="E68" s="43" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F68" s="43" t="s">
         <v>289</v>
@@ -6966,11 +6979,11 @@
         <v>3</v>
       </c>
       <c r="C69" s="43" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D69" s="43"/>
       <c r="E69" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F69" s="43" t="s">
         <v>289</v>
@@ -6981,16 +6994,14 @@
         <v>3</v>
       </c>
       <c r="C70" s="43" t="s">
-        <v>290</v>
-      </c>
-      <c r="D70" s="43" t="s">
-        <v>291</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="D70" s="43"/>
       <c r="E70" s="43" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="F70" s="43" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.25">
@@ -6998,115 +7009,132 @@
         <v>3</v>
       </c>
       <c r="C71" s="43" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D71" s="43" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E71" s="43" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F71" s="43" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="72" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="73" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B73" s="7" t="s">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="43" t="s">
+        <v>293</v>
+      </c>
+      <c r="D72" s="43" t="s">
+        <v>294</v>
+      </c>
+      <c r="E72" s="43" t="s">
+        <v>295</v>
+      </c>
+      <c r="F72" s="43" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B74" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
-      <c r="G73" t="s">
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:12" ht="176.25" x14ac:dyDescent="0.25">
-      <c r="B75" s="44" t="s">
+    <row r="76" spans="2:12" ht="176.25" x14ac:dyDescent="0.25">
+      <c r="B76" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="C75" s="45" t="s">
+      <c r="C76" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D75" s="46" t="s">
+      <c r="D76" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="E75" s="46" t="s">
+      <c r="E76" s="46" t="s">
         <v>303</v>
       </c>
-      <c r="F75" s="46" t="s">
+      <c r="F76" s="46" t="s">
         <v>304</v>
       </c>
-      <c r="G75" s="51" t="s">
+      <c r="G76" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="H75" s="51" t="s">
+      <c r="H76" s="51" t="s">
         <v>306</v>
       </c>
-      <c r="I75" s="51" t="s">
+      <c r="I76" s="51" t="s">
         <v>307</v>
       </c>
-      <c r="J75" s="51" t="s">
+      <c r="J76" s="51" t="s">
         <v>308</v>
       </c>
-      <c r="K75" s="51" t="s">
+      <c r="K76" s="51" t="s">
         <v>309</v>
       </c>
-      <c r="L75" s="51" t="s">
+      <c r="L76" s="51" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B76" s="3" t="s">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B77" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="43" t="s">
+      <c r="C77" s="43" t="s">
         <v>311</v>
       </c>
-      <c r="D76" s="43">
+      <c r="D77" s="43">
         <v>2</v>
       </c>
-      <c r="E76" s="43">
+      <c r="E77" s="43">
         <v>1</v>
       </c>
-      <c r="F76" s="43">
+      <c r="F77" s="43">
         <v>1</v>
       </c>
-      <c r="G76" s="43">
+      <c r="G77" s="43">
         <v>0.5</v>
       </c>
-      <c r="H76" s="43">
+      <c r="H77" s="43">
         <v>0.5</v>
       </c>
-      <c r="I76" s="43">
+      <c r="I77" s="43">
         <v>0.5</v>
       </c>
-      <c r="J76" s="43">
+      <c r="J77" s="43">
         <v>14400</v>
       </c>
-      <c r="K76" s="43">
+      <c r="K77" s="43">
         <v>86400</v>
       </c>
-      <c r="L76" s="43">
+      <c r="L77" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J78" t="s">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J79" t="s">
         <v>312</v>
       </c>
-      <c r="K78" t="s">
+      <c r="K79" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="81" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J81">
+    <row r="82" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J82">
         <f>3600*4</f>
         <v>14400</v>
       </c>
-      <c r="K81">
+      <c r="K82">
         <f>3600*24</f>
         <v>86400</v>
       </c>
@@ -7116,8 +7144,8 @@
     <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D42:D51 D11:F11 E61:E62 D61:D66 D17:D37"/>
-    <dataValidation type="list" sqref="E42:E51">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D43:D52 D11:F11 E62:E63 D62:D67 D17:D38"/>
+    <dataValidation type="list" sqref="E43:E52">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Jalapeno chage name season, avoiding Ñ. add Jalapeno season correct naem to SP_seasonal
Former-commit-id: 600ec0a03fa6d7e7c8c436d79bb9eace8c5fe8db
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="343">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1064,9 +1064,6 @@
     <t>TID_SEASON_CANDY_NAME</t>
   </si>
   <si>
-    <t>jalapeño</t>
-  </si>
-  <si>
     <t>Anniversary_No_Equip</t>
   </si>
   <si>
@@ -1083,6 +1080,15 @@
   </si>
   <si>
     <t>TID_ENTITY_DISGUISE_ALIEN_NAME</t>
+  </si>
+  <si>
+    <t>jalapeno</t>
+  </si>
+  <si>
+    <t>icon_season_jalapeno</t>
+  </si>
+  <si>
+    <t>TID_SEASON_JALAPENO_NAME</t>
   </si>
 </sst>
 </file>
@@ -1546,106 +1552,6 @@
   </cellStyles>
   <dxfs count="94">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2393,6 +2299,96 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3473,6 +3469,16 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5483,125 +5489,125 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="gameSettings9" displayName="gameSettings9" ref="B4:R5" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="gameSettings9" displayName="gameSettings9" ref="B4:R5" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90" totalsRowBorderDxfId="89">
   <autoFilter ref="B4:R5"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="89"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="87"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="86"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="85"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="84"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="83"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="82"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="81"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="80"/>
-    <tableColumn id="17" name="[miniMapTimerAd]" dataDxfId="79"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="78"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="77"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="75"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="74"/>
-    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="73"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="88"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="86"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="85"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="84"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="83"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="82"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="81"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="80"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="79"/>
+    <tableColumn id="17" name="[miniMapTimerAd]" dataDxfId="78"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="77"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="74"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="73"/>
+    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="gameSettings2110" displayName="gameSettings2110" ref="B10:G11" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70" totalsRowBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="gameSettings2110" displayName="gameSettings2110" ref="B10:G11" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="68"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="67"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="66"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="65"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="64"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="63"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="67"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="65"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="64"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="63"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H38" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H38" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
   <autoFilter ref="B16:H38"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="58"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="57"/>
-    <tableColumn id="3" name="[active]" dataDxfId="56"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="55"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="54"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="53"/>
-    <tableColumn id="7" name="[pillParticles]" dataDxfId="52"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="56"/>
+    <tableColumn id="3" name="[active]" dataDxfId="55"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="54"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="53"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="52"/>
+    <tableColumn id="7" name="[pillParticles]" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B42:G52" totalsRowShown="0" headerRowDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B42:G52" totalsRowShown="0" headerRowDxfId="50">
   <autoFilter ref="B42:G52"/>
   <sortState ref="B34:G44">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="48"/>
-    <tableColumn id="4" name="[type]" dataDxfId="47"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="46"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="45"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
+    <tableColumn id="4" name="[type]" dataDxfId="46"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="40"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="3" name="[order]" dataDxfId="38"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="37"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="36"/>
-    <tableColumn id="11" name="[android]" dataDxfId="35"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="34"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="33"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="32"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="31"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="30"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="29"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" name="[order]" dataDxfId="28"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
+    <tableColumn id="11" name="[android]" dataDxfId="25"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="24"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="22"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="21"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="16"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="14"/>
-    <tableColumn id="2" name="[url]" dataDxfId="13"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="12"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="11"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="10"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
+    <tableColumn id="2" name="[url]" dataDxfId="3"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5876,7 +5882,7 @@
   <dimension ref="A1:R82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6500,16 +6506,16 @@
         <v>3</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="D36" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E36" s="39" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="F36" s="39" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="G36" s="39"/>
       <c r="H36" s="39"/>
@@ -6519,16 +6525,16 @@
         <v>3</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D37" s="38" t="b">
         <v>0</v>
       </c>
       <c r="E37" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="F37" s="37" t="s">
         <v>336</v>
-      </c>
-      <c r="F37" s="37" t="s">
-        <v>337</v>
       </c>
       <c r="G37" s="37"/>
       <c r="H37" s="37"/>
@@ -6538,16 +6544,16 @@
         <v>3</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D38" s="38" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="37" t="s">
+        <v>338</v>
+      </c>
+      <c r="F38" s="37" t="s">
         <v>339</v>
-      </c>
-      <c r="F38" s="37" t="s">
-        <v>340</v>
       </c>
       <c r="G38" s="37"/>
       <c r="H38" s="37"/>
@@ -7141,7 +7147,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D43:D52 D11:F11 E62:E63 D62:D67 D17:D38"/>
@@ -8226,31 +8232,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="L5:L16">

</xml_diff>

<commit_message>
added season Halloween_china Equip animals with hat witch
Former-commit-id: aff5440b757c0e6b1135e2fcec260b8ffd8afe97
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
+    <workbookView minimized="1" xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="344">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1089,6 +1089,9 @@
   </si>
   <si>
     <t>TID_SEASON_JALAPENO_NAME</t>
+  </si>
+  <si>
+    <t>halloween_China</t>
   </si>
 </sst>
 </file>
@@ -1552,6 +1555,106 @@
   </cellStyles>
   <dxfs count="94">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2299,96 +2402,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3469,16 +3482,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5489,125 +5492,125 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="gameSettings9" displayName="gameSettings9" ref="B4:R5" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90" totalsRowBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="gameSettings9" displayName="gameSettings9" ref="B4:R5" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
   <autoFilter ref="B4:R5"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="88"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="86"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="85"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="84"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="83"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="82"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="81"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="80"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="79"/>
-    <tableColumn id="17" name="[miniMapTimerAd]" dataDxfId="78"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="77"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="74"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="73"/>
-    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="72"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="89"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="87"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="86"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="85"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="84"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="83"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="82"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="81"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="80"/>
+    <tableColumn id="17" name="[miniMapTimerAd]" dataDxfId="79"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="78"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="77"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="75"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="74"/>
+    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="gameSettings2110" displayName="gameSettings2110" ref="B10:G11" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="gameSettings2110" displayName="gameSettings2110" ref="B10:G11" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="67"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="65"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="64"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="63"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="62"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="68"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="67"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="66"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="65"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="64"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H38" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
-  <autoFilter ref="B16:H38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H39" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+  <autoFilter ref="B16:H39"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="57"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="56"/>
-    <tableColumn id="3" name="[active]" dataDxfId="55"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="54"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="53"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="52"/>
-    <tableColumn id="7" name="[pillParticles]" dataDxfId="51"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="58"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="57"/>
+    <tableColumn id="3" name="[active]" dataDxfId="56"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="55"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="54"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="53"/>
+    <tableColumn id="7" name="[pillParticles]" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B42:G52" totalsRowShown="0" headerRowDxfId="50">
-  <autoFilter ref="B42:G52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B43:G53" totalsRowShown="0" headerRowDxfId="51">
+  <autoFilter ref="B43:G53"/>
   <sortState ref="B34:G44">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
-    <tableColumn id="4" name="[type]" dataDxfId="46"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="48"/>
+    <tableColumn id="4" name="[type]" dataDxfId="47"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="46"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="3" name="[order]" dataDxfId="28"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
-    <tableColumn id="11" name="[android]" dataDxfId="25"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="40"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="3" name="[order]" dataDxfId="38"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="37"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="36"/>
+    <tableColumn id="11" name="[android]" dataDxfId="35"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="34"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="33"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="32"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="31"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="30"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="24"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="22"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
-    <tableColumn id="2" name="[url]" dataDxfId="3"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="16"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="15"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="14"/>
+    <tableColumn id="2" name="[url]" dataDxfId="13"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="12"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="11"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5879,10 +5882,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:R82"/>
+  <dimension ref="A1:R83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6558,57 +6561,58 @@
       <c r="G38" s="37"/>
       <c r="H38" s="37"/>
     </row>
-    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B40" s="7" t="s">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>343</v>
+      </c>
+      <c r="D39" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B41" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" t="s">
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="138" x14ac:dyDescent="0.25">
-      <c r="B42" s="31" t="s">
+    <row r="43" spans="2:8" ht="138" x14ac:dyDescent="0.25">
+      <c r="B43" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="C43" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="33" t="s">
+      <c r="D43" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="E42" s="34" t="s">
+      <c r="E43" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="F42" s="34" t="s">
+      <c r="F43" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="G42" s="35" t="s">
+      <c r="G43" s="35" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D43" s="36">
-        <v>3000000</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="F43" s="18">
-        <v>1</v>
-      </c>
-      <c r="G43" s="18" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
@@ -6616,104 +6620,106 @@
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D44" s="36">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F44" s="18">
-        <v>5</v>
-      </c>
-      <c r="G44" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D45" s="36">
-        <v>2000000</v>
+        <v>2500000</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F45" s="18">
-        <v>1</v>
-      </c>
-      <c r="G45" s="18" t="s">
-        <v>140</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G45" s="18"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D46" s="36">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F46" s="18">
-        <v>5</v>
-      </c>
-      <c r="G46" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D47" s="36">
-        <v>1000000</v>
+        <v>1500000</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F47" s="18">
-        <v>1</v>
-      </c>
-      <c r="G47" s="18" t="s">
-        <v>139</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G47" s="18"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D48" s="36">
-        <v>500000</v>
+        <v>1000000</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F48" s="18">
-        <v>5</v>
-      </c>
-      <c r="G48" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D49" s="36">
-        <v>250000</v>
+        <v>500000</v>
       </c>
       <c r="E49" s="18" t="s">
         <v>134</v>
@@ -6728,16 +6734,16 @@
         <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D50" s="36">
-        <v>100000</v>
+        <v>250000</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="F50" s="18">
-        <v>1500</v>
+        <v>5</v>
       </c>
       <c r="G50" s="18"/>
     </row>
@@ -6746,16 +6752,16 @@
         <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D51" s="36">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="E51" s="18" t="s">
         <v>123</v>
       </c>
       <c r="F51" s="18">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="G51" s="18"/>
     </row>
@@ -6764,64 +6770,65 @@
         <v>3</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D52" s="36">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="E52" s="18" t="s">
         <v>123</v>
       </c>
       <c r="F52" s="18">
+        <v>500</v>
+      </c>
+      <c r="G52" s="18"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D53" s="36">
+        <v>10000</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F53" s="18">
         <v>100</v>
       </c>
-      <c r="G52" s="18"/>
-    </row>
-    <row r="54" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B55" s="7" t="s">
+      <c r="G53" s="18"/>
+    </row>
+    <row r="55" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B56" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" t="s">
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
-      <c r="B57" s="44" t="s">
+    <row r="58" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
+      <c r="B58" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="C57" s="45" t="s">
+      <c r="C58" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="46" t="s">
+      <c r="D58" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E57" s="46" t="s">
+      <c r="E58" s="46" t="s">
         <v>250</v>
       </c>
-      <c r="F57" s="46" t="s">
+      <c r="F58" s="46" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58" s="43" t="s">
-        <v>246</v>
-      </c>
-      <c r="D58" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="E58" s="43" t="s">
-        <v>252</v>
-      </c>
-      <c r="F58" s="43" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
@@ -6829,13 +6836,13 @@
         <v>3</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D59" s="43" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E59" s="43" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F59" s="43" t="s">
         <v>288</v>
@@ -6846,13 +6853,13 @@
         <v>3</v>
       </c>
       <c r="C60" s="43" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D60" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E60" s="43" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F60" s="43" t="s">
         <v>288</v>
@@ -6863,13 +6870,13 @@
         <v>3</v>
       </c>
       <c r="C61" s="43" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D61" s="43" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E61" s="43" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F61" s="43" t="s">
         <v>288</v>
@@ -6880,14 +6887,16 @@
         <v>3</v>
       </c>
       <c r="C62" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="D62" s="43"/>
+        <v>249</v>
+      </c>
+      <c r="D62" s="43" t="s">
+        <v>257</v>
+      </c>
       <c r="E62" s="43" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F62" s="43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.25">
@@ -6895,11 +6904,11 @@
         <v>3</v>
       </c>
       <c r="C63" s="43" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D63" s="43"/>
       <c r="E63" s="43" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F63" s="43" t="s">
         <v>289</v>
@@ -6910,11 +6919,11 @@
         <v>3</v>
       </c>
       <c r="C64" s="43" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D64" s="43"/>
       <c r="E64" s="43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F64" s="43" t="s">
         <v>289</v>
@@ -6925,11 +6934,11 @@
         <v>3</v>
       </c>
       <c r="C65" s="43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D65" s="43"/>
       <c r="E65" s="43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F65" s="43" t="s">
         <v>289</v>
@@ -6940,11 +6949,11 @@
         <v>3</v>
       </c>
       <c r="C66" s="43" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D66" s="43"/>
       <c r="E66" s="43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F66" s="43" t="s">
         <v>289</v>
@@ -6955,11 +6964,11 @@
         <v>3</v>
       </c>
       <c r="C67" s="43" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D67" s="43"/>
       <c r="E67" s="43" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F67" s="43" t="s">
         <v>289</v>
@@ -6970,11 +6979,11 @@
         <v>3</v>
       </c>
       <c r="C68" s="43" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D68" s="43"/>
       <c r="E68" s="43" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F68" s="43" t="s">
         <v>289</v>
@@ -6985,11 +6994,11 @@
         <v>3</v>
       </c>
       <c r="C69" s="43" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D69" s="43"/>
       <c r="E69" s="43" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F69" s="43" t="s">
         <v>289</v>
@@ -7000,11 +7009,11 @@
         <v>3</v>
       </c>
       <c r="C70" s="43" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D70" s="43"/>
       <c r="E70" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F70" s="43" t="s">
         <v>289</v>
@@ -7015,16 +7024,14 @@
         <v>3</v>
       </c>
       <c r="C71" s="43" t="s">
-        <v>290</v>
-      </c>
-      <c r="D71" s="43" t="s">
-        <v>291</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="D71" s="43"/>
       <c r="E71" s="43" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="F71" s="43" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.25">
@@ -7032,126 +7039,143 @@
         <v>3</v>
       </c>
       <c r="C72" s="43" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D72" s="43" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E72" s="43" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F72" s="43" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="73" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B74" s="7" t="s">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B73" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="43" t="s">
+        <v>293</v>
+      </c>
+      <c r="D73" s="43" t="s">
+        <v>294</v>
+      </c>
+      <c r="E73" s="43" t="s">
+        <v>295</v>
+      </c>
+      <c r="F73" s="43" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B75" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="7"/>
-      <c r="G74" t="s">
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:12" ht="176.25" x14ac:dyDescent="0.25">
-      <c r="B76" s="44" t="s">
+    <row r="77" spans="2:12" ht="176.25" x14ac:dyDescent="0.25">
+      <c r="B77" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="C76" s="45" t="s">
+      <c r="C77" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D76" s="46" t="s">
+      <c r="D77" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="E76" s="46" t="s">
+      <c r="E77" s="46" t="s">
         <v>303</v>
       </c>
-      <c r="F76" s="46" t="s">
+      <c r="F77" s="46" t="s">
         <v>304</v>
       </c>
-      <c r="G76" s="51" t="s">
+      <c r="G77" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="H76" s="51" t="s">
+      <c r="H77" s="51" t="s">
         <v>306</v>
       </c>
-      <c r="I76" s="51" t="s">
+      <c r="I77" s="51" t="s">
         <v>307</v>
       </c>
-      <c r="J76" s="51" t="s">
+      <c r="J77" s="51" t="s">
         <v>308</v>
       </c>
-      <c r="K76" s="51" t="s">
+      <c r="K77" s="51" t="s">
         <v>309</v>
       </c>
-      <c r="L76" s="51" t="s">
+      <c r="L77" s="51" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B77" s="3" t="s">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B78" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="43" t="s">
+      <c r="C78" s="43" t="s">
         <v>311</v>
       </c>
-      <c r="D77" s="43">
+      <c r="D78" s="43">
         <v>2</v>
       </c>
-      <c r="E77" s="43">
+      <c r="E78" s="43">
         <v>1</v>
       </c>
-      <c r="F77" s="43">
+      <c r="F78" s="43">
         <v>1</v>
       </c>
-      <c r="G77" s="43">
+      <c r="G78" s="43">
         <v>0.5</v>
       </c>
-      <c r="H77" s="43">
+      <c r="H78" s="43">
         <v>0.5</v>
       </c>
-      <c r="I77" s="43">
+      <c r="I78" s="43">
         <v>0.5</v>
       </c>
-      <c r="J77" s="43">
+      <c r="J78" s="43">
         <v>14400</v>
       </c>
-      <c r="K77" s="43">
+      <c r="K78" s="43">
         <v>86400</v>
       </c>
-      <c r="L77" s="43">
+      <c r="L78" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J79" t="s">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
         <v>312</v>
       </c>
-      <c r="K79" t="s">
+      <c r="K80" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="82" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J82">
+    <row r="83" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J83">
         <f>3600*4</f>
         <v>14400</v>
       </c>
-      <c r="K82">
+      <c r="K83">
         <f>3600*24</f>
         <v>86400</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="93" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D43:D52 D11:F11 E62:E63 D62:D67 D17:D38"/>
-    <dataValidation type="list" sqref="E43:E52">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D44:D53 D11:F11 E63:E64 D63:D68 D17:D39"/>
+    <dataValidation type="list" sqref="E44:E53">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8232,31 +8256,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="L5:L16">

</xml_diff>

<commit_message>
added season werewolf and vampire. Also mods
Former-commit-id: f5cfd701e121b27fc114e3218d7e1284ad9a0000
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="350">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1092,6 +1092,24 @@
   </si>
   <si>
     <t>halloween_China</t>
+  </si>
+  <si>
+    <t>werewolf</t>
+  </si>
+  <si>
+    <t>icon_season_werewolf</t>
+  </si>
+  <si>
+    <t>TID_SEASON_WEREWOLF_NAME</t>
+  </si>
+  <si>
+    <t>vampire</t>
+  </si>
+  <si>
+    <t>icon_season_vampire</t>
+  </si>
+  <si>
+    <t>TID_SEASON_VAMPIRE_NAME</t>
   </si>
 </sst>
 </file>
@@ -5533,8 +5551,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H39" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
-  <autoFilter ref="B16:H39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H41" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+  <autoFilter ref="B16:H41"/>
   <tableColumns count="7">
     <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="58"/>
     <tableColumn id="2" name="[sku]" dataDxfId="57"/>
@@ -5549,8 +5567,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B43:G53" totalsRowShown="0" headerRowDxfId="51">
-  <autoFilter ref="B43:G53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B45:G55" totalsRowShown="0" headerRowDxfId="51">
+  <autoFilter ref="B45:G55"/>
   <sortState ref="B34:G44">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
@@ -5882,10 +5900,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:R83"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6582,95 +6600,99 @@
         <v>298</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B41" s="7" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="D40" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="39" t="s">
+        <v>345</v>
+      </c>
+      <c r="F40" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>347</v>
+      </c>
+      <c r="D41" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="F41" s="39" t="s">
+        <v>349</v>
+      </c>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B43" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" t="s">
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="138" x14ac:dyDescent="0.25">
-      <c r="B43" s="31" t="s">
+    <row r="45" spans="2:8" ht="138" x14ac:dyDescent="0.25">
+      <c r="B45" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="C45" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D45" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="E43" s="34" t="s">
+      <c r="E45" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="F43" s="34" t="s">
+      <c r="F45" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="G43" s="35" t="s">
+      <c r="G45" s="35" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D44" s="36">
-        <v>3000000</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="F44" s="18">
-        <v>1</v>
-      </c>
-      <c r="G44" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D45" s="36">
-        <v>2500000</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="F45" s="18">
-        <v>5</v>
-      </c>
-      <c r="G45" s="18"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D46" s="36">
-        <v>2000000</v>
+        <v>3000000</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F46" s="18">
         <v>1</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
@@ -6678,13 +6700,13 @@
         <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D47" s="36">
-        <v>1500000</v>
+        <v>2500000</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F47" s="18">
         <v>5</v>
@@ -6696,10 +6718,10 @@
         <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D48" s="36">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="E48" s="18" t="s">
         <v>135</v>
@@ -6708,7 +6730,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
@@ -6716,10 +6738,10 @@
         <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D49" s="36">
-        <v>500000</v>
+        <v>1500000</v>
       </c>
       <c r="E49" s="18" t="s">
         <v>134</v>
@@ -6734,34 +6756,36 @@
         <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D50" s="36">
-        <v>250000</v>
+        <v>1000000</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F50" s="18">
-        <v>5</v>
-      </c>
-      <c r="G50" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D51" s="36">
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="F51" s="18">
-        <v>1500</v>
+        <v>5</v>
       </c>
       <c r="G51" s="18"/>
     </row>
@@ -6770,16 +6794,16 @@
         <v>3</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D52" s="36">
-        <v>50000</v>
+        <v>250000</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="F52" s="18">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="G52" s="18"/>
     </row>
@@ -6788,81 +6812,83 @@
         <v>3</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="D53" s="36">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="E53" s="18" t="s">
         <v>123</v>
       </c>
       <c r="F53" s="18">
+        <v>1500</v>
+      </c>
+      <c r="G53" s="18"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" s="36">
+        <v>50000</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F54" s="18">
+        <v>500</v>
+      </c>
+      <c r="G54" s="18"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" s="36">
+        <v>10000</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F55" s="18">
         <v>100</v>
       </c>
-      <c r="G53" s="18"/>
-    </row>
-    <row r="55" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B56" s="7" t="s">
+      <c r="G55" s="18"/>
+    </row>
+    <row r="57" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B58" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" t="s">
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
-      <c r="B58" s="44" t="s">
+    <row r="60" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
+      <c r="B60" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="C58" s="45" t="s">
+      <c r="C60" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="46" t="s">
+      <c r="D60" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E58" s="46" t="s">
+      <c r="E60" s="46" t="s">
         <v>250</v>
       </c>
-      <c r="F58" s="46" t="s">
+      <c r="F60" s="46" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C59" s="43" t="s">
-        <v>246</v>
-      </c>
-      <c r="D59" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="E59" s="43" t="s">
-        <v>252</v>
-      </c>
-      <c r="F59" s="43" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="43" t="s">
-        <v>247</v>
-      </c>
-      <c r="D60" s="43" t="s">
-        <v>253</v>
-      </c>
-      <c r="E60" s="43" t="s">
-        <v>254</v>
-      </c>
-      <c r="F60" s="43" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
@@ -6870,13 +6896,13 @@
         <v>3</v>
       </c>
       <c r="C61" s="43" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D61" s="43" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E61" s="43" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F61" s="43" t="s">
         <v>288</v>
@@ -6887,13 +6913,13 @@
         <v>3</v>
       </c>
       <c r="C62" s="43" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D62" s="43" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E62" s="43" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F62" s="43" t="s">
         <v>288</v>
@@ -6904,14 +6930,16 @@
         <v>3</v>
       </c>
       <c r="C63" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="D63" s="43"/>
+        <v>248</v>
+      </c>
+      <c r="D63" s="43" t="s">
+        <v>255</v>
+      </c>
       <c r="E63" s="43" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F63" s="43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
@@ -6919,14 +6947,16 @@
         <v>3</v>
       </c>
       <c r="C64" s="43" t="s">
-        <v>269</v>
-      </c>
-      <c r="D64" s="43"/>
+        <v>249</v>
+      </c>
+      <c r="D64" s="43" t="s">
+        <v>257</v>
+      </c>
       <c r="E64" s="43" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F64" s="43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.25">
@@ -6934,11 +6964,11 @@
         <v>3</v>
       </c>
       <c r="C65" s="43" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D65" s="43"/>
       <c r="E65" s="43" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F65" s="43" t="s">
         <v>289</v>
@@ -6949,11 +6979,11 @@
         <v>3</v>
       </c>
       <c r="C66" s="43" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D66" s="43"/>
       <c r="E66" s="43" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F66" s="43" t="s">
         <v>289</v>
@@ -6964,11 +6994,11 @@
         <v>3</v>
       </c>
       <c r="C67" s="43" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D67" s="43"/>
       <c r="E67" s="43" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F67" s="43" t="s">
         <v>289</v>
@@ -6979,11 +7009,11 @@
         <v>3</v>
       </c>
       <c r="C68" s="43" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D68" s="43"/>
       <c r="E68" s="43" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F68" s="43" t="s">
         <v>289</v>
@@ -6994,11 +7024,11 @@
         <v>3</v>
       </c>
       <c r="C69" s="43" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D69" s="43"/>
       <c r="E69" s="43" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F69" s="43" t="s">
         <v>289</v>
@@ -7009,11 +7039,11 @@
         <v>3</v>
       </c>
       <c r="C70" s="43" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D70" s="43"/>
       <c r="E70" s="43" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F70" s="43" t="s">
         <v>289</v>
@@ -7024,11 +7054,11 @@
         <v>3</v>
       </c>
       <c r="C71" s="43" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D71" s="43"/>
       <c r="E71" s="43" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F71" s="43" t="s">
         <v>289</v>
@@ -7039,16 +7069,14 @@
         <v>3</v>
       </c>
       <c r="C72" s="43" t="s">
-        <v>290</v>
-      </c>
-      <c r="D72" s="43" t="s">
-        <v>291</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="D72" s="43"/>
       <c r="E72" s="43" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
       <c r="F72" s="43" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.25">
@@ -7056,115 +7084,147 @@
         <v>3</v>
       </c>
       <c r="C73" s="43" t="s">
+        <v>276</v>
+      </c>
+      <c r="D73" s="43"/>
+      <c r="E73" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="F73" s="43" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="43" t="s">
+        <v>290</v>
+      </c>
+      <c r="D74" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="E74" s="43" t="s">
+        <v>292</v>
+      </c>
+      <c r="F74" s="43" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B75" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="D73" s="43" t="s">
+      <c r="D75" s="43" t="s">
         <v>294</v>
       </c>
-      <c r="E73" s="43" t="s">
+      <c r="E75" s="43" t="s">
         <v>295</v>
       </c>
-      <c r="F73" s="43" t="s">
+      <c r="F75" s="43" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="74" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B75" s="7" t="s">
+    <row r="76" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B77" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-      <c r="G75" t="s">
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:12" ht="176.25" x14ac:dyDescent="0.25">
-      <c r="B77" s="44" t="s">
+    <row r="79" spans="2:12" ht="176.25" x14ac:dyDescent="0.25">
+      <c r="B79" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="C77" s="45" t="s">
+      <c r="C79" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D77" s="46" t="s">
+      <c r="D79" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="E77" s="46" t="s">
+      <c r="E79" s="46" t="s">
         <v>303</v>
       </c>
-      <c r="F77" s="46" t="s">
+      <c r="F79" s="46" t="s">
         <v>304</v>
       </c>
-      <c r="G77" s="51" t="s">
+      <c r="G79" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="H77" s="51" t="s">
+      <c r="H79" s="51" t="s">
         <v>306</v>
       </c>
-      <c r="I77" s="51" t="s">
+      <c r="I79" s="51" t="s">
         <v>307</v>
       </c>
-      <c r="J77" s="51" t="s">
+      <c r="J79" s="51" t="s">
         <v>308</v>
       </c>
-      <c r="K77" s="51" t="s">
+      <c r="K79" s="51" t="s">
         <v>309</v>
       </c>
-      <c r="L77" s="51" t="s">
+      <c r="L79" s="51" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B78" s="3" t="s">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B80" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C78" s="43" t="s">
+      <c r="C80" s="43" t="s">
         <v>311</v>
       </c>
-      <c r="D78" s="43">
+      <c r="D80" s="43">
         <v>2</v>
       </c>
-      <c r="E78" s="43">
+      <c r="E80" s="43">
         <v>1</v>
       </c>
-      <c r="F78" s="43">
+      <c r="F80" s="43">
         <v>1</v>
       </c>
-      <c r="G78" s="43">
+      <c r="G80" s="43">
         <v>0.5</v>
       </c>
-      <c r="H78" s="43">
+      <c r="H80" s="43">
         <v>0.5</v>
       </c>
-      <c r="I78" s="43">
+      <c r="I80" s="43">
         <v>0.5</v>
       </c>
-      <c r="J78" s="43">
+      <c r="J80" s="43">
         <v>14400</v>
       </c>
-      <c r="K78" s="43">
+      <c r="K80" s="43">
         <v>86400</v>
       </c>
-      <c r="L78" s="43">
+      <c r="L80" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J80" t="s">
+    <row r="82" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J82" t="s">
         <v>312</v>
       </c>
-      <c r="K80" t="s">
+      <c r="K82" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="83" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J83">
+    <row r="85" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J85">
         <f>3600*4</f>
         <v>14400</v>
       </c>
-      <c r="K83">
+      <c r="K85">
         <f>3600*24</f>
         <v>86400</v>
       </c>
@@ -7174,8 +7234,8 @@
     <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D44:D53 D11:F11 E63:E64 D63:D68 D17:D39"/>
-    <dataValidation type="list" sqref="E44:E53">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D46:D55 D11:F11 E65:E66 D65:D70 D17:D41"/>
+    <dataValidation type="list" sqref="E46:E55">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
adde new mod bunnies (flying and ground)  ground bunnies added season bunnies added to sp_bunny season chinese autumn and bunnies added bundles to new invasion scenes added icon bunnies added bunnies tour and quest
Former-commit-id: 6886957fe6eb46ecbcc5393d4fcde1a97d26b890
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="353">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1110,13 +1110,25 @@
   </si>
   <si>
     <t>TID_SEASON_VAMPIRE_NAME</t>
+  </si>
+  <si>
+    <t>bunnies</t>
+  </si>
+  <si>
+    <t>icon_season_bunnies</t>
+  </si>
+  <si>
+    <t>TID_SEASON_BUNNIES_NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1195,6 +1207,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1463,10 +1482,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1567,11 +1587,233 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="10" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="94">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2571,220 +2813,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -5551,84 +5579,84 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H41" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
-  <autoFilter ref="B16:H41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H42" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="B16:H42"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="58"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="57"/>
-    <tableColumn id="3" name="[active]" dataDxfId="56"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="55"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="54"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="53"/>
-    <tableColumn id="7" name="[pillParticles]" dataDxfId="52"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="6"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="3" name="[active]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="2"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="1"/>
+    <tableColumn id="7" name="[pillParticles]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B45:G55" totalsRowShown="0" headerRowDxfId="51">
-  <autoFilter ref="B45:G55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B46:G56" totalsRowShown="0" headerRowDxfId="62">
+  <autoFilter ref="B46:G56"/>
   <sortState ref="B34:G44">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="48"/>
-    <tableColumn id="4" name="[type]" dataDxfId="47"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="46"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="45"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="61"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="60"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="59"/>
+    <tableColumn id="4" name="[type]" dataDxfId="58"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="57"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="40"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="3" name="[order]" dataDxfId="38"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="37"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="36"/>
-    <tableColumn id="11" name="[android]" dataDxfId="35"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="34"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="33"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="32"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="31"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="30"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="29"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="51"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="3" name="[order]" dataDxfId="49"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="48"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="47"/>
+    <tableColumn id="11" name="[android]" dataDxfId="46"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="45"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="44"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="43"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="42"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="41"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="24"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="22"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="21"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="35"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="34"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="33"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="16"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="14"/>
-    <tableColumn id="2" name="[url]" dataDxfId="13"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="12"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="11"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="10"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="27"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="26"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="25"/>
+    <tableColumn id="2" name="[url]" dataDxfId="24"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="23"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="22"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5900,10 +5928,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:R85"/>
+  <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6621,78 +6649,77 @@
         <v>298</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
+    <row r="41" spans="2:8" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="C41" s="55" t="s">
         <v>347</v>
       </c>
-      <c r="D41" s="1" t="b">
+      <c r="D41" s="56" t="b">
         <v>0</v>
       </c>
-      <c r="E41" s="39" t="s">
+      <c r="E41" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="F41" s="39" t="s">
+      <c r="F41" s="57" t="s">
         <v>349</v>
       </c>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39" t="s">
+      <c r="G41" s="57"/>
+      <c r="H41" s="57" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B43" s="7" t="s">
+    <row r="42" spans="2:8" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="55" t="s">
+        <v>350</v>
+      </c>
+      <c r="D42" s="60" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="55" t="s">
+        <v>351</v>
+      </c>
+      <c r="F42" s="55" t="s">
+        <v>352</v>
+      </c>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55"/>
+    </row>
+    <row r="43" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B44" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" t="s">
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="138" x14ac:dyDescent="0.25">
-      <c r="B45" s="31" t="s">
+    <row r="46" spans="2:8" ht="138" x14ac:dyDescent="0.25">
+      <c r="B46" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="C46" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="33" t="s">
+      <c r="D46" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="E45" s="34" t="s">
+      <c r="E46" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="F45" s="34" t="s">
+      <c r="F46" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="G45" s="35" t="s">
+      <c r="G46" s="35" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D46" s="36">
-        <v>3000000</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="F46" s="18">
-        <v>1</v>
-      </c>
-      <c r="G46" s="18" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
@@ -6700,104 +6727,106 @@
         <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D47" s="36">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F47" s="18">
-        <v>5</v>
-      </c>
-      <c r="G47" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D48" s="36">
-        <v>2000000</v>
+        <v>2500000</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F48" s="18">
-        <v>1</v>
-      </c>
-      <c r="G48" s="18" t="s">
-        <v>140</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D49" s="36">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F49" s="18">
-        <v>5</v>
-      </c>
-      <c r="G49" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D50" s="36">
-        <v>1000000</v>
+        <v>1500000</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F50" s="18">
-        <v>1</v>
-      </c>
-      <c r="G50" s="18" t="s">
-        <v>139</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G50" s="18"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D51" s="36">
-        <v>500000</v>
+        <v>1000000</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F51" s="18">
-        <v>5</v>
-      </c>
-      <c r="G51" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D52" s="36">
-        <v>250000</v>
+        <v>500000</v>
       </c>
       <c r="E52" s="18" t="s">
         <v>134</v>
@@ -6812,16 +6841,16 @@
         <v>3</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D53" s="36">
-        <v>100000</v>
+        <v>250000</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="F53" s="18">
-        <v>1500</v>
+        <v>5</v>
       </c>
       <c r="G53" s="18"/>
     </row>
@@ -6830,16 +6859,16 @@
         <v>3</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D54" s="36">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="E54" s="18" t="s">
         <v>123</v>
       </c>
       <c r="F54" s="18">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="G54" s="18"/>
     </row>
@@ -6848,64 +6877,65 @@
         <v>3</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D55" s="36">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="E55" s="18" t="s">
         <v>123</v>
       </c>
       <c r="F55" s="18">
+        <v>500</v>
+      </c>
+      <c r="G55" s="18"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" s="36">
+        <v>10000</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F56" s="18">
         <v>100</v>
       </c>
-      <c r="G55" s="18"/>
-    </row>
-    <row r="57" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B58" s="7" t="s">
+      <c r="G56" s="18"/>
+    </row>
+    <row r="58" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B59" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" t="s">
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
-      <c r="B60" s="44" t="s">
+    <row r="61" spans="2:7" ht="124.5" x14ac:dyDescent="0.25">
+      <c r="B61" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="C60" s="45" t="s">
+      <c r="C61" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D60" s="46" t="s">
+      <c r="D61" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E60" s="46" t="s">
+      <c r="E61" s="46" t="s">
         <v>250</v>
       </c>
-      <c r="F60" s="46" t="s">
+      <c r="F61" s="46" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C61" s="43" t="s">
-        <v>246</v>
-      </c>
-      <c r="D61" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="E61" s="43" t="s">
-        <v>252</v>
-      </c>
-      <c r="F61" s="43" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
@@ -6913,13 +6943,13 @@
         <v>3</v>
       </c>
       <c r="C62" s="43" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D62" s="43" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E62" s="43" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F62" s="43" t="s">
         <v>288</v>
@@ -6930,13 +6960,13 @@
         <v>3</v>
       </c>
       <c r="C63" s="43" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D63" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E63" s="43" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F63" s="43" t="s">
         <v>288</v>
@@ -6947,13 +6977,13 @@
         <v>3</v>
       </c>
       <c r="C64" s="43" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D64" s="43" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E64" s="43" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F64" s="43" t="s">
         <v>288</v>
@@ -6964,14 +6994,16 @@
         <v>3</v>
       </c>
       <c r="C65" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="D65" s="43"/>
+        <v>249</v>
+      </c>
+      <c r="D65" s="43" t="s">
+        <v>257</v>
+      </c>
       <c r="E65" s="43" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F65" s="43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.25">
@@ -6979,11 +7011,11 @@
         <v>3</v>
       </c>
       <c r="C66" s="43" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D66" s="43"/>
       <c r="E66" s="43" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F66" s="43" t="s">
         <v>289</v>
@@ -6994,11 +7026,11 @@
         <v>3</v>
       </c>
       <c r="C67" s="43" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D67" s="43"/>
       <c r="E67" s="43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F67" s="43" t="s">
         <v>289</v>
@@ -7009,11 +7041,11 @@
         <v>3</v>
       </c>
       <c r="C68" s="43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D68" s="43"/>
       <c r="E68" s="43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F68" s="43" t="s">
         <v>289</v>
@@ -7024,11 +7056,11 @@
         <v>3</v>
       </c>
       <c r="C69" s="43" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D69" s="43"/>
       <c r="E69" s="43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F69" s="43" t="s">
         <v>289</v>
@@ -7039,11 +7071,11 @@
         <v>3</v>
       </c>
       <c r="C70" s="43" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D70" s="43"/>
       <c r="E70" s="43" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F70" s="43" t="s">
         <v>289</v>
@@ -7054,11 +7086,11 @@
         <v>3</v>
       </c>
       <c r="C71" s="43" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D71" s="43"/>
       <c r="E71" s="43" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F71" s="43" t="s">
         <v>289</v>
@@ -7069,11 +7101,11 @@
         <v>3</v>
       </c>
       <c r="C72" s="43" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D72" s="43"/>
       <c r="E72" s="43" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F72" s="43" t="s">
         <v>289</v>
@@ -7084,11 +7116,11 @@
         <v>3</v>
       </c>
       <c r="C73" s="43" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D73" s="43"/>
       <c r="E73" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F73" s="43" t="s">
         <v>289</v>
@@ -7099,16 +7131,14 @@
         <v>3</v>
       </c>
       <c r="C74" s="43" t="s">
-        <v>290</v>
-      </c>
-      <c r="D74" s="43" t="s">
-        <v>291</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="D74" s="43"/>
       <c r="E74" s="43" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="F74" s="43" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.25">
@@ -7116,126 +7146,143 @@
         <v>3</v>
       </c>
       <c r="C75" s="43" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D75" s="43" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E75" s="43" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F75" s="43" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="76" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B77" s="7" t="s">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="43" t="s">
+        <v>293</v>
+      </c>
+      <c r="D76" s="43" t="s">
+        <v>294</v>
+      </c>
+      <c r="E76" s="43" t="s">
+        <v>295</v>
+      </c>
+      <c r="F76" s="43" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B78" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
-      <c r="G77" t="s">
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:12" ht="176.25" x14ac:dyDescent="0.25">
-      <c r="B79" s="44" t="s">
+    <row r="80" spans="2:12" ht="176.25" x14ac:dyDescent="0.25">
+      <c r="B80" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="C79" s="45" t="s">
+      <c r="C80" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D79" s="46" t="s">
+      <c r="D80" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="E79" s="46" t="s">
+      <c r="E80" s="46" t="s">
         <v>303</v>
       </c>
-      <c r="F79" s="46" t="s">
+      <c r="F80" s="46" t="s">
         <v>304</v>
       </c>
-      <c r="G79" s="51" t="s">
+      <c r="G80" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="H79" s="51" t="s">
+      <c r="H80" s="51" t="s">
         <v>306</v>
       </c>
-      <c r="I79" s="51" t="s">
+      <c r="I80" s="51" t="s">
         <v>307</v>
       </c>
-      <c r="J79" s="51" t="s">
+      <c r="J80" s="51" t="s">
         <v>308</v>
       </c>
-      <c r="K79" s="51" t="s">
+      <c r="K80" s="51" t="s">
         <v>309</v>
       </c>
-      <c r="L79" s="51" t="s">
+      <c r="L80" s="51" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B80" s="3" t="s">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C80" s="43" t="s">
+      <c r="C81" s="43" t="s">
         <v>311</v>
       </c>
-      <c r="D80" s="43">
+      <c r="D81" s="43">
         <v>2</v>
       </c>
-      <c r="E80" s="43">
+      <c r="E81" s="43">
         <v>1</v>
       </c>
-      <c r="F80" s="43">
+      <c r="F81" s="43">
         <v>1</v>
       </c>
-      <c r="G80" s="43">
+      <c r="G81" s="43">
         <v>0.5</v>
       </c>
-      <c r="H80" s="43">
+      <c r="H81" s="43">
         <v>0.5</v>
       </c>
-      <c r="I80" s="43">
+      <c r="I81" s="43">
         <v>0.5</v>
       </c>
-      <c r="J80" s="43">
+      <c r="J81" s="43">
         <v>14400</v>
       </c>
-      <c r="K80" s="43">
+      <c r="K81" s="43">
         <v>86400</v>
       </c>
-      <c r="L80" s="43">
+      <c r="L81" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J82" t="s">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J83" t="s">
         <v>312</v>
       </c>
-      <c r="K82" t="s">
+      <c r="K83" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="85" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J85">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J86">
         <f>3600*4</f>
         <v>14400</v>
       </c>
-      <c r="K85">
+      <c r="K86">
         <f>3600*24</f>
         <v>86400</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D46:D55 D11:F11 E65:E66 D65:D70 D17:D41"/>
-    <dataValidation type="list" sqref="E46:E55">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D47:D56 D11:F11 E66:E67 D66:D71 D17:D42"/>
+    <dataValidation type="list" sqref="E47:E56">
       <formula1>"sc,pc,gf,egg,pet,skin"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8316,31 +8363,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="L5:L16">

</xml_diff>

<commit_message>
deleted bundle werewolf_invasion_2 Added sesaon werewolf to PF villagers with werewolf mask Seasonal Scenes added component for bunny to activate in easter  toggleby flavour graves: ART_halloween
Former-commit-id: 3a2997565b04f67a2a72541d8cc836e37a0e82b4
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_General.xlsx
+++ b/Docs/Content/HungryDragonContent_General.xlsx
@@ -1094,9 +1094,6 @@
     <t>halloween_China</t>
   </si>
   <si>
-    <t>werewolf</t>
-  </si>
-  <si>
     <t>icon_season_werewolf</t>
   </si>
   <si>
@@ -1119,6 +1116,9 @@
   </si>
   <si>
     <t>TID_SEASON_BUNNIES_NAME</t>
+  </si>
+  <si>
+    <t>werewolf_vampire</t>
   </si>
 </sst>
 </file>
@@ -1601,320 +1601,6 @@
   </cellStyles>
   <dxfs count="94">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2662,6 +2348,96 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2850,80 +2626,73 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3071,266 +2840,12 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3362,23 +2877,19 @@
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3390,23 +2901,43 @@
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3528,6 +3059,475 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5538,125 +5538,125 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="gameSettings9" displayName="gameSettings9" ref="B4:R5" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="gameSettings9" displayName="gameSettings9" ref="B4:R5" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90" totalsRowBorderDxfId="89">
   <autoFilter ref="B4:R5"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="{gameSettings}" dataDxfId="89"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
-    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="87"/>
-    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="86"/>
-    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="85"/>
-    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="84"/>
-    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="83"/>
-    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="82"/>
-    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="81"/>
-    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="80"/>
-    <tableColumn id="17" name="[miniMapTimerAd]" dataDxfId="79"/>
-    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="78"/>
-    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="77"/>
-    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
-    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="75"/>
-    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="74"/>
-    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="73"/>
+    <tableColumn id="1" name="{gameSettings}" dataDxfId="88"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
+    <tableColumn id="3" name="[timeToPCCoefA]" dataDxfId="86"/>
+    <tableColumn id="4" name="[timeToPCCoefB]" dataDxfId="85"/>
+    <tableColumn id="5" name="[incentivizeFBGem]" dataDxfId="84"/>
+    <tableColumn id="6" name="[dailyAdsRemoveMissions]" dataDxfId="83"/>
+    <tableColumn id="15" name="[maxAdsSkipMissions]" dataDxfId="82"/>
+    <tableColumn id="16" name="[cooldownAdsSkipMissions]" dataDxfId="81"/>
+    <tableColumn id="7" name="[miniMapHCCost]" dataDxfId="80"/>
+    <tableColumn id="8" name="[miniMapTimer]" dataDxfId="79"/>
+    <tableColumn id="17" name="[miniMapTimerAd]" dataDxfId="78"/>
+    <tableColumn id="9" name="[missingRessourcesPCperSC]" dataDxfId="77"/>
+    <tableColumn id="10" name="[MaxGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="76"/>
+    <tableColumn id="11" name="[AdditionalGoldRushCompletitionPercentageForConsecutiveRushes]" dataDxfId="75"/>
+    <tableColumn id="12" name="[flyingPigsProbaCoefA]" dataDxfId="74"/>
+    <tableColumn id="13" name="[flyingPigsProbaCoefB]" dataDxfId="73"/>
+    <tableColumn id="14" name="[goldenFragmentsToHCCoef]" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="gameSettings2110" displayName="gameSettings2110" ref="B10:G11" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70" totalsRowBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="gameSettings2110" displayName="gameSettings2110" ref="B10:G11" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <autoFilter ref="B10:G11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{initialSettings}" dataDxfId="68"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="67"/>
-    <tableColumn id="3" name="[softCurrency]" dataDxfId="66"/>
-    <tableColumn id="8" name="[hardCurrency]" dataDxfId="65"/>
-    <tableColumn id="4" name="[goldenFragments]" dataDxfId="64"/>
-    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="63"/>
+    <tableColumn id="1" name="{initialSettings}" dataDxfId="67"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="3" name="[softCurrency]" dataDxfId="65"/>
+    <tableColumn id="8" name="[hardCurrency]" dataDxfId="64"/>
+    <tableColumn id="4" name="[goldenFragments]" dataDxfId="63"/>
+    <tableColumn id="6" name="[initialDragonSKU]" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H42" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="gameSettings211411" displayName="gameSettings211411" ref="B16:H42" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
   <autoFilter ref="B16:H42"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="6"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="3" name="[active]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="2"/>
-    <tableColumn id="6" name="[bloodParticles]" dataDxfId="1"/>
-    <tableColumn id="7" name="[pillParticles]" dataDxfId="0"/>
+    <tableColumn id="1" name="{seasonsDefinitions}" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="56"/>
+    <tableColumn id="3" name="[active]" dataDxfId="55"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="54"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="53"/>
+    <tableColumn id="6" name="[bloodParticles]" dataDxfId="52"/>
+    <tableColumn id="7" name="[pillParticles]" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B46:G56" totalsRowShown="0" headerRowDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="preRegRewardsDefinitions12" displayName="preRegRewardsDefinitions12" ref="B46:G56" totalsRowShown="0" headerRowDxfId="50">
   <autoFilter ref="B46:G56"/>
   <sortState ref="B34:G44">
     <sortCondition descending="1" ref="D24:D35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="61"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="60"/>
-    <tableColumn id="3" name="[threshold]" dataDxfId="59"/>
-    <tableColumn id="4" name="[type]" dataDxfId="58"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="57"/>
-    <tableColumn id="6" name="[rewardSku]" dataDxfId="56"/>
+    <tableColumn id="1" name="{preRegRewardsDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="3" name="[threshold]" dataDxfId="47"/>
+    <tableColumn id="4" name="[type]" dataDxfId="46"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="45"/>
+    <tableColumn id="6" name="[rewardSku]" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="localizationDefinitions" displayName="localizationDefinitions" ref="B4:M16" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B4:M16"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="51"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="3" name="[order]" dataDxfId="49"/>
-    <tableColumn id="4" name="[isoCode]" dataDxfId="48"/>
-    <tableColumn id="7" name="[serverCode]" dataDxfId="47"/>
-    <tableColumn id="11" name="[android]" dataDxfId="46"/>
-    <tableColumn id="12" name="[iOS]" dataDxfId="45"/>
-    <tableColumn id="5" name="[txtFilename]" dataDxfId="44"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="43"/>
-    <tableColumn id="10" name="[logo]" dataDxfId="42"/>
-    <tableColumn id="6" name="[fontGroup]" dataDxfId="41"/>
-    <tableColumn id="9" name="[tidName]" dataDxfId="40"/>
+    <tableColumn id="1" name="{localizationDefinitions}" dataDxfId="30"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" name="[order]" dataDxfId="28"/>
+    <tableColumn id="4" name="[isoCode]" dataDxfId="27"/>
+    <tableColumn id="7" name="[serverCode]" dataDxfId="26"/>
+    <tableColumn id="11" name="[android]" dataDxfId="25"/>
+    <tableColumn id="12" name="[iOS]" dataDxfId="24"/>
+    <tableColumn id="5" name="[txtFilename]" dataDxfId="23"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="22"/>
+    <tableColumn id="10" name="[logo]" dataDxfId="21"/>
+    <tableColumn id="6" name="[fontGroup]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidName]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fontGroupsDefinitions6" displayName="fontGroupsDefinitions6" ref="B21:E27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="B21:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="35"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="34"/>
-    <tableColumn id="11" name="[fonts]" dataDxfId="33"/>
-    <tableColumn id="2" name="[defaultFont]" dataDxfId="32"/>
+    <tableColumn id="1" name="{fontGroupsDefinitions}" dataDxfId="14"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="11" name="[fonts]" dataDxfId="12"/>
+    <tableColumn id="2" name="[defaultFont]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="fontGroupsDefinitions68" displayName="fontGroupsDefinitions68" ref="B34:H50" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B34:H50"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="27"/>
-    <tableColumn id="8" name="[sku]" dataDxfId="26"/>
-    <tableColumn id="11" name="[prefab]" dataDxfId="25"/>
-    <tableColumn id="2" name="[url]" dataDxfId="24"/>
-    <tableColumn id="3" name="[urlChina]" dataDxfId="23"/>
-    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="22"/>
-    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="21"/>
+    <tableColumn id="1" name="{shareLocationDefinitions}" dataDxfId="6"/>
+    <tableColumn id="8" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="11" name="[prefab]" dataDxfId="4"/>
+    <tableColumn id="2" name="[url]" dataDxfId="3"/>
+    <tableColumn id="3" name="[urlChina]" dataDxfId="2"/>
+    <tableColumn id="4" name="[tidPrewrittenCaption]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidCallToAction]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5931,7 +5931,7 @@
   <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6633,16 +6633,16 @@
         <v>3</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="D40" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E40" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="F40" s="39" t="s">
         <v>345</v>
-      </c>
-      <c r="F40" s="39" t="s">
-        <v>346</v>
       </c>
       <c r="G40" s="39"/>
       <c r="H40" s="39" t="s">
@@ -6654,16 +6654,16 @@
         <v>3</v>
       </c>
       <c r="C41" s="55" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D41" s="56" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="57" t="s">
+        <v>347</v>
+      </c>
+      <c r="F41" s="57" t="s">
         <v>348</v>
-      </c>
-      <c r="F41" s="57" t="s">
-        <v>349</v>
       </c>
       <c r="G41" s="57"/>
       <c r="H41" s="57" t="s">
@@ -6675,16 +6675,16 @@
         <v>3</v>
       </c>
       <c r="C42" s="55" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D42" s="60" t="b">
         <v>0</v>
       </c>
       <c r="E42" s="55" t="s">
+        <v>350</v>
+      </c>
+      <c r="F42" s="55" t="s">
         <v>351</v>
-      </c>
-      <c r="F42" s="55" t="s">
-        <v>352</v>
       </c>
       <c r="G42" s="55"/>
       <c r="H42" s="55"/>
@@ -7278,7 +7278,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D47:D56 D11:F11 E66:E67 D66:D71 D17:D42"/>
@@ -8363,31 +8363,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C16">
-    <cfRule type="duplicateValues" dxfId="19" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="duplicateValues" dxfId="18" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C46">
-    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="duplicateValues" dxfId="16" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C40">
-    <cfRule type="duplicateValues" dxfId="15" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="duplicateValues" dxfId="14" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="13" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="L5:L16">

</xml_diff>